<commit_message>
WLCMS-2831 Session ID column in Classroom batch import file
</commit_message>
<xml_diff>
--- a/lcms.web/src/main/webapp/theme/samplefile/Classroom batch import template.xlsx
+++ b/lcms.web/src/main/webapp/theme/samplefile/Classroom batch import template.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="389">
   <si>
     <t>(GMT -12:00) Dateline (Eniwetok)</t>
   </si>
@@ -1990,6 +1990,33 @@
         <scheme val="minor"/>
       </rPr>
       <t>john.doe@360training.com</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Session Key</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Session1</t>
     </r>
   </si>
 </sst>
@@ -2162,7 +2189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2273,6 +2300,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2596,27 +2626,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="1"/>
-    <col min="2" max="3" width="26.42578125" style="32" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="1" max="3" width="26.42578125" style="26" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" style="26" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="26" customWidth="1"/>
     <col min="6" max="6" width="32.28515625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="87" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="42" t="s">
         <v>380</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="42" t="s">
         <v>383</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="42" t="s">
         <v>381</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="42" t="s">
         <v>382</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="42" t="s">
         <v>384</v>
       </c>
       <c r="F1" s="41" t="s">
@@ -3370,7 +3399,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I679"/>
+  <dimension ref="A1:J679"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -3381,15 +3410,16 @@
   <cols>
     <col min="1" max="1" width="28.28515625" style="11" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" style="11" customWidth="1"/>
-    <col min="3" max="3" width="51" style="11" customWidth="1"/>
-    <col min="4" max="4" width="29.42578125" style="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.42578125" style="25" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" style="25" customWidth="1"/>
-    <col min="7" max="7" width="18" style="11" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="11"/>
+    <col min="3" max="3" width="41.140625" style="11" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" style="11" customWidth="1"/>
+    <col min="5" max="5" width="29.42578125" style="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.42578125" style="25" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" style="25" customWidth="1"/>
+    <col min="8" max="8" width="18" style="11" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="39" t="s">
         <v>378</v>
       </c>
@@ -3400,2671 +3430,2676 @@
         <v>307</v>
       </c>
       <c r="D1" s="24" t="s">
+        <v>388</v>
+      </c>
+      <c r="E1" s="24" t="s">
         <v>315</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="F1" s="24" t="s">
         <v>314</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C2" s="2"/>
-      <c r="D2" s="21"/>
+      <c r="D2" s="37"/>
       <c r="E2" s="21"/>
       <c r="F2" s="21"/>
-      <c r="G2" s="2"/>
+      <c r="G2" s="21"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F3" s="21"/>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D4" s="21"/>
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G3" s="21"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E4" s="21"/>
       <c r="F4" s="21"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E5" s="21"/>
+      <c r="G4" s="21"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F5" s="21"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E6" s="21"/>
+      <c r="G5" s="21"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F6" s="21"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E7" s="21"/>
+      <c r="G6" s="21"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F7" s="21"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E8" s="21"/>
+      <c r="G7" s="21"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F8" s="21"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E9" s="21"/>
+      <c r="G8" s="21"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F9" s="21"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E10" s="21"/>
+      <c r="G9" s="21"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F10" s="21"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E11" s="21"/>
+      <c r="G10" s="21"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F11" s="21"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E12" s="21"/>
+      <c r="G11" s="21"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F12" s="21"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E13" s="21"/>
+      <c r="G12" s="21"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F13" s="21"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E14" s="21"/>
+      <c r="G13" s="21"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F14" s="21"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E15" s="21"/>
+      <c r="G14" s="21"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F15" s="21"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E16" s="21"/>
+      <c r="G15" s="21"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F16" s="21"/>
-    </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E17" s="21"/>
+      <c r="G16" s="21"/>
+    </row>
+    <row r="17" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F17" s="21"/>
-    </row>
-    <row r="18" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E18" s="21"/>
+      <c r="G17" s="21"/>
+    </row>
+    <row r="18" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F18" s="21"/>
-    </row>
-    <row r="19" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E19" s="21"/>
+      <c r="G18" s="21"/>
+    </row>
+    <row r="19" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F19" s="21"/>
-    </row>
-    <row r="20" spans="5:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E20" s="21"/>
+      <c r="G19" s="21"/>
+    </row>
+    <row r="20" spans="6:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F20" s="21"/>
-    </row>
-    <row r="21" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E21" s="21"/>
+      <c r="G20" s="21"/>
+    </row>
+    <row r="21" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F21" s="21"/>
-    </row>
-    <row r="22" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E22" s="21"/>
+      <c r="G21" s="21"/>
+    </row>
+    <row r="22" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F22" s="21"/>
-    </row>
-    <row r="23" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E23" s="21"/>
+      <c r="G22" s="21"/>
+    </row>
+    <row r="23" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F23" s="21"/>
-    </row>
-    <row r="24" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E24" s="21"/>
+      <c r="G23" s="21"/>
+    </row>
+    <row r="24" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F24" s="21"/>
-    </row>
-    <row r="25" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E25" s="21"/>
+      <c r="G24" s="21"/>
+    </row>
+    <row r="25" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F25" s="21"/>
-    </row>
-    <row r="26" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E26" s="21"/>
+      <c r="G25" s="21"/>
+    </row>
+    <row r="26" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F26" s="21"/>
-    </row>
-    <row r="27" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E27" s="21"/>
+      <c r="G26" s="21"/>
+    </row>
+    <row r="27" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F27" s="21"/>
-    </row>
-    <row r="28" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E28" s="21"/>
+      <c r="G27" s="21"/>
+    </row>
+    <row r="28" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F28" s="21"/>
-    </row>
-    <row r="29" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E29" s="21"/>
+      <c r="G28" s="21"/>
+    </row>
+    <row r="29" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F29" s="21"/>
-    </row>
-    <row r="30" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E30" s="21"/>
+      <c r="G29" s="21"/>
+    </row>
+    <row r="30" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F30" s="21"/>
-    </row>
-    <row r="31" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E31" s="21"/>
+      <c r="G30" s="21"/>
+    </row>
+    <row r="31" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F31" s="21"/>
-    </row>
-    <row r="32" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E32" s="21"/>
+      <c r="G31" s="21"/>
+    </row>
+    <row r="32" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F32" s="21"/>
-    </row>
-    <row r="33" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E33" s="21"/>
+      <c r="G32" s="21"/>
+    </row>
+    <row r="33" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F33" s="21"/>
-    </row>
-    <row r="34" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E34" s="21"/>
+      <c r="G33" s="21"/>
+    </row>
+    <row r="34" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F34" s="21"/>
-    </row>
-    <row r="35" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E35" s="21"/>
+      <c r="G34" s="21"/>
+    </row>
+    <row r="35" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F35" s="21"/>
-    </row>
-    <row r="36" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E36" s="21"/>
+      <c r="G35" s="21"/>
+    </row>
+    <row r="36" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F36" s="21"/>
-    </row>
-    <row r="37" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E37" s="21"/>
+      <c r="G36" s="21"/>
+    </row>
+    <row r="37" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F37" s="21"/>
-    </row>
-    <row r="38" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E38" s="21"/>
+      <c r="G37" s="21"/>
+    </row>
+    <row r="38" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F38" s="21"/>
-    </row>
-    <row r="39" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E39" s="21"/>
+      <c r="G38" s="21"/>
+    </row>
+    <row r="39" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F39" s="21"/>
-    </row>
-    <row r="40" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E40" s="21"/>
+      <c r="G39" s="21"/>
+    </row>
+    <row r="40" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F40" s="21"/>
-    </row>
-    <row r="41" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E41" s="21"/>
+      <c r="G40" s="21"/>
+    </row>
+    <row r="41" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F41" s="21"/>
-    </row>
-    <row r="42" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E42" s="21"/>
+      <c r="G41" s="21"/>
+    </row>
+    <row r="42" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F42" s="21"/>
-    </row>
-    <row r="43" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E43" s="21"/>
+      <c r="G42" s="21"/>
+    </row>
+    <row r="43" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F43" s="21"/>
-    </row>
-    <row r="44" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E44" s="21"/>
+      <c r="G43" s="21"/>
+    </row>
+    <row r="44" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F44" s="21"/>
-    </row>
-    <row r="45" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E45" s="21"/>
+      <c r="G44" s="21"/>
+    </row>
+    <row r="45" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F45" s="21"/>
-    </row>
-    <row r="46" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E46" s="21"/>
+      <c r="G45" s="21"/>
+    </row>
+    <row r="46" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F46" s="21"/>
-    </row>
-    <row r="47" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E47" s="21"/>
+      <c r="G46" s="21"/>
+    </row>
+    <row r="47" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F47" s="21"/>
-    </row>
-    <row r="48" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E48" s="21"/>
+      <c r="G47" s="21"/>
+    </row>
+    <row r="48" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F48" s="21"/>
-    </row>
-    <row r="49" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E49" s="21"/>
+      <c r="G48" s="21"/>
+    </row>
+    <row r="49" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F49" s="21"/>
-    </row>
-    <row r="50" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E50" s="21"/>
+      <c r="G49" s="21"/>
+    </row>
+    <row r="50" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F50" s="21"/>
-    </row>
-    <row r="51" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E51" s="21"/>
+      <c r="G50" s="21"/>
+    </row>
+    <row r="51" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F51" s="21"/>
-    </row>
-    <row r="52" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E52" s="21"/>
+      <c r="G51" s="21"/>
+    </row>
+    <row r="52" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F52" s="21"/>
-    </row>
-    <row r="53" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E53" s="21"/>
+      <c r="G52" s="21"/>
+    </row>
+    <row r="53" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F53" s="21"/>
-    </row>
-    <row r="54" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E54" s="21"/>
+      <c r="G53" s="21"/>
+    </row>
+    <row r="54" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F54" s="21"/>
-    </row>
-    <row r="55" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E55" s="21"/>
+      <c r="G54" s="21"/>
+    </row>
+    <row r="55" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F55" s="21"/>
-    </row>
-    <row r="56" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E56" s="21"/>
+      <c r="G55" s="21"/>
+    </row>
+    <row r="56" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F56" s="21"/>
-    </row>
-    <row r="57" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E57" s="21"/>
+      <c r="G56" s="21"/>
+    </row>
+    <row r="57" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F57" s="21"/>
-    </row>
-    <row r="58" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E58" s="21"/>
+      <c r="G57" s="21"/>
+    </row>
+    <row r="58" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F58" s="21"/>
-    </row>
-    <row r="59" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E59" s="21"/>
+      <c r="G58" s="21"/>
+    </row>
+    <row r="59" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F59" s="21"/>
-    </row>
-    <row r="60" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E60" s="21"/>
+      <c r="G59" s="21"/>
+    </row>
+    <row r="60" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F60" s="21"/>
-    </row>
-    <row r="61" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E61" s="21"/>
+      <c r="G60" s="21"/>
+    </row>
+    <row r="61" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F61" s="21"/>
-    </row>
-    <row r="62" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E62" s="21"/>
+      <c r="G61" s="21"/>
+    </row>
+    <row r="62" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F62" s="21"/>
-    </row>
-    <row r="63" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E63" s="21"/>
+      <c r="G62" s="21"/>
+    </row>
+    <row r="63" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F63" s="21"/>
-    </row>
-    <row r="64" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E64" s="21"/>
+      <c r="G63" s="21"/>
+    </row>
+    <row r="64" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F64" s="21"/>
-    </row>
-    <row r="71" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E71" s="21"/>
+      <c r="G64" s="21"/>
+    </row>
+    <row r="71" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F71" s="21"/>
-    </row>
-    <row r="72" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E72" s="21"/>
+      <c r="G71" s="21"/>
+    </row>
+    <row r="72" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F72" s="21"/>
-    </row>
-    <row r="73" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E73" s="21"/>
+      <c r="G72" s="21"/>
+    </row>
+    <row r="73" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F73" s="21"/>
-    </row>
-    <row r="74" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E74" s="21"/>
+      <c r="G73" s="21"/>
+    </row>
+    <row r="74" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F74" s="21"/>
-    </row>
-    <row r="75" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E75" s="21"/>
+      <c r="G74" s="21"/>
+    </row>
+    <row r="75" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F75" s="21"/>
-    </row>
-    <row r="76" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E76" s="21"/>
+      <c r="G75" s="21"/>
+    </row>
+    <row r="76" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F76" s="21"/>
-    </row>
-    <row r="77" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E77" s="21"/>
+      <c r="G76" s="21"/>
+    </row>
+    <row r="77" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F77" s="21"/>
-    </row>
-    <row r="78" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E78" s="21"/>
+      <c r="G77" s="21"/>
+    </row>
+    <row r="78" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F78" s="21"/>
-    </row>
-    <row r="79" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E79" s="21"/>
+      <c r="G78" s="21"/>
+    </row>
+    <row r="79" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F79" s="21"/>
-    </row>
-    <row r="80" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E80" s="21"/>
+      <c r="G79" s="21"/>
+    </row>
+    <row r="80" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F80" s="21"/>
-    </row>
-    <row r="81" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E81" s="21"/>
+      <c r="G80" s="21"/>
+    </row>
+    <row r="81" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F81" s="21"/>
-    </row>
-    <row r="82" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E82" s="21"/>
+      <c r="G81" s="21"/>
+    </row>
+    <row r="82" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F82" s="21"/>
-    </row>
-    <row r="83" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E83" s="21"/>
+      <c r="G82" s="21"/>
+    </row>
+    <row r="83" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F83" s="21"/>
-    </row>
-    <row r="84" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E84" s="21"/>
+      <c r="G83" s="21"/>
+    </row>
+    <row r="84" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F84" s="21"/>
-    </row>
-    <row r="85" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E85" s="21"/>
+      <c r="G84" s="21"/>
+    </row>
+    <row r="85" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F85" s="21"/>
-    </row>
-    <row r="86" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E86" s="21"/>
+      <c r="G85" s="21"/>
+    </row>
+    <row r="86" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F86" s="21"/>
-    </row>
-    <row r="87" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E87" s="21"/>
+      <c r="G86" s="21"/>
+    </row>
+    <row r="87" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F87" s="21"/>
-    </row>
-    <row r="88" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E88" s="21"/>
+      <c r="G87" s="21"/>
+    </row>
+    <row r="88" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F88" s="21"/>
-    </row>
-    <row r="89" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E89" s="21"/>
+      <c r="G88" s="21"/>
+    </row>
+    <row r="89" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F89" s="21"/>
-    </row>
-    <row r="90" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E90" s="21"/>
+      <c r="G89" s="21"/>
+    </row>
+    <row r="90" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F90" s="21"/>
-    </row>
-    <row r="91" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E91" s="21"/>
+      <c r="G90" s="21"/>
+    </row>
+    <row r="91" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F91" s="21"/>
-    </row>
-    <row r="92" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E92" s="21"/>
+      <c r="G91" s="21"/>
+    </row>
+    <row r="92" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F92" s="21"/>
-    </row>
-    <row r="93" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E93" s="21"/>
+      <c r="G92" s="21"/>
+    </row>
+    <row r="93" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F93" s="21"/>
-    </row>
-    <row r="94" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E94" s="21"/>
+      <c r="G93" s="21"/>
+    </row>
+    <row r="94" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F94" s="21"/>
-    </row>
-    <row r="95" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E95" s="21"/>
+      <c r="G94" s="21"/>
+    </row>
+    <row r="95" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F95" s="21"/>
-    </row>
-    <row r="96" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E96" s="21"/>
+      <c r="G95" s="21"/>
+    </row>
+    <row r="96" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F96" s="21"/>
-    </row>
-    <row r="97" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E97" s="21"/>
+      <c r="G96" s="21"/>
+    </row>
+    <row r="97" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F97" s="21"/>
-    </row>
-    <row r="98" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E98" s="21"/>
+      <c r="G97" s="21"/>
+    </row>
+    <row r="98" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F98" s="21"/>
-    </row>
-    <row r="99" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E99" s="21"/>
+      <c r="G98" s="21"/>
+    </row>
+    <row r="99" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F99" s="21"/>
-    </row>
-    <row r="100" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E100" s="21"/>
+      <c r="G99" s="21"/>
+    </row>
+    <row r="100" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F100" s="21"/>
-    </row>
-    <row r="101" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E101" s="21"/>
+      <c r="G100" s="21"/>
+    </row>
+    <row r="101" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F101" s="21"/>
-    </row>
-    <row r="102" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E102" s="21"/>
+      <c r="G101" s="21"/>
+    </row>
+    <row r="102" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F102" s="21"/>
-    </row>
-    <row r="103" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E103" s="21"/>
+      <c r="G102" s="21"/>
+    </row>
+    <row r="103" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F103" s="21"/>
-    </row>
-    <row r="104" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E104" s="21"/>
+      <c r="G103" s="21"/>
+    </row>
+    <row r="104" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F104" s="21"/>
-    </row>
-    <row r="105" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E105" s="21"/>
+      <c r="G104" s="21"/>
+    </row>
+    <row r="105" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F105" s="21"/>
-    </row>
-    <row r="106" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E106" s="21"/>
+      <c r="G105" s="21"/>
+    </row>
+    <row r="106" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F106" s="21"/>
-    </row>
-    <row r="107" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E107" s="21"/>
+      <c r="G106" s="21"/>
+    </row>
+    <row r="107" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F107" s="21"/>
-    </row>
-    <row r="108" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E108" s="21"/>
+      <c r="G107" s="21"/>
+    </row>
+    <row r="108" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F108" s="21"/>
-    </row>
-    <row r="109" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E109" s="21"/>
+      <c r="G108" s="21"/>
+    </row>
+    <row r="109" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F109" s="21"/>
-    </row>
-    <row r="110" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E110" s="21"/>
+      <c r="G109" s="21"/>
+    </row>
+    <row r="110" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F110" s="21"/>
-    </row>
-    <row r="111" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E111" s="21"/>
+      <c r="G110" s="21"/>
+    </row>
+    <row r="111" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F111" s="21"/>
-    </row>
-    <row r="112" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E112" s="21"/>
+      <c r="G111" s="21"/>
+    </row>
+    <row r="112" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F112" s="21"/>
-    </row>
-    <row r="113" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E113" s="21"/>
+      <c r="G112" s="21"/>
+    </row>
+    <row r="113" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F113" s="21"/>
-    </row>
-    <row r="114" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E114" s="21"/>
+      <c r="G113" s="21"/>
+    </row>
+    <row r="114" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F114" s="21"/>
-    </row>
-    <row r="115" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E115" s="21"/>
+      <c r="G114" s="21"/>
+    </row>
+    <row r="115" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F115" s="21"/>
-    </row>
-    <row r="116" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E116" s="21"/>
+      <c r="G115" s="21"/>
+    </row>
+    <row r="116" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F116" s="21"/>
-    </row>
-    <row r="117" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E117" s="21"/>
+      <c r="G116" s="21"/>
+    </row>
+    <row r="117" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F117" s="21"/>
-    </row>
-    <row r="118" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E118" s="21"/>
+      <c r="G117" s="21"/>
+    </row>
+    <row r="118" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F118" s="21"/>
-    </row>
-    <row r="119" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E119" s="21"/>
+      <c r="G118" s="21"/>
+    </row>
+    <row r="119" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F119" s="21"/>
-    </row>
-    <row r="120" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E120" s="21"/>
+      <c r="G119" s="21"/>
+    </row>
+    <row r="120" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F120" s="21"/>
-    </row>
-    <row r="121" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E121" s="21"/>
+      <c r="G120" s="21"/>
+    </row>
+    <row r="121" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F121" s="21"/>
-    </row>
-    <row r="122" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E122" s="21"/>
+      <c r="G121" s="21"/>
+    </row>
+    <row r="122" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F122" s="21"/>
-    </row>
-    <row r="123" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E123" s="21"/>
+      <c r="G122" s="21"/>
+    </row>
+    <row r="123" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F123" s="21"/>
-    </row>
-    <row r="124" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E124" s="21"/>
+      <c r="G123" s="21"/>
+    </row>
+    <row r="124" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F124" s="21"/>
-    </row>
-    <row r="125" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E125" s="21"/>
+      <c r="G124" s="21"/>
+    </row>
+    <row r="125" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F125" s="21"/>
-    </row>
-    <row r="126" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E126" s="21"/>
+      <c r="G125" s="21"/>
+    </row>
+    <row r="126" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F126" s="21"/>
-    </row>
-    <row r="127" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E127" s="21"/>
+      <c r="G126" s="21"/>
+    </row>
+    <row r="127" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F127" s="21"/>
-    </row>
-    <row r="128" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E128" s="21"/>
+      <c r="G127" s="21"/>
+    </row>
+    <row r="128" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F128" s="21"/>
-    </row>
-    <row r="129" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E129" s="21"/>
+      <c r="G128" s="21"/>
+    </row>
+    <row r="129" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F129" s="21"/>
-    </row>
-    <row r="130" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E130" s="21"/>
+      <c r="G129" s="21"/>
+    </row>
+    <row r="130" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F130" s="21"/>
-    </row>
-    <row r="131" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E131" s="21"/>
+      <c r="G130" s="21"/>
+    </row>
+    <row r="131" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F131" s="21"/>
-    </row>
-    <row r="132" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E132" s="21"/>
+      <c r="G131" s="21"/>
+    </row>
+    <row r="132" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F132" s="21"/>
-    </row>
-    <row r="133" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E133" s="21"/>
+      <c r="G132" s="21"/>
+    </row>
+    <row r="133" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F133" s="21"/>
-    </row>
-    <row r="134" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E134" s="21"/>
+      <c r="G133" s="21"/>
+    </row>
+    <row r="134" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F134" s="21"/>
-    </row>
-    <row r="135" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E135" s="21"/>
+      <c r="G134" s="21"/>
+    </row>
+    <row r="135" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F135" s="21"/>
-    </row>
-    <row r="136" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E136" s="21"/>
+      <c r="G135" s="21"/>
+    </row>
+    <row r="136" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F136" s="21"/>
-    </row>
-    <row r="137" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E137" s="21"/>
+      <c r="G136" s="21"/>
+    </row>
+    <row r="137" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F137" s="21"/>
-    </row>
-    <row r="138" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E138" s="21"/>
+      <c r="G137" s="21"/>
+    </row>
+    <row r="138" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F138" s="21"/>
-    </row>
-    <row r="139" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E139" s="21"/>
+      <c r="G138" s="21"/>
+    </row>
+    <row r="139" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F139" s="21"/>
-    </row>
-    <row r="140" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E140" s="21"/>
+      <c r="G139" s="21"/>
+    </row>
+    <row r="140" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F140" s="21"/>
-    </row>
-    <row r="141" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E141" s="21"/>
+      <c r="G140" s="21"/>
+    </row>
+    <row r="141" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F141" s="21"/>
-    </row>
-    <row r="142" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E142" s="21"/>
+      <c r="G141" s="21"/>
+    </row>
+    <row r="142" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F142" s="21"/>
-    </row>
-    <row r="143" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E143" s="21"/>
+      <c r="G142" s="21"/>
+    </row>
+    <row r="143" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F143" s="21"/>
-    </row>
-    <row r="144" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E144" s="21"/>
+      <c r="G143" s="21"/>
+    </row>
+    <row r="144" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F144" s="21"/>
-    </row>
-    <row r="145" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E145" s="21"/>
+      <c r="G144" s="21"/>
+    </row>
+    <row r="145" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F145" s="21"/>
-    </row>
-    <row r="146" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E146" s="21"/>
+      <c r="G145" s="21"/>
+    </row>
+    <row r="146" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F146" s="21"/>
-    </row>
-    <row r="147" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E147" s="21"/>
+      <c r="G146" s="21"/>
+    </row>
+    <row r="147" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F147" s="21"/>
-    </row>
-    <row r="148" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E148" s="21"/>
+      <c r="G147" s="21"/>
+    </row>
+    <row r="148" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F148" s="21"/>
-    </row>
-    <row r="149" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E149" s="21"/>
+      <c r="G148" s="21"/>
+    </row>
+    <row r="149" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F149" s="21"/>
-    </row>
-    <row r="150" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E150" s="21"/>
+      <c r="G149" s="21"/>
+    </row>
+    <row r="150" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F150" s="21"/>
-    </row>
-    <row r="151" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E151" s="21"/>
+      <c r="G150" s="21"/>
+    </row>
+    <row r="151" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F151" s="21"/>
-    </row>
-    <row r="152" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E152" s="21"/>
+      <c r="G151" s="21"/>
+    </row>
+    <row r="152" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F152" s="21"/>
-    </row>
-    <row r="153" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E153" s="21"/>
+      <c r="G152" s="21"/>
+    </row>
+    <row r="153" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F153" s="21"/>
-    </row>
-    <row r="154" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E154" s="21"/>
+      <c r="G153" s="21"/>
+    </row>
+    <row r="154" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F154" s="21"/>
-    </row>
-    <row r="155" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E155" s="21"/>
+      <c r="G154" s="21"/>
+    </row>
+    <row r="155" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F155" s="21"/>
-    </row>
-    <row r="156" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E156" s="21"/>
+      <c r="G155" s="21"/>
+    </row>
+    <row r="156" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F156" s="21"/>
-    </row>
-    <row r="157" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E157" s="21"/>
+      <c r="G156" s="21"/>
+    </row>
+    <row r="157" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F157" s="21"/>
-    </row>
-    <row r="158" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E158" s="21"/>
+      <c r="G157" s="21"/>
+    </row>
+    <row r="158" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F158" s="21"/>
-    </row>
-    <row r="159" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E159" s="21"/>
+      <c r="G158" s="21"/>
+    </row>
+    <row r="159" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F159" s="21"/>
-    </row>
-    <row r="160" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E160" s="21"/>
+      <c r="G159" s="21"/>
+    </row>
+    <row r="160" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F160" s="21"/>
-    </row>
-    <row r="161" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E161" s="21"/>
+      <c r="G160" s="21"/>
+    </row>
+    <row r="161" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F161" s="21"/>
-    </row>
-    <row r="162" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E162" s="21"/>
+      <c r="G161" s="21"/>
+    </row>
+    <row r="162" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F162" s="21"/>
-    </row>
-    <row r="163" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E163" s="21"/>
+      <c r="G162" s="21"/>
+    </row>
+    <row r="163" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F163" s="21"/>
-    </row>
-    <row r="164" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E164" s="21"/>
+      <c r="G163" s="21"/>
+    </row>
+    <row r="164" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F164" s="21"/>
-    </row>
-    <row r="165" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E165" s="21"/>
+      <c r="G164" s="21"/>
+    </row>
+    <row r="165" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F165" s="21"/>
-    </row>
-    <row r="166" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E166" s="21"/>
+      <c r="G165" s="21"/>
+    </row>
+    <row r="166" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F166" s="21"/>
-    </row>
-    <row r="167" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E167" s="21"/>
+      <c r="G166" s="21"/>
+    </row>
+    <row r="167" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F167" s="21"/>
-    </row>
-    <row r="168" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E168" s="21"/>
+      <c r="G167" s="21"/>
+    </row>
+    <row r="168" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F168" s="21"/>
-    </row>
-    <row r="169" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E169" s="21"/>
+      <c r="G168" s="21"/>
+    </row>
+    <row r="169" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F169" s="21"/>
-    </row>
-    <row r="170" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E170" s="21"/>
+      <c r="G169" s="21"/>
+    </row>
+    <row r="170" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F170" s="21"/>
-    </row>
-    <row r="171" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E171" s="21"/>
+      <c r="G170" s="21"/>
+    </row>
+    <row r="171" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F171" s="21"/>
-    </row>
-    <row r="172" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E172" s="21"/>
+      <c r="G171" s="21"/>
+    </row>
+    <row r="172" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F172" s="21"/>
-    </row>
-    <row r="173" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E173" s="21"/>
+      <c r="G172" s="21"/>
+    </row>
+    <row r="173" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F173" s="21"/>
-    </row>
-    <row r="174" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E174" s="21"/>
+      <c r="G173" s="21"/>
+    </row>
+    <row r="174" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F174" s="21"/>
-    </row>
-    <row r="175" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E175" s="21"/>
+      <c r="G174" s="21"/>
+    </row>
+    <row r="175" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F175" s="21"/>
-    </row>
-    <row r="176" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E176" s="21"/>
+      <c r="G175" s="21"/>
+    </row>
+    <row r="176" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F176" s="21"/>
-    </row>
-    <row r="177" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E177" s="21"/>
+      <c r="G176" s="21"/>
+    </row>
+    <row r="177" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F177" s="21"/>
-    </row>
-    <row r="178" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E178" s="21"/>
+      <c r="G177" s="21"/>
+    </row>
+    <row r="178" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F178" s="21"/>
-    </row>
-    <row r="179" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E179" s="21"/>
+      <c r="G178" s="21"/>
+    </row>
+    <row r="179" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F179" s="21"/>
-    </row>
-    <row r="180" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E180" s="21"/>
+      <c r="G179" s="21"/>
+    </row>
+    <row r="180" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F180" s="21"/>
-    </row>
-    <row r="181" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E181" s="21"/>
+      <c r="G180" s="21"/>
+    </row>
+    <row r="181" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F181" s="21"/>
-    </row>
-    <row r="182" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E182" s="21"/>
+      <c r="G181" s="21"/>
+    </row>
+    <row r="182" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F182" s="21"/>
-    </row>
-    <row r="183" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E183" s="21"/>
+      <c r="G182" s="21"/>
+    </row>
+    <row r="183" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F183" s="21"/>
-    </row>
-    <row r="184" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E184" s="21"/>
+      <c r="G183" s="21"/>
+    </row>
+    <row r="184" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F184" s="21"/>
-    </row>
-    <row r="185" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E185" s="21"/>
+      <c r="G184" s="21"/>
+    </row>
+    <row r="185" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F185" s="21"/>
-    </row>
-    <row r="186" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E186" s="21"/>
+      <c r="G185" s="21"/>
+    </row>
+    <row r="186" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F186" s="21"/>
-    </row>
-    <row r="187" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E187" s="21"/>
+      <c r="G186" s="21"/>
+    </row>
+    <row r="187" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F187" s="21"/>
-    </row>
-    <row r="188" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E188" s="21"/>
+      <c r="G187" s="21"/>
+    </row>
+    <row r="188" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F188" s="21"/>
-    </row>
-    <row r="189" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E189" s="21"/>
+      <c r="G188" s="21"/>
+    </row>
+    <row r="189" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F189" s="21"/>
-    </row>
-    <row r="190" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E190" s="21"/>
+      <c r="G189" s="21"/>
+    </row>
+    <row r="190" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F190" s="21"/>
-    </row>
-    <row r="191" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E191" s="21"/>
+      <c r="G190" s="21"/>
+    </row>
+    <row r="191" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F191" s="21"/>
-    </row>
-    <row r="192" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E192" s="21"/>
+      <c r="G191" s="21"/>
+    </row>
+    <row r="192" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F192" s="21"/>
-    </row>
-    <row r="193" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E193" s="21"/>
+      <c r="G192" s="21"/>
+    </row>
+    <row r="193" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F193" s="21"/>
-    </row>
-    <row r="194" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E194" s="21"/>
+      <c r="G193" s="21"/>
+    </row>
+    <row r="194" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F194" s="21"/>
-    </row>
-    <row r="195" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E195" s="21"/>
+      <c r="G194" s="21"/>
+    </row>
+    <row r="195" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F195" s="21"/>
-    </row>
-    <row r="196" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E196" s="21"/>
+      <c r="G195" s="21"/>
+    </row>
+    <row r="196" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F196" s="21"/>
-    </row>
-    <row r="197" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E197" s="21"/>
+      <c r="G196" s="21"/>
+    </row>
+    <row r="197" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F197" s="21"/>
-    </row>
-    <row r="198" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E198" s="21"/>
+      <c r="G197" s="21"/>
+    </row>
+    <row r="198" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F198" s="21"/>
-    </row>
-    <row r="199" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E199" s="21"/>
+      <c r="G198" s="21"/>
+    </row>
+    <row r="199" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F199" s="21"/>
-    </row>
-    <row r="200" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E200" s="21"/>
+      <c r="G199" s="21"/>
+    </row>
+    <row r="200" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F200" s="21"/>
-    </row>
-    <row r="201" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E201" s="21"/>
+      <c r="G200" s="21"/>
+    </row>
+    <row r="201" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F201" s="21"/>
-    </row>
-    <row r="202" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E202" s="21"/>
+      <c r="G201" s="21"/>
+    </row>
+    <row r="202" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F202" s="21"/>
-    </row>
-    <row r="203" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E203" s="21"/>
+      <c r="G202" s="21"/>
+    </row>
+    <row r="203" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F203" s="21"/>
-    </row>
-    <row r="204" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E204" s="21"/>
+      <c r="G203" s="21"/>
+    </row>
+    <row r="204" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F204" s="21"/>
-    </row>
-    <row r="205" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E205" s="21"/>
+      <c r="G204" s="21"/>
+    </row>
+    <row r="205" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F205" s="21"/>
-    </row>
-    <row r="206" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E206" s="21"/>
+      <c r="G205" s="21"/>
+    </row>
+    <row r="206" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F206" s="21"/>
-    </row>
-    <row r="207" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E207" s="21"/>
+      <c r="G206" s="21"/>
+    </row>
+    <row r="207" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F207" s="21"/>
-    </row>
-    <row r="208" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E208" s="21"/>
+      <c r="G207" s="21"/>
+    </row>
+    <row r="208" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F208" s="21"/>
-    </row>
-    <row r="209" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E209" s="21"/>
+      <c r="G208" s="21"/>
+    </row>
+    <row r="209" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F209" s="21"/>
-    </row>
-    <row r="210" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E210" s="21"/>
+      <c r="G209" s="21"/>
+    </row>
+    <row r="210" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F210" s="21"/>
-    </row>
-    <row r="211" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E211" s="21"/>
+      <c r="G210" s="21"/>
+    </row>
+    <row r="211" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F211" s="21"/>
-    </row>
-    <row r="212" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E212" s="21"/>
+      <c r="G211" s="21"/>
+    </row>
+    <row r="212" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F212" s="21"/>
-    </row>
-    <row r="213" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E213" s="21"/>
+      <c r="G212" s="21"/>
+    </row>
+    <row r="213" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F213" s="21"/>
-    </row>
-    <row r="214" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E214" s="21"/>
+      <c r="G213" s="21"/>
+    </row>
+    <row r="214" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F214" s="21"/>
-    </row>
-    <row r="215" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E215" s="21"/>
+      <c r="G214" s="21"/>
+    </row>
+    <row r="215" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F215" s="21"/>
-    </row>
-    <row r="216" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E216" s="21"/>
+      <c r="G215" s="21"/>
+    </row>
+    <row r="216" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F216" s="21"/>
-    </row>
-    <row r="217" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E217" s="21"/>
+      <c r="G216" s="21"/>
+    </row>
+    <row r="217" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F217" s="21"/>
-    </row>
-    <row r="218" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E218" s="21"/>
+      <c r="G217" s="21"/>
+    </row>
+    <row r="218" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F218" s="21"/>
-    </row>
-    <row r="219" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E219" s="21"/>
+      <c r="G218" s="21"/>
+    </row>
+    <row r="219" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F219" s="21"/>
-    </row>
-    <row r="220" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E220" s="21"/>
+      <c r="G219" s="21"/>
+    </row>
+    <row r="220" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F220" s="21"/>
-    </row>
-    <row r="221" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E221" s="21"/>
+      <c r="G220" s="21"/>
+    </row>
+    <row r="221" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F221" s="21"/>
-    </row>
-    <row r="222" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E222" s="21"/>
+      <c r="G221" s="21"/>
+    </row>
+    <row r="222" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F222" s="21"/>
-    </row>
-    <row r="223" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E223" s="21"/>
+      <c r="G222" s="21"/>
+    </row>
+    <row r="223" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F223" s="21"/>
-    </row>
-    <row r="224" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E224" s="21"/>
+      <c r="G223" s="21"/>
+    </row>
+    <row r="224" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F224" s="21"/>
-    </row>
-    <row r="225" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E225" s="21"/>
+      <c r="G224" s="21"/>
+    </row>
+    <row r="225" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F225" s="21"/>
-    </row>
-    <row r="226" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E226" s="21"/>
+      <c r="G225" s="21"/>
+    </row>
+    <row r="226" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F226" s="21"/>
-    </row>
-    <row r="227" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E227" s="21"/>
+      <c r="G226" s="21"/>
+    </row>
+    <row r="227" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F227" s="21"/>
-    </row>
-    <row r="228" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E228" s="21"/>
+      <c r="G227" s="21"/>
+    </row>
+    <row r="228" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F228" s="21"/>
-    </row>
-    <row r="229" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E229" s="21"/>
+      <c r="G228" s="21"/>
+    </row>
+    <row r="229" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F229" s="21"/>
-    </row>
-    <row r="230" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E230" s="21"/>
+      <c r="G229" s="21"/>
+    </row>
+    <row r="230" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F230" s="21"/>
-    </row>
-    <row r="231" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E231" s="21"/>
+      <c r="G230" s="21"/>
+    </row>
+    <row r="231" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F231" s="21"/>
-    </row>
-    <row r="232" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E232" s="21"/>
+      <c r="G231" s="21"/>
+    </row>
+    <row r="232" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F232" s="21"/>
-    </row>
-    <row r="233" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E233" s="21"/>
+      <c r="G232" s="21"/>
+    </row>
+    <row r="233" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F233" s="21"/>
-    </row>
-    <row r="234" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E234" s="21"/>
+      <c r="G233" s="21"/>
+    </row>
+    <row r="234" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F234" s="21"/>
-    </row>
-    <row r="235" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E235" s="21"/>
+      <c r="G234" s="21"/>
+    </row>
+    <row r="235" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F235" s="21"/>
-    </row>
-    <row r="236" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E236" s="21"/>
+      <c r="G235" s="21"/>
+    </row>
+    <row r="236" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F236" s="21"/>
-    </row>
-    <row r="237" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E237" s="21"/>
+      <c r="G236" s="21"/>
+    </row>
+    <row r="237" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F237" s="21"/>
-    </row>
-    <row r="238" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E238" s="21"/>
+      <c r="G237" s="21"/>
+    </row>
+    <row r="238" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F238" s="21"/>
-    </row>
-    <row r="239" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E239" s="21"/>
+      <c r="G238" s="21"/>
+    </row>
+    <row r="239" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F239" s="21"/>
-    </row>
-    <row r="240" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E240" s="21"/>
+      <c r="G239" s="21"/>
+    </row>
+    <row r="240" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F240" s="21"/>
-    </row>
-    <row r="241" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E241" s="21"/>
+      <c r="G240" s="21"/>
+    </row>
+    <row r="241" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F241" s="21"/>
-    </row>
-    <row r="242" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E242" s="21"/>
+      <c r="G241" s="21"/>
+    </row>
+    <row r="242" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F242" s="21"/>
-    </row>
-    <row r="243" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E243" s="21"/>
+      <c r="G242" s="21"/>
+    </row>
+    <row r="243" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F243" s="21"/>
-    </row>
-    <row r="244" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E244" s="21"/>
+      <c r="G243" s="21"/>
+    </row>
+    <row r="244" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F244" s="21"/>
-    </row>
-    <row r="245" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E245" s="21"/>
+      <c r="G244" s="21"/>
+    </row>
+    <row r="245" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F245" s="21"/>
-    </row>
-    <row r="246" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E246" s="21"/>
+      <c r="G245" s="21"/>
+    </row>
+    <row r="246" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F246" s="21"/>
-    </row>
-    <row r="247" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E247" s="21"/>
+      <c r="G246" s="21"/>
+    </row>
+    <row r="247" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F247" s="21"/>
-    </row>
-    <row r="248" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E248" s="21"/>
+      <c r="G247" s="21"/>
+    </row>
+    <row r="248" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F248" s="21"/>
-    </row>
-    <row r="249" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E249" s="21"/>
+      <c r="G248" s="21"/>
+    </row>
+    <row r="249" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F249" s="21"/>
-    </row>
-    <row r="250" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E250" s="21"/>
+      <c r="G249" s="21"/>
+    </row>
+    <row r="250" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F250" s="21"/>
-    </row>
-    <row r="251" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E251" s="21"/>
+      <c r="G250" s="21"/>
+    </row>
+    <row r="251" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F251" s="21"/>
-    </row>
-    <row r="252" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E252" s="21"/>
+      <c r="G251" s="21"/>
+    </row>
+    <row r="252" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F252" s="21"/>
-    </row>
-    <row r="253" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E253" s="21"/>
+      <c r="G252" s="21"/>
+    </row>
+    <row r="253" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F253" s="21"/>
-    </row>
-    <row r="254" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E254" s="21"/>
+      <c r="G253" s="21"/>
+    </row>
+    <row r="254" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F254" s="21"/>
-    </row>
-    <row r="255" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E255" s="21"/>
+      <c r="G254" s="21"/>
+    </row>
+    <row r="255" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F255" s="21"/>
-    </row>
-    <row r="256" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E256" s="21"/>
+      <c r="G255" s="21"/>
+    </row>
+    <row r="256" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F256" s="21"/>
-    </row>
-    <row r="257" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E257" s="21"/>
+      <c r="G256" s="21"/>
+    </row>
+    <row r="257" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F257" s="21"/>
-    </row>
-    <row r="258" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E258" s="21"/>
+      <c r="G257" s="21"/>
+    </row>
+    <row r="258" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F258" s="21"/>
-    </row>
-    <row r="259" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E259" s="21"/>
+      <c r="G258" s="21"/>
+    </row>
+    <row r="259" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F259" s="21"/>
-    </row>
-    <row r="260" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E260" s="21"/>
+      <c r="G259" s="21"/>
+    </row>
+    <row r="260" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F260" s="21"/>
-    </row>
-    <row r="261" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E261" s="21"/>
+      <c r="G260" s="21"/>
+    </row>
+    <row r="261" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F261" s="21"/>
-    </row>
-    <row r="262" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E262" s="21"/>
+      <c r="G261" s="21"/>
+    </row>
+    <row r="262" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F262" s="21"/>
-    </row>
-    <row r="263" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E263" s="21"/>
+      <c r="G262" s="21"/>
+    </row>
+    <row r="263" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F263" s="21"/>
-    </row>
-    <row r="264" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E264" s="21"/>
+      <c r="G263" s="21"/>
+    </row>
+    <row r="264" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F264" s="21"/>
-    </row>
-    <row r="265" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E265" s="21"/>
+      <c r="G264" s="21"/>
+    </row>
+    <row r="265" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F265" s="21"/>
-    </row>
-    <row r="266" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E266" s="21"/>
+      <c r="G265" s="21"/>
+    </row>
+    <row r="266" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F266" s="21"/>
-    </row>
-    <row r="267" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E267" s="21"/>
+      <c r="G266" s="21"/>
+    </row>
+    <row r="267" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F267" s="21"/>
-    </row>
-    <row r="268" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E268" s="21"/>
+      <c r="G267" s="21"/>
+    </row>
+    <row r="268" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F268" s="21"/>
-    </row>
-    <row r="269" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E269" s="21"/>
+      <c r="G268" s="21"/>
+    </row>
+    <row r="269" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F269" s="21"/>
-    </row>
-    <row r="270" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E270" s="21"/>
+      <c r="G269" s="21"/>
+    </row>
+    <row r="270" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F270" s="21"/>
-    </row>
-    <row r="271" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E271" s="21"/>
+      <c r="G270" s="21"/>
+    </row>
+    <row r="271" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F271" s="21"/>
-    </row>
-    <row r="272" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E272" s="21"/>
+      <c r="G271" s="21"/>
+    </row>
+    <row r="272" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F272" s="21"/>
-    </row>
-    <row r="273" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E273" s="21"/>
+      <c r="G272" s="21"/>
+    </row>
+    <row r="273" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F273" s="21"/>
-    </row>
-    <row r="274" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E274" s="21"/>
+      <c r="G273" s="21"/>
+    </row>
+    <row r="274" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F274" s="21"/>
-    </row>
-    <row r="275" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E275" s="21"/>
+      <c r="G274" s="21"/>
+    </row>
+    <row r="275" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F275" s="21"/>
-    </row>
-    <row r="276" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E276" s="21"/>
+      <c r="G275" s="21"/>
+    </row>
+    <row r="276" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F276" s="21"/>
-    </row>
-    <row r="277" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E277" s="21"/>
+      <c r="G276" s="21"/>
+    </row>
+    <row r="277" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F277" s="21"/>
-    </row>
-    <row r="278" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E278" s="21"/>
+      <c r="G277" s="21"/>
+    </row>
+    <row r="278" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F278" s="21"/>
-    </row>
-    <row r="279" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E279" s="21"/>
+      <c r="G278" s="21"/>
+    </row>
+    <row r="279" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F279" s="21"/>
-    </row>
-    <row r="280" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E280" s="21"/>
+      <c r="G279" s="21"/>
+    </row>
+    <row r="280" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F280" s="21"/>
-    </row>
-    <row r="281" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E281" s="21"/>
+      <c r="G280" s="21"/>
+    </row>
+    <row r="281" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F281" s="21"/>
-    </row>
-    <row r="282" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E282" s="21"/>
+      <c r="G281" s="21"/>
+    </row>
+    <row r="282" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F282" s="21"/>
-    </row>
-    <row r="283" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E283" s="21"/>
+      <c r="G282" s="21"/>
+    </row>
+    <row r="283" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F283" s="21"/>
-    </row>
-    <row r="284" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E284" s="21"/>
+      <c r="G283" s="21"/>
+    </row>
+    <row r="284" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F284" s="21"/>
-    </row>
-    <row r="285" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E285" s="21"/>
+      <c r="G284" s="21"/>
+    </row>
+    <row r="285" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F285" s="21"/>
-    </row>
-    <row r="286" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E286" s="21"/>
+      <c r="G285" s="21"/>
+    </row>
+    <row r="286" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F286" s="21"/>
-    </row>
-    <row r="287" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E287" s="21"/>
+      <c r="G286" s="21"/>
+    </row>
+    <row r="287" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F287" s="21"/>
-    </row>
-    <row r="288" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E288" s="21"/>
+      <c r="G287" s="21"/>
+    </row>
+    <row r="288" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F288" s="21"/>
-    </row>
-    <row r="289" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E289" s="21"/>
+      <c r="G288" s="21"/>
+    </row>
+    <row r="289" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F289" s="21"/>
-    </row>
-    <row r="290" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E290" s="21"/>
+      <c r="G289" s="21"/>
+    </row>
+    <row r="290" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F290" s="21"/>
-    </row>
-    <row r="291" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E291" s="21"/>
+      <c r="G290" s="21"/>
+    </row>
+    <row r="291" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F291" s="21"/>
-    </row>
-    <row r="292" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E292" s="21"/>
+      <c r="G291" s="21"/>
+    </row>
+    <row r="292" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F292" s="21"/>
-    </row>
-    <row r="293" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E293" s="21"/>
+      <c r="G292" s="21"/>
+    </row>
+    <row r="293" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F293" s="21"/>
-    </row>
-    <row r="294" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E294" s="21"/>
+      <c r="G293" s="21"/>
+    </row>
+    <row r="294" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F294" s="21"/>
-    </row>
-    <row r="295" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E295" s="21"/>
+      <c r="G294" s="21"/>
+    </row>
+    <row r="295" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F295" s="21"/>
-    </row>
-    <row r="296" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E296" s="21"/>
+      <c r="G295" s="21"/>
+    </row>
+    <row r="296" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F296" s="21"/>
-    </row>
-    <row r="297" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E297" s="21"/>
+      <c r="G296" s="21"/>
+    </row>
+    <row r="297" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F297" s="21"/>
-    </row>
-    <row r="298" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E298" s="21"/>
+      <c r="G297" s="21"/>
+    </row>
+    <row r="298" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F298" s="21"/>
-    </row>
-    <row r="299" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E299" s="21"/>
+      <c r="G298" s="21"/>
+    </row>
+    <row r="299" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F299" s="21"/>
-    </row>
-    <row r="300" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E300" s="21"/>
+      <c r="G299" s="21"/>
+    </row>
+    <row r="300" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F300" s="21"/>
-    </row>
-    <row r="301" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E301" s="21"/>
+      <c r="G300" s="21"/>
+    </row>
+    <row r="301" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F301" s="21"/>
-    </row>
-    <row r="302" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E302" s="21"/>
+      <c r="G301" s="21"/>
+    </row>
+    <row r="302" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F302" s="21"/>
-    </row>
-    <row r="303" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E303" s="21"/>
+      <c r="G302" s="21"/>
+    </row>
+    <row r="303" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F303" s="21"/>
-    </row>
-    <row r="304" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E304" s="21"/>
+      <c r="G303" s="21"/>
+    </row>
+    <row r="304" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F304" s="21"/>
-    </row>
-    <row r="305" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E305" s="21"/>
+      <c r="G304" s="21"/>
+    </row>
+    <row r="305" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F305" s="21"/>
-    </row>
-    <row r="306" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E306" s="21"/>
+      <c r="G305" s="21"/>
+    </row>
+    <row r="306" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F306" s="21"/>
-    </row>
-    <row r="307" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E307" s="21"/>
+      <c r="G306" s="21"/>
+    </row>
+    <row r="307" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F307" s="21"/>
-    </row>
-    <row r="308" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E308" s="21"/>
+      <c r="G307" s="21"/>
+    </row>
+    <row r="308" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F308" s="21"/>
-    </row>
-    <row r="309" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E309" s="21"/>
+      <c r="G308" s="21"/>
+    </row>
+    <row r="309" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F309" s="21"/>
-    </row>
-    <row r="310" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E310" s="21"/>
+      <c r="G309" s="21"/>
+    </row>
+    <row r="310" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F310" s="21"/>
-    </row>
-    <row r="311" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E311" s="21"/>
+      <c r="G310" s="21"/>
+    </row>
+    <row r="311" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F311" s="21"/>
-    </row>
-    <row r="312" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E312" s="21"/>
+      <c r="G311" s="21"/>
+    </row>
+    <row r="312" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F312" s="21"/>
-    </row>
-    <row r="313" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E313" s="21"/>
+      <c r="G312" s="21"/>
+    </row>
+    <row r="313" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F313" s="21"/>
-    </row>
-    <row r="314" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E314" s="21"/>
+      <c r="G313" s="21"/>
+    </row>
+    <row r="314" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F314" s="21"/>
-    </row>
-    <row r="315" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E315" s="21"/>
+      <c r="G314" s="21"/>
+    </row>
+    <row r="315" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F315" s="21"/>
-    </row>
-    <row r="316" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E316" s="21"/>
+      <c r="G315" s="21"/>
+    </row>
+    <row r="316" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F316" s="21"/>
-    </row>
-    <row r="317" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E317" s="21"/>
+      <c r="G316" s="21"/>
+    </row>
+    <row r="317" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F317" s="21"/>
-    </row>
-    <row r="318" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E318" s="21"/>
+      <c r="G317" s="21"/>
+    </row>
+    <row r="318" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F318" s="21"/>
-    </row>
-    <row r="319" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E319" s="21"/>
+      <c r="G318" s="21"/>
+    </row>
+    <row r="319" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F319" s="21"/>
-    </row>
-    <row r="320" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E320" s="21"/>
+      <c r="G319" s="21"/>
+    </row>
+    <row r="320" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F320" s="21"/>
-    </row>
-    <row r="321" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E321" s="21"/>
+      <c r="G320" s="21"/>
+    </row>
+    <row r="321" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F321" s="21"/>
-    </row>
-    <row r="322" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E322" s="21"/>
+      <c r="G321" s="21"/>
+    </row>
+    <row r="322" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F322" s="21"/>
-    </row>
-    <row r="323" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E323" s="21"/>
+      <c r="G322" s="21"/>
+    </row>
+    <row r="323" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F323" s="21"/>
-    </row>
-    <row r="324" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E324" s="21"/>
+      <c r="G323" s="21"/>
+    </row>
+    <row r="324" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F324" s="21"/>
-    </row>
-    <row r="325" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E325" s="21"/>
+      <c r="G324" s="21"/>
+    </row>
+    <row r="325" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F325" s="21"/>
-    </row>
-    <row r="326" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E326" s="21"/>
+      <c r="G325" s="21"/>
+    </row>
+    <row r="326" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F326" s="21"/>
-    </row>
-    <row r="327" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E327" s="21"/>
+      <c r="G326" s="21"/>
+    </row>
+    <row r="327" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F327" s="21"/>
-    </row>
-    <row r="328" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E328" s="21"/>
+      <c r="G327" s="21"/>
+    </row>
+    <row r="328" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F328" s="21"/>
-    </row>
-    <row r="329" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E329" s="21"/>
+      <c r="G328" s="21"/>
+    </row>
+    <row r="329" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F329" s="21"/>
-    </row>
-    <row r="330" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E330" s="21"/>
+      <c r="G329" s="21"/>
+    </row>
+    <row r="330" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F330" s="21"/>
-    </row>
-    <row r="331" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E331" s="21"/>
+      <c r="G330" s="21"/>
+    </row>
+    <row r="331" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F331" s="21"/>
-    </row>
-    <row r="332" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E332" s="21"/>
+      <c r="G331" s="21"/>
+    </row>
+    <row r="332" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F332" s="21"/>
-    </row>
-    <row r="333" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E333" s="21"/>
+      <c r="G332" s="21"/>
+    </row>
+    <row r="333" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F333" s="21"/>
-    </row>
-    <row r="334" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E334" s="21"/>
+      <c r="G333" s="21"/>
+    </row>
+    <row r="334" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F334" s="21"/>
-    </row>
-    <row r="335" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E335" s="21"/>
+      <c r="G334" s="21"/>
+    </row>
+    <row r="335" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F335" s="21"/>
-    </row>
-    <row r="336" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E336" s="21"/>
+      <c r="G335" s="21"/>
+    </row>
+    <row r="336" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F336" s="21"/>
-    </row>
-    <row r="337" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E337" s="21"/>
+      <c r="G336" s="21"/>
+    </row>
+    <row r="337" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F337" s="21"/>
-    </row>
-    <row r="338" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E338" s="21"/>
+      <c r="G337" s="21"/>
+    </row>
+    <row r="338" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F338" s="21"/>
-    </row>
-    <row r="339" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E339" s="21"/>
+      <c r="G338" s="21"/>
+    </row>
+    <row r="339" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F339" s="21"/>
-    </row>
-    <row r="340" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E340" s="21"/>
+      <c r="G339" s="21"/>
+    </row>
+    <row r="340" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F340" s="21"/>
-    </row>
-    <row r="341" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E341" s="21"/>
+      <c r="G340" s="21"/>
+    </row>
+    <row r="341" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F341" s="21"/>
-    </row>
-    <row r="342" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E342" s="21"/>
+      <c r="G341" s="21"/>
+    </row>
+    <row r="342" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F342" s="21"/>
-    </row>
-    <row r="343" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E343" s="21"/>
+      <c r="G342" s="21"/>
+    </row>
+    <row r="343" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F343" s="21"/>
-    </row>
-    <row r="344" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E344" s="21"/>
+      <c r="G343" s="21"/>
+    </row>
+    <row r="344" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F344" s="21"/>
-    </row>
-    <row r="345" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E345" s="21"/>
+      <c r="G344" s="21"/>
+    </row>
+    <row r="345" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F345" s="21"/>
-    </row>
-    <row r="346" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E346" s="21"/>
+      <c r="G345" s="21"/>
+    </row>
+    <row r="346" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F346" s="21"/>
-    </row>
-    <row r="347" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E347" s="21"/>
+      <c r="G346" s="21"/>
+    </row>
+    <row r="347" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F347" s="21"/>
-    </row>
-    <row r="348" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E348" s="21"/>
+      <c r="G347" s="21"/>
+    </row>
+    <row r="348" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F348" s="21"/>
-    </row>
-    <row r="349" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E349" s="21"/>
+      <c r="G348" s="21"/>
+    </row>
+    <row r="349" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F349" s="21"/>
-    </row>
-    <row r="350" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E350" s="21"/>
+      <c r="G349" s="21"/>
+    </row>
+    <row r="350" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F350" s="21"/>
-    </row>
-    <row r="351" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E351" s="21"/>
+      <c r="G350" s="21"/>
+    </row>
+    <row r="351" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F351" s="21"/>
-    </row>
-    <row r="352" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E352" s="21"/>
+      <c r="G351" s="21"/>
+    </row>
+    <row r="352" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F352" s="21"/>
-    </row>
-    <row r="353" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E353" s="21"/>
+      <c r="G352" s="21"/>
+    </row>
+    <row r="353" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F353" s="21"/>
-    </row>
-    <row r="354" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E354" s="21"/>
+      <c r="G353" s="21"/>
+    </row>
+    <row r="354" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F354" s="21"/>
-    </row>
-    <row r="355" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E355" s="21"/>
+      <c r="G354" s="21"/>
+    </row>
+    <row r="355" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F355" s="21"/>
-    </row>
-    <row r="356" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E356" s="21"/>
+      <c r="G355" s="21"/>
+    </row>
+    <row r="356" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F356" s="21"/>
-    </row>
-    <row r="357" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E357" s="21"/>
+      <c r="G356" s="21"/>
+    </row>
+    <row r="357" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F357" s="21"/>
-    </row>
-    <row r="358" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E358" s="21"/>
+      <c r="G357" s="21"/>
+    </row>
+    <row r="358" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F358" s="21"/>
-    </row>
-    <row r="359" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E359" s="21"/>
+      <c r="G358" s="21"/>
+    </row>
+    <row r="359" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F359" s="21"/>
-    </row>
-    <row r="360" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E360" s="21"/>
+      <c r="G359" s="21"/>
+    </row>
+    <row r="360" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F360" s="21"/>
-    </row>
-    <row r="361" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E361" s="21"/>
+      <c r="G360" s="21"/>
+    </row>
+    <row r="361" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F361" s="21"/>
-    </row>
-    <row r="362" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E362" s="21"/>
+      <c r="G361" s="21"/>
+    </row>
+    <row r="362" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F362" s="21"/>
-    </row>
-    <row r="369" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E369" s="21"/>
+      <c r="G362" s="21"/>
+    </row>
+    <row r="369" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F369" s="21"/>
-    </row>
-    <row r="370" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E370" s="21"/>
+      <c r="G369" s="21"/>
+    </row>
+    <row r="370" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F370" s="21"/>
-    </row>
-    <row r="371" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E371" s="21"/>
+      <c r="G370" s="21"/>
+    </row>
+    <row r="371" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F371" s="21"/>
-    </row>
-    <row r="372" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E372" s="21"/>
+      <c r="G371" s="21"/>
+    </row>
+    <row r="372" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F372" s="21"/>
-    </row>
-    <row r="373" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E373" s="21"/>
+      <c r="G372" s="21"/>
+    </row>
+    <row r="373" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F373" s="21"/>
-    </row>
-    <row r="374" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E374" s="21"/>
+      <c r="G373" s="21"/>
+    </row>
+    <row r="374" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F374" s="21"/>
-    </row>
-    <row r="375" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E375" s="21"/>
+      <c r="G374" s="21"/>
+    </row>
+    <row r="375" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F375" s="21"/>
-    </row>
-    <row r="376" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E376" s="21"/>
+      <c r="G375" s="21"/>
+    </row>
+    <row r="376" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F376" s="21"/>
-    </row>
-    <row r="377" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E377" s="21"/>
+      <c r="G376" s="21"/>
+    </row>
+    <row r="377" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F377" s="21"/>
-    </row>
-    <row r="378" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E378" s="21"/>
+      <c r="G377" s="21"/>
+    </row>
+    <row r="378" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F378" s="21"/>
-    </row>
-    <row r="379" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E379" s="21"/>
+      <c r="G378" s="21"/>
+    </row>
+    <row r="379" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F379" s="21"/>
-    </row>
-    <row r="380" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E380" s="21"/>
+      <c r="G379" s="21"/>
+    </row>
+    <row r="380" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F380" s="21"/>
-    </row>
-    <row r="381" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E381" s="21"/>
+      <c r="G380" s="21"/>
+    </row>
+    <row r="381" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F381" s="21"/>
-    </row>
-    <row r="382" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E382" s="21"/>
+      <c r="G381" s="21"/>
+    </row>
+    <row r="382" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F382" s="21"/>
-    </row>
-    <row r="383" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E383" s="21"/>
+      <c r="G382" s="21"/>
+    </row>
+    <row r="383" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F383" s="21"/>
-    </row>
-    <row r="384" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E384" s="21"/>
+      <c r="G383" s="21"/>
+    </row>
+    <row r="384" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F384" s="21"/>
-    </row>
-    <row r="385" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E385" s="21"/>
+      <c r="G384" s="21"/>
+    </row>
+    <row r="385" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F385" s="21"/>
-    </row>
-    <row r="386" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E386" s="21"/>
+      <c r="G385" s="21"/>
+    </row>
+    <row r="386" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F386" s="21"/>
-    </row>
-    <row r="387" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E387" s="21"/>
+      <c r="G386" s="21"/>
+    </row>
+    <row r="387" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F387" s="21"/>
-    </row>
-    <row r="388" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E388" s="21"/>
+      <c r="G387" s="21"/>
+    </row>
+    <row r="388" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F388" s="21"/>
-    </row>
-    <row r="389" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E389" s="21"/>
+      <c r="G388" s="21"/>
+    </row>
+    <row r="389" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F389" s="21"/>
-    </row>
-    <row r="390" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E390" s="21"/>
+      <c r="G389" s="21"/>
+    </row>
+    <row r="390" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F390" s="21"/>
-    </row>
-    <row r="391" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E391" s="21"/>
+      <c r="G390" s="21"/>
+    </row>
+    <row r="391" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F391" s="21"/>
-    </row>
-    <row r="392" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E392" s="21"/>
+      <c r="G391" s="21"/>
+    </row>
+    <row r="392" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F392" s="21"/>
-    </row>
-    <row r="393" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E393" s="21"/>
+      <c r="G392" s="21"/>
+    </row>
+    <row r="393" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F393" s="21"/>
-    </row>
-    <row r="394" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E394" s="21"/>
+      <c r="G393" s="21"/>
+    </row>
+    <row r="394" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F394" s="21"/>
-    </row>
-    <row r="395" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E395" s="21"/>
+      <c r="G394" s="21"/>
+    </row>
+    <row r="395" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F395" s="21"/>
-    </row>
-    <row r="396" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E396" s="21"/>
+      <c r="G395" s="21"/>
+    </row>
+    <row r="396" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F396" s="21"/>
-    </row>
-    <row r="397" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E397" s="21"/>
+      <c r="G396" s="21"/>
+    </row>
+    <row r="397" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F397" s="21"/>
-    </row>
-    <row r="398" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E398" s="21"/>
+      <c r="G397" s="21"/>
+    </row>
+    <row r="398" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F398" s="21"/>
-    </row>
-    <row r="399" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E399" s="21"/>
+      <c r="G398" s="21"/>
+    </row>
+    <row r="399" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F399" s="21"/>
-    </row>
-    <row r="400" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E400" s="21"/>
+      <c r="G399" s="21"/>
+    </row>
+    <row r="400" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F400" s="21"/>
-    </row>
-    <row r="401" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E401" s="21"/>
+      <c r="G400" s="21"/>
+    </row>
+    <row r="401" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F401" s="21"/>
-    </row>
-    <row r="402" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E402" s="21"/>
+      <c r="G401" s="21"/>
+    </row>
+    <row r="402" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F402" s="21"/>
-    </row>
-    <row r="403" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E403" s="21"/>
+      <c r="G402" s="21"/>
+    </row>
+    <row r="403" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F403" s="21"/>
-    </row>
-    <row r="404" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E404" s="21"/>
+      <c r="G403" s="21"/>
+    </row>
+    <row r="404" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F404" s="21"/>
-    </row>
-    <row r="405" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E405" s="21"/>
+      <c r="G404" s="21"/>
+    </row>
+    <row r="405" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F405" s="21"/>
-    </row>
-    <row r="406" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E406" s="21"/>
+      <c r="G405" s="21"/>
+    </row>
+    <row r="406" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F406" s="21"/>
-    </row>
-    <row r="407" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E407" s="21"/>
+      <c r="G406" s="21"/>
+    </row>
+    <row r="407" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F407" s="21"/>
-    </row>
-    <row r="408" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E408" s="21"/>
+      <c r="G407" s="21"/>
+    </row>
+    <row r="408" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F408" s="21"/>
-    </row>
-    <row r="409" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E409" s="21"/>
+      <c r="G408" s="21"/>
+    </row>
+    <row r="409" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F409" s="21"/>
-    </row>
-    <row r="410" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E410" s="21"/>
+      <c r="G409" s="21"/>
+    </row>
+    <row r="410" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F410" s="21"/>
-    </row>
-    <row r="411" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E411" s="21"/>
+      <c r="G410" s="21"/>
+    </row>
+    <row r="411" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F411" s="21"/>
-    </row>
-    <row r="412" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E412" s="21"/>
+      <c r="G411" s="21"/>
+    </row>
+    <row r="412" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F412" s="21"/>
-    </row>
-    <row r="413" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E413" s="21"/>
+      <c r="G412" s="21"/>
+    </row>
+    <row r="413" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F413" s="21"/>
-    </row>
-    <row r="414" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E414" s="21"/>
+      <c r="G413" s="21"/>
+    </row>
+    <row r="414" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F414" s="21"/>
-    </row>
-    <row r="415" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E415" s="21"/>
+      <c r="G414" s="21"/>
+    </row>
+    <row r="415" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F415" s="21"/>
-    </row>
-    <row r="416" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E416" s="21"/>
+      <c r="G415" s="21"/>
+    </row>
+    <row r="416" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F416" s="21"/>
-    </row>
-    <row r="417" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E417" s="21"/>
+      <c r="G416" s="21"/>
+    </row>
+    <row r="417" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F417" s="21"/>
-    </row>
-    <row r="418" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E418" s="21"/>
+      <c r="G417" s="21"/>
+    </row>
+    <row r="418" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F418" s="21"/>
-    </row>
-    <row r="419" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E419" s="21"/>
+      <c r="G418" s="21"/>
+    </row>
+    <row r="419" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F419" s="21"/>
-    </row>
-    <row r="420" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E420" s="21"/>
+      <c r="G419" s="21"/>
+    </row>
+    <row r="420" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F420" s="21"/>
-    </row>
-    <row r="421" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E421" s="21"/>
+      <c r="G420" s="21"/>
+    </row>
+    <row r="421" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F421" s="21"/>
-    </row>
-    <row r="422" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E422" s="21"/>
+      <c r="G421" s="21"/>
+    </row>
+    <row r="422" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F422" s="21"/>
-    </row>
-    <row r="423" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E423" s="21"/>
+      <c r="G422" s="21"/>
+    </row>
+    <row r="423" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F423" s="21"/>
-    </row>
-    <row r="424" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E424" s="21"/>
+      <c r="G423" s="21"/>
+    </row>
+    <row r="424" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F424" s="21"/>
-    </row>
-    <row r="425" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E425" s="21"/>
+      <c r="G424" s="21"/>
+    </row>
+    <row r="425" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F425" s="21"/>
-    </row>
-    <row r="426" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E426" s="21"/>
+      <c r="G425" s="21"/>
+    </row>
+    <row r="426" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F426" s="21"/>
-    </row>
-    <row r="427" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E427" s="21"/>
+      <c r="G426" s="21"/>
+    </row>
+    <row r="427" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F427" s="21"/>
-    </row>
-    <row r="428" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E428" s="21"/>
+      <c r="G427" s="21"/>
+    </row>
+    <row r="428" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F428" s="21"/>
-    </row>
-    <row r="429" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E429" s="21"/>
+      <c r="G428" s="21"/>
+    </row>
+    <row r="429" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F429" s="21"/>
-    </row>
-    <row r="430" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E430" s="21"/>
+      <c r="G429" s="21"/>
+    </row>
+    <row r="430" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F430" s="21"/>
-    </row>
-    <row r="431" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E431" s="21"/>
+      <c r="G430" s="21"/>
+    </row>
+    <row r="431" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F431" s="21"/>
-    </row>
-    <row r="432" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E432" s="21"/>
+      <c r="G431" s="21"/>
+    </row>
+    <row r="432" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F432" s="21"/>
-    </row>
-    <row r="433" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E433" s="21"/>
+      <c r="G432" s="21"/>
+    </row>
+    <row r="433" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F433" s="21"/>
-    </row>
-    <row r="434" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E434" s="21"/>
+      <c r="G433" s="21"/>
+    </row>
+    <row r="434" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F434" s="21"/>
-    </row>
-    <row r="435" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E435" s="21"/>
+      <c r="G434" s="21"/>
+    </row>
+    <row r="435" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F435" s="21"/>
-    </row>
-    <row r="436" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E436" s="21"/>
+      <c r="G435" s="21"/>
+    </row>
+    <row r="436" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F436" s="21"/>
-    </row>
-    <row r="437" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E437" s="21"/>
+      <c r="G436" s="21"/>
+    </row>
+    <row r="437" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F437" s="21"/>
-    </row>
-    <row r="438" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E438" s="21"/>
+      <c r="G437" s="21"/>
+    </row>
+    <row r="438" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F438" s="21"/>
-    </row>
-    <row r="439" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E439" s="21"/>
+      <c r="G438" s="21"/>
+    </row>
+    <row r="439" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F439" s="21"/>
-    </row>
-    <row r="440" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E440" s="21"/>
+      <c r="G439" s="21"/>
+    </row>
+    <row r="440" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F440" s="21"/>
-    </row>
-    <row r="441" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E441" s="21"/>
+      <c r="G440" s="21"/>
+    </row>
+    <row r="441" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F441" s="21"/>
-    </row>
-    <row r="442" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E442" s="21"/>
+      <c r="G441" s="21"/>
+    </row>
+    <row r="442" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F442" s="21"/>
-    </row>
-    <row r="443" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E443" s="21"/>
+      <c r="G442" s="21"/>
+    </row>
+    <row r="443" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F443" s="21"/>
-    </row>
-    <row r="444" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E444" s="21"/>
+      <c r="G443" s="21"/>
+    </row>
+    <row r="444" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F444" s="21"/>
-    </row>
-    <row r="445" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E445" s="21"/>
+      <c r="G444" s="21"/>
+    </row>
+    <row r="445" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F445" s="21"/>
-    </row>
-    <row r="446" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E446" s="21"/>
+      <c r="G445" s="21"/>
+    </row>
+    <row r="446" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F446" s="21"/>
-    </row>
-    <row r="447" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E447" s="21"/>
+      <c r="G446" s="21"/>
+    </row>
+    <row r="447" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F447" s="21"/>
-    </row>
-    <row r="448" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E448" s="21"/>
+      <c r="G447" s="21"/>
+    </row>
+    <row r="448" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F448" s="21"/>
-    </row>
-    <row r="449" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E449" s="21"/>
+      <c r="G448" s="21"/>
+    </row>
+    <row r="449" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F449" s="21"/>
-    </row>
-    <row r="450" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E450" s="21"/>
+      <c r="G449" s="21"/>
+    </row>
+    <row r="450" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F450" s="21"/>
-    </row>
-    <row r="451" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E451" s="21"/>
+      <c r="G450" s="21"/>
+    </row>
+    <row r="451" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F451" s="21"/>
-    </row>
-    <row r="452" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E452" s="21"/>
+      <c r="G451" s="21"/>
+    </row>
+    <row r="452" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F452" s="21"/>
-    </row>
-    <row r="453" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E453" s="21"/>
+      <c r="G452" s="21"/>
+    </row>
+    <row r="453" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F453" s="21"/>
-    </row>
-    <row r="454" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E454" s="21"/>
+      <c r="G453" s="21"/>
+    </row>
+    <row r="454" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F454" s="21"/>
-    </row>
-    <row r="455" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E455" s="21"/>
+      <c r="G454" s="21"/>
+    </row>
+    <row r="455" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F455" s="21"/>
-    </row>
-    <row r="456" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E456" s="21"/>
+      <c r="G455" s="21"/>
+    </row>
+    <row r="456" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F456" s="21"/>
-    </row>
-    <row r="457" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E457" s="21"/>
+      <c r="G456" s="21"/>
+    </row>
+    <row r="457" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F457" s="21"/>
-    </row>
-    <row r="458" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E458" s="21"/>
+      <c r="G457" s="21"/>
+    </row>
+    <row r="458" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F458" s="21"/>
-    </row>
-    <row r="459" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E459" s="21"/>
+      <c r="G458" s="21"/>
+    </row>
+    <row r="459" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F459" s="21"/>
-    </row>
-    <row r="460" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E460" s="21"/>
+      <c r="G459" s="21"/>
+    </row>
+    <row r="460" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F460" s="21"/>
-    </row>
-    <row r="461" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E461" s="21"/>
+      <c r="G460" s="21"/>
+    </row>
+    <row r="461" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F461" s="21"/>
-    </row>
-    <row r="462" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E462" s="21"/>
+      <c r="G461" s="21"/>
+    </row>
+    <row r="462" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F462" s="21"/>
-    </row>
-    <row r="463" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E463" s="21"/>
+      <c r="G462" s="21"/>
+    </row>
+    <row r="463" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F463" s="21"/>
-    </row>
-    <row r="464" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E464" s="21"/>
+      <c r="G463" s="21"/>
+    </row>
+    <row r="464" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F464" s="21"/>
-    </row>
-    <row r="465" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E465" s="21"/>
+      <c r="G464" s="21"/>
+    </row>
+    <row r="465" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F465" s="21"/>
-    </row>
-    <row r="466" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E466" s="21"/>
+      <c r="G465" s="21"/>
+    </row>
+    <row r="466" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F466" s="21"/>
-    </row>
-    <row r="467" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E467" s="21"/>
+      <c r="G466" s="21"/>
+    </row>
+    <row r="467" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F467" s="21"/>
-    </row>
-    <row r="468" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E468" s="21"/>
+      <c r="G467" s="21"/>
+    </row>
+    <row r="468" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F468" s="21"/>
-    </row>
-    <row r="469" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E469" s="21"/>
+      <c r="G468" s="21"/>
+    </row>
+    <row r="469" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F469" s="21"/>
-    </row>
-    <row r="470" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E470" s="21"/>
+      <c r="G469" s="21"/>
+    </row>
+    <row r="470" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F470" s="21"/>
-    </row>
-    <row r="471" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E471" s="21"/>
+      <c r="G470" s="21"/>
+    </row>
+    <row r="471" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F471" s="21"/>
-    </row>
-    <row r="472" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E472" s="21"/>
+      <c r="G471" s="21"/>
+    </row>
+    <row r="472" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F472" s="21"/>
-    </row>
-    <row r="473" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E473" s="21"/>
+      <c r="G472" s="21"/>
+    </row>
+    <row r="473" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F473" s="21"/>
-    </row>
-    <row r="474" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E474" s="21"/>
+      <c r="G473" s="21"/>
+    </row>
+    <row r="474" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F474" s="21"/>
-    </row>
-    <row r="475" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E475" s="21"/>
+      <c r="G474" s="21"/>
+    </row>
+    <row r="475" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F475" s="21"/>
-    </row>
-    <row r="476" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E476" s="21"/>
+      <c r="G475" s="21"/>
+    </row>
+    <row r="476" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F476" s="21"/>
-    </row>
-    <row r="477" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E477" s="21"/>
+      <c r="G476" s="21"/>
+    </row>
+    <row r="477" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F477" s="21"/>
-    </row>
-    <row r="478" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E478" s="21"/>
+      <c r="G477" s="21"/>
+    </row>
+    <row r="478" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F478" s="21"/>
-    </row>
-    <row r="479" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E479" s="21"/>
+      <c r="G478" s="21"/>
+    </row>
+    <row r="479" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F479" s="21"/>
-    </row>
-    <row r="480" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E480" s="21"/>
+      <c r="G479" s="21"/>
+    </row>
+    <row r="480" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F480" s="21"/>
-    </row>
-    <row r="481" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E481" s="21"/>
+      <c r="G480" s="21"/>
+    </row>
+    <row r="481" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F481" s="21"/>
-    </row>
-    <row r="482" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E482" s="21"/>
+      <c r="G481" s="21"/>
+    </row>
+    <row r="482" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F482" s="21"/>
-    </row>
-    <row r="483" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E483" s="21"/>
+      <c r="G482" s="21"/>
+    </row>
+    <row r="483" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F483" s="21"/>
-    </row>
-    <row r="484" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E484" s="21"/>
+      <c r="G483" s="21"/>
+    </row>
+    <row r="484" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F484" s="21"/>
-    </row>
-    <row r="485" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E485" s="21"/>
+      <c r="G484" s="21"/>
+    </row>
+    <row r="485" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F485" s="21"/>
-    </row>
-    <row r="486" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E486" s="21"/>
+      <c r="G485" s="21"/>
+    </row>
+    <row r="486" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F486" s="21"/>
-    </row>
-    <row r="487" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E487" s="21"/>
+      <c r="G486" s="21"/>
+    </row>
+    <row r="487" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F487" s="21"/>
-    </row>
-    <row r="488" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E488" s="21"/>
+      <c r="G487" s="21"/>
+    </row>
+    <row r="488" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F488" s="21"/>
-    </row>
-    <row r="489" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E489" s="21"/>
+      <c r="G488" s="21"/>
+    </row>
+    <row r="489" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F489" s="21"/>
-    </row>
-    <row r="490" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E490" s="21"/>
+      <c r="G489" s="21"/>
+    </row>
+    <row r="490" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F490" s="21"/>
-    </row>
-    <row r="491" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E491" s="21"/>
+      <c r="G490" s="21"/>
+    </row>
+    <row r="491" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F491" s="21"/>
-    </row>
-    <row r="492" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E492" s="21"/>
+      <c r="G491" s="21"/>
+    </row>
+    <row r="492" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F492" s="21"/>
-    </row>
-    <row r="493" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E493" s="21"/>
+      <c r="G492" s="21"/>
+    </row>
+    <row r="493" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F493" s="21"/>
-    </row>
-    <row r="494" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E494" s="21"/>
+      <c r="G493" s="21"/>
+    </row>
+    <row r="494" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F494" s="21"/>
-    </row>
-    <row r="495" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E495" s="21"/>
+      <c r="G494" s="21"/>
+    </row>
+    <row r="495" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F495" s="21"/>
-    </row>
-    <row r="496" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E496" s="21"/>
+      <c r="G495" s="21"/>
+    </row>
+    <row r="496" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F496" s="21"/>
-    </row>
-    <row r="497" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E497" s="21"/>
+      <c r="G496" s="21"/>
+    </row>
+    <row r="497" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F497" s="21"/>
-    </row>
-    <row r="498" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E498" s="21"/>
+      <c r="G497" s="21"/>
+    </row>
+    <row r="498" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F498" s="21"/>
-    </row>
-    <row r="499" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E499" s="21"/>
+      <c r="G498" s="21"/>
+    </row>
+    <row r="499" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F499" s="21"/>
-    </row>
-    <row r="500" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E500" s="21"/>
+      <c r="G499" s="21"/>
+    </row>
+    <row r="500" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F500" s="21"/>
-    </row>
-    <row r="501" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E501" s="21"/>
+      <c r="G500" s="21"/>
+    </row>
+    <row r="501" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F501" s="21"/>
-    </row>
-    <row r="502" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E502" s="21"/>
+      <c r="G501" s="21"/>
+    </row>
+    <row r="502" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F502" s="21"/>
-    </row>
-    <row r="503" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E503" s="21"/>
+      <c r="G502" s="21"/>
+    </row>
+    <row r="503" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F503" s="21"/>
-    </row>
-    <row r="504" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E504" s="21"/>
+      <c r="G503" s="21"/>
+    </row>
+    <row r="504" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F504" s="21"/>
-    </row>
-    <row r="505" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E505" s="21"/>
+      <c r="G504" s="21"/>
+    </row>
+    <row r="505" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F505" s="21"/>
-    </row>
-    <row r="506" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E506" s="21"/>
+      <c r="G505" s="21"/>
+    </row>
+    <row r="506" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F506" s="21"/>
-    </row>
-    <row r="507" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E507" s="21"/>
+      <c r="G506" s="21"/>
+    </row>
+    <row r="507" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F507" s="21"/>
-    </row>
-    <row r="508" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E508" s="21"/>
+      <c r="G507" s="21"/>
+    </row>
+    <row r="508" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F508" s="21"/>
-    </row>
-    <row r="509" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E509" s="21"/>
+      <c r="G508" s="21"/>
+    </row>
+    <row r="509" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F509" s="21"/>
-    </row>
-    <row r="510" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E510" s="21"/>
+      <c r="G509" s="21"/>
+    </row>
+    <row r="510" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F510" s="21"/>
-    </row>
-    <row r="511" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E511" s="21"/>
+      <c r="G510" s="21"/>
+    </row>
+    <row r="511" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F511" s="21"/>
-    </row>
-    <row r="512" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E512" s="21"/>
+      <c r="G511" s="21"/>
+    </row>
+    <row r="512" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F512" s="21"/>
-    </row>
-    <row r="513" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E513" s="21"/>
+      <c r="G512" s="21"/>
+    </row>
+    <row r="513" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F513" s="21"/>
-    </row>
-    <row r="514" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E514" s="21"/>
+      <c r="G513" s="21"/>
+    </row>
+    <row r="514" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F514" s="21"/>
-    </row>
-    <row r="515" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E515" s="21"/>
+      <c r="G514" s="21"/>
+    </row>
+    <row r="515" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F515" s="21"/>
-    </row>
-    <row r="516" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E516" s="21"/>
+      <c r="G515" s="21"/>
+    </row>
+    <row r="516" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F516" s="21"/>
-    </row>
-    <row r="517" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E517" s="21"/>
+      <c r="G516" s="21"/>
+    </row>
+    <row r="517" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F517" s="21"/>
-    </row>
-    <row r="518" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E518" s="21"/>
+      <c r="G517" s="21"/>
+    </row>
+    <row r="518" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F518" s="21"/>
-    </row>
-    <row r="519" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E519" s="21"/>
+      <c r="G518" s="21"/>
+    </row>
+    <row r="519" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F519" s="21"/>
-    </row>
-    <row r="520" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E520" s="21"/>
+      <c r="G519" s="21"/>
+    </row>
+    <row r="520" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F520" s="21"/>
-    </row>
-    <row r="521" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E521" s="21"/>
+      <c r="G520" s="21"/>
+    </row>
+    <row r="521" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F521" s="21"/>
-    </row>
-    <row r="522" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E522" s="21"/>
+      <c r="G521" s="21"/>
+    </row>
+    <row r="522" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F522" s="21"/>
-    </row>
-    <row r="523" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E523" s="21"/>
+      <c r="G522" s="21"/>
+    </row>
+    <row r="523" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F523" s="21"/>
-    </row>
-    <row r="524" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E524" s="21"/>
+      <c r="G523" s="21"/>
+    </row>
+    <row r="524" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F524" s="21"/>
-    </row>
-    <row r="525" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E525" s="21"/>
+      <c r="G524" s="21"/>
+    </row>
+    <row r="525" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F525" s="21"/>
-    </row>
-    <row r="526" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E526" s="21"/>
+      <c r="G525" s="21"/>
+    </row>
+    <row r="526" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F526" s="21"/>
-    </row>
-    <row r="527" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E527" s="21"/>
+      <c r="G526" s="21"/>
+    </row>
+    <row r="527" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F527" s="21"/>
-    </row>
-    <row r="528" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E528" s="21"/>
+      <c r="G527" s="21"/>
+    </row>
+    <row r="528" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F528" s="21"/>
-    </row>
-    <row r="529" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E529" s="21"/>
+      <c r="G528" s="21"/>
+    </row>
+    <row r="529" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F529" s="21"/>
-    </row>
-    <row r="530" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E530" s="21"/>
+      <c r="G529" s="21"/>
+    </row>
+    <row r="530" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F530" s="21"/>
-    </row>
-    <row r="531" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E531" s="21"/>
+      <c r="G530" s="21"/>
+    </row>
+    <row r="531" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F531" s="21"/>
-    </row>
-    <row r="532" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E532" s="21"/>
+      <c r="G531" s="21"/>
+    </row>
+    <row r="532" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F532" s="21"/>
-    </row>
-    <row r="533" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E533" s="21"/>
+      <c r="G532" s="21"/>
+    </row>
+    <row r="533" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F533" s="21"/>
-    </row>
-    <row r="534" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E534" s="21"/>
+      <c r="G533" s="21"/>
+    </row>
+    <row r="534" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F534" s="21"/>
-    </row>
-    <row r="535" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E535" s="21"/>
+      <c r="G534" s="21"/>
+    </row>
+    <row r="535" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F535" s="21"/>
-    </row>
-    <row r="536" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E536" s="21"/>
+      <c r="G535" s="21"/>
+    </row>
+    <row r="536" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F536" s="21"/>
-    </row>
-    <row r="537" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E537" s="21"/>
+      <c r="G536" s="21"/>
+    </row>
+    <row r="537" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F537" s="21"/>
-    </row>
-    <row r="538" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E538" s="21"/>
+      <c r="G537" s="21"/>
+    </row>
+    <row r="538" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F538" s="21"/>
-    </row>
-    <row r="539" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E539" s="21"/>
+      <c r="G538" s="21"/>
+    </row>
+    <row r="539" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F539" s="21"/>
-    </row>
-    <row r="540" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E540" s="21"/>
+      <c r="G539" s="21"/>
+    </row>
+    <row r="540" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F540" s="21"/>
-    </row>
-    <row r="541" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E541" s="21"/>
+      <c r="G540" s="21"/>
+    </row>
+    <row r="541" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F541" s="21"/>
-    </row>
-    <row r="542" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E542" s="21"/>
+      <c r="G541" s="21"/>
+    </row>
+    <row r="542" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F542" s="21"/>
-    </row>
-    <row r="543" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E543" s="21"/>
+      <c r="G542" s="21"/>
+    </row>
+    <row r="543" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F543" s="21"/>
-    </row>
-    <row r="544" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E544" s="21"/>
+      <c r="G543" s="21"/>
+    </row>
+    <row r="544" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F544" s="21"/>
-    </row>
-    <row r="545" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E545" s="21"/>
+      <c r="G544" s="21"/>
+    </row>
+    <row r="545" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F545" s="21"/>
-    </row>
-    <row r="546" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E546" s="21"/>
+      <c r="G545" s="21"/>
+    </row>
+    <row r="546" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F546" s="21"/>
-    </row>
-    <row r="547" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E547" s="21"/>
+      <c r="G546" s="21"/>
+    </row>
+    <row r="547" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F547" s="21"/>
-    </row>
-    <row r="548" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E548" s="21"/>
+      <c r="G547" s="21"/>
+    </row>
+    <row r="548" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F548" s="21"/>
-    </row>
-    <row r="549" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E549" s="21"/>
+      <c r="G548" s="21"/>
+    </row>
+    <row r="549" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F549" s="21"/>
-    </row>
-    <row r="550" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E550" s="21"/>
+      <c r="G549" s="21"/>
+    </row>
+    <row r="550" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F550" s="21"/>
-    </row>
-    <row r="551" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E551" s="21"/>
+      <c r="G550" s="21"/>
+    </row>
+    <row r="551" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F551" s="21"/>
-    </row>
-    <row r="552" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E552" s="21"/>
+      <c r="G551" s="21"/>
+    </row>
+    <row r="552" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F552" s="21"/>
-    </row>
-    <row r="553" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E553" s="21"/>
+      <c r="G552" s="21"/>
+    </row>
+    <row r="553" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F553" s="21"/>
-    </row>
-    <row r="554" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E554" s="21"/>
+      <c r="G553" s="21"/>
+    </row>
+    <row r="554" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F554" s="21"/>
-    </row>
-    <row r="555" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E555" s="21"/>
+      <c r="G554" s="21"/>
+    </row>
+    <row r="555" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F555" s="21"/>
-    </row>
-    <row r="556" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E556" s="21"/>
+      <c r="G555" s="21"/>
+    </row>
+    <row r="556" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F556" s="21"/>
-    </row>
-    <row r="557" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E557" s="21"/>
+      <c r="G556" s="21"/>
+    </row>
+    <row r="557" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F557" s="21"/>
-    </row>
-    <row r="558" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E558" s="21"/>
+      <c r="G557" s="21"/>
+    </row>
+    <row r="558" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F558" s="21"/>
-    </row>
-    <row r="559" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E559" s="21"/>
+      <c r="G558" s="21"/>
+    </row>
+    <row r="559" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F559" s="21"/>
-    </row>
-    <row r="560" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E560" s="21"/>
+      <c r="G559" s="21"/>
+    </row>
+    <row r="560" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F560" s="21"/>
-    </row>
-    <row r="561" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E561" s="21"/>
+      <c r="G560" s="21"/>
+    </row>
+    <row r="561" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F561" s="21"/>
-    </row>
-    <row r="562" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E562" s="21"/>
+      <c r="G561" s="21"/>
+    </row>
+    <row r="562" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F562" s="21"/>
-    </row>
-    <row r="563" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E563" s="21"/>
+      <c r="G562" s="21"/>
+    </row>
+    <row r="563" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F563" s="21"/>
-    </row>
-    <row r="564" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E564" s="21"/>
+      <c r="G563" s="21"/>
+    </row>
+    <row r="564" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F564" s="21"/>
-    </row>
-    <row r="565" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E565" s="21"/>
+      <c r="G564" s="21"/>
+    </row>
+    <row r="565" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F565" s="21"/>
-    </row>
-    <row r="566" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E566" s="21"/>
+      <c r="G565" s="21"/>
+    </row>
+    <row r="566" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F566" s="21"/>
-    </row>
-    <row r="567" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E567" s="21"/>
+      <c r="G566" s="21"/>
+    </row>
+    <row r="567" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F567" s="21"/>
-    </row>
-    <row r="568" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E568" s="21"/>
+      <c r="G567" s="21"/>
+    </row>
+    <row r="568" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F568" s="21"/>
-    </row>
-    <row r="569" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E569" s="21"/>
+      <c r="G568" s="21"/>
+    </row>
+    <row r="569" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F569" s="21"/>
-    </row>
-    <row r="570" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E570" s="21"/>
+      <c r="G569" s="21"/>
+    </row>
+    <row r="570" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F570" s="21"/>
-    </row>
-    <row r="571" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E571" s="21"/>
+      <c r="G570" s="21"/>
+    </row>
+    <row r="571" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F571" s="21"/>
-    </row>
-    <row r="572" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E572" s="21"/>
+      <c r="G571" s="21"/>
+    </row>
+    <row r="572" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F572" s="21"/>
-    </row>
-    <row r="573" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E573" s="21"/>
+      <c r="G572" s="21"/>
+    </row>
+    <row r="573" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F573" s="21"/>
-    </row>
-    <row r="574" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E574" s="21"/>
+      <c r="G573" s="21"/>
+    </row>
+    <row r="574" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F574" s="21"/>
-    </row>
-    <row r="575" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E575" s="21"/>
+      <c r="G574" s="21"/>
+    </row>
+    <row r="575" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F575" s="21"/>
-    </row>
-    <row r="576" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E576" s="21"/>
+      <c r="G575" s="21"/>
+    </row>
+    <row r="576" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F576" s="21"/>
-    </row>
-    <row r="577" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E577" s="21"/>
+      <c r="G576" s="21"/>
+    </row>
+    <row r="577" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F577" s="21"/>
-    </row>
-    <row r="578" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E578" s="21"/>
+      <c r="G577" s="21"/>
+    </row>
+    <row r="578" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F578" s="21"/>
-    </row>
-    <row r="579" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E579" s="21"/>
+      <c r="G578" s="21"/>
+    </row>
+    <row r="579" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F579" s="21"/>
-    </row>
-    <row r="580" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E580" s="21"/>
+      <c r="G579" s="21"/>
+    </row>
+    <row r="580" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F580" s="21"/>
-    </row>
-    <row r="581" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E581" s="21"/>
+      <c r="G580" s="21"/>
+    </row>
+    <row r="581" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F581" s="21"/>
-    </row>
-    <row r="582" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E582" s="21"/>
+      <c r="G581" s="21"/>
+    </row>
+    <row r="582" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F582" s="21"/>
-    </row>
-    <row r="583" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E583" s="21"/>
+      <c r="G582" s="21"/>
+    </row>
+    <row r="583" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F583" s="21"/>
-    </row>
-    <row r="584" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E584" s="21"/>
+      <c r="G583" s="21"/>
+    </row>
+    <row r="584" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F584" s="21"/>
-    </row>
-    <row r="585" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E585" s="21"/>
+      <c r="G584" s="21"/>
+    </row>
+    <row r="585" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F585" s="21"/>
-    </row>
-    <row r="586" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E586" s="21"/>
+      <c r="G585" s="21"/>
+    </row>
+    <row r="586" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F586" s="21"/>
-    </row>
-    <row r="587" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E587" s="21"/>
+      <c r="G586" s="21"/>
+    </row>
+    <row r="587" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F587" s="21"/>
-    </row>
-    <row r="588" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E588" s="21"/>
+      <c r="G587" s="21"/>
+    </row>
+    <row r="588" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F588" s="21"/>
-    </row>
-    <row r="589" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E589" s="21"/>
+      <c r="G588" s="21"/>
+    </row>
+    <row r="589" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F589" s="21"/>
-    </row>
-    <row r="590" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E590" s="21"/>
+      <c r="G589" s="21"/>
+    </row>
+    <row r="590" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F590" s="21"/>
-    </row>
-    <row r="591" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E591" s="21"/>
+      <c r="G590" s="21"/>
+    </row>
+    <row r="591" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F591" s="21"/>
-    </row>
-    <row r="592" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E592" s="21"/>
+      <c r="G591" s="21"/>
+    </row>
+    <row r="592" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F592" s="21"/>
-    </row>
-    <row r="593" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E593" s="21"/>
+      <c r="G592" s="21"/>
+    </row>
+    <row r="593" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F593" s="21"/>
-    </row>
-    <row r="594" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E594" s="21"/>
+      <c r="G593" s="21"/>
+    </row>
+    <row r="594" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F594" s="21"/>
-    </row>
-    <row r="595" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E595" s="21"/>
+      <c r="G594" s="21"/>
+    </row>
+    <row r="595" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F595" s="21"/>
-    </row>
-    <row r="596" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E596" s="21"/>
+      <c r="G595" s="21"/>
+    </row>
+    <row r="596" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F596" s="21"/>
-    </row>
-    <row r="597" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E597" s="21"/>
+      <c r="G596" s="21"/>
+    </row>
+    <row r="597" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F597" s="21"/>
-    </row>
-    <row r="598" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E598" s="21"/>
+      <c r="G597" s="21"/>
+    </row>
+    <row r="598" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F598" s="21"/>
-    </row>
-    <row r="599" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E599" s="21"/>
+      <c r="G598" s="21"/>
+    </row>
+    <row r="599" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F599" s="21"/>
-    </row>
-    <row r="600" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E600" s="21"/>
+      <c r="G599" s="21"/>
+    </row>
+    <row r="600" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F600" s="21"/>
-    </row>
-    <row r="601" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E601" s="21"/>
+      <c r="G600" s="21"/>
+    </row>
+    <row r="601" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F601" s="21"/>
-    </row>
-    <row r="602" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E602" s="21"/>
+      <c r="G601" s="21"/>
+    </row>
+    <row r="602" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F602" s="21"/>
-    </row>
-    <row r="603" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E603" s="21"/>
+      <c r="G602" s="21"/>
+    </row>
+    <row r="603" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F603" s="21"/>
-    </row>
-    <row r="604" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E604" s="21"/>
+      <c r="G603" s="21"/>
+    </row>
+    <row r="604" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F604" s="21"/>
-    </row>
-    <row r="605" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E605" s="21"/>
+      <c r="G604" s="21"/>
+    </row>
+    <row r="605" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F605" s="21"/>
-    </row>
-    <row r="606" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E606" s="21"/>
+      <c r="G605" s="21"/>
+    </row>
+    <row r="606" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F606" s="21"/>
-    </row>
-    <row r="607" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E607" s="21"/>
+      <c r="G606" s="21"/>
+    </row>
+    <row r="607" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F607" s="21"/>
-    </row>
-    <row r="608" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E608" s="21"/>
+      <c r="G607" s="21"/>
+    </row>
+    <row r="608" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F608" s="21"/>
-    </row>
-    <row r="609" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E609" s="21"/>
+      <c r="G608" s="21"/>
+    </row>
+    <row r="609" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F609" s="21"/>
-    </row>
-    <row r="610" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E610" s="21"/>
+      <c r="G609" s="21"/>
+    </row>
+    <row r="610" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F610" s="21"/>
-    </row>
-    <row r="611" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E611" s="21"/>
+      <c r="G610" s="21"/>
+    </row>
+    <row r="611" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F611" s="21"/>
-    </row>
-    <row r="612" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E612" s="21"/>
+      <c r="G611" s="21"/>
+    </row>
+    <row r="612" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F612" s="21"/>
-    </row>
-    <row r="613" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E613" s="21"/>
+      <c r="G612" s="21"/>
+    </row>
+    <row r="613" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F613" s="21"/>
-    </row>
-    <row r="614" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E614" s="21"/>
+      <c r="G613" s="21"/>
+    </row>
+    <row r="614" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F614" s="21"/>
-    </row>
-    <row r="615" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E615" s="21"/>
+      <c r="G614" s="21"/>
+    </row>
+    <row r="615" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F615" s="21"/>
-    </row>
-    <row r="616" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E616" s="21"/>
+      <c r="G615" s="21"/>
+    </row>
+    <row r="616" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F616" s="21"/>
-    </row>
-    <row r="617" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E617" s="21"/>
+      <c r="G616" s="21"/>
+    </row>
+    <row r="617" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F617" s="21"/>
-    </row>
-    <row r="618" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E618" s="21"/>
+      <c r="G617" s="21"/>
+    </row>
+    <row r="618" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F618" s="21"/>
-    </row>
-    <row r="619" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E619" s="21"/>
+      <c r="G618" s="21"/>
+    </row>
+    <row r="619" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F619" s="21"/>
-    </row>
-    <row r="620" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E620" s="21"/>
+      <c r="G619" s="21"/>
+    </row>
+    <row r="620" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F620" s="21"/>
-    </row>
-    <row r="621" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E621" s="21"/>
+      <c r="G620" s="21"/>
+    </row>
+    <row r="621" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F621" s="21"/>
-    </row>
-    <row r="622" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E622" s="21"/>
+      <c r="G621" s="21"/>
+    </row>
+    <row r="622" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F622" s="21"/>
-    </row>
-    <row r="623" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E623" s="21"/>
+      <c r="G622" s="21"/>
+    </row>
+    <row r="623" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F623" s="21"/>
-    </row>
-    <row r="624" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E624" s="21"/>
+      <c r="G623" s="21"/>
+    </row>
+    <row r="624" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F624" s="21"/>
-    </row>
-    <row r="625" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E625" s="21"/>
+      <c r="G624" s="21"/>
+    </row>
+    <row r="625" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F625" s="21"/>
-    </row>
-    <row r="626" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E626" s="21"/>
+      <c r="G625" s="21"/>
+    </row>
+    <row r="626" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F626" s="21"/>
-    </row>
-    <row r="627" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E627" s="21"/>
+      <c r="G626" s="21"/>
+    </row>
+    <row r="627" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F627" s="21"/>
-    </row>
-    <row r="628" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E628" s="21"/>
+      <c r="G627" s="21"/>
+    </row>
+    <row r="628" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F628" s="21"/>
-    </row>
-    <row r="629" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E629" s="21"/>
+      <c r="G628" s="21"/>
+    </row>
+    <row r="629" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F629" s="21"/>
-    </row>
-    <row r="630" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E630" s="21"/>
+      <c r="G629" s="21"/>
+    </row>
+    <row r="630" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F630" s="21"/>
-    </row>
-    <row r="631" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E631" s="21"/>
+      <c r="G630" s="21"/>
+    </row>
+    <row r="631" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F631" s="21"/>
-    </row>
-    <row r="632" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E632" s="21"/>
+      <c r="G631" s="21"/>
+    </row>
+    <row r="632" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F632" s="21"/>
-    </row>
-    <row r="633" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E633" s="21"/>
+      <c r="G632" s="21"/>
+    </row>
+    <row r="633" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F633" s="21"/>
-    </row>
-    <row r="634" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E634" s="21"/>
+      <c r="G633" s="21"/>
+    </row>
+    <row r="634" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F634" s="21"/>
-    </row>
-    <row r="635" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E635" s="21"/>
+      <c r="G634" s="21"/>
+    </row>
+    <row r="635" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F635" s="21"/>
-    </row>
-    <row r="636" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E636" s="21"/>
+      <c r="G635" s="21"/>
+    </row>
+    <row r="636" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F636" s="21"/>
-    </row>
-    <row r="637" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E637" s="21"/>
+      <c r="G636" s="21"/>
+    </row>
+    <row r="637" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F637" s="21"/>
-    </row>
-    <row r="638" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E638" s="21"/>
+      <c r="G637" s="21"/>
+    </row>
+    <row r="638" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F638" s="21"/>
-    </row>
-    <row r="639" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E639" s="21"/>
+      <c r="G638" s="21"/>
+    </row>
+    <row r="639" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F639" s="21"/>
-    </row>
-    <row r="640" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E640" s="21"/>
+      <c r="G639" s="21"/>
+    </row>
+    <row r="640" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F640" s="21"/>
-    </row>
-    <row r="641" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E641" s="21"/>
+      <c r="G640" s="21"/>
+    </row>
+    <row r="641" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F641" s="21"/>
-    </row>
-    <row r="642" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E642" s="21"/>
+      <c r="G641" s="21"/>
+    </row>
+    <row r="642" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F642" s="21"/>
-    </row>
-    <row r="643" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E643" s="21"/>
+      <c r="G642" s="21"/>
+    </row>
+    <row r="643" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F643" s="21"/>
-    </row>
-    <row r="644" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E644" s="21"/>
+      <c r="G643" s="21"/>
+    </row>
+    <row r="644" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F644" s="21"/>
-    </row>
-    <row r="645" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E645" s="21"/>
+      <c r="G644" s="21"/>
+    </row>
+    <row r="645" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F645" s="21"/>
-    </row>
-    <row r="646" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E646" s="21"/>
+      <c r="G645" s="21"/>
+    </row>
+    <row r="646" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F646" s="21"/>
-    </row>
-    <row r="647" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E647" s="21"/>
+      <c r="G646" s="21"/>
+    </row>
+    <row r="647" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F647" s="21"/>
-    </row>
-    <row r="648" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E648" s="21"/>
+      <c r="G647" s="21"/>
+    </row>
+    <row r="648" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F648" s="21"/>
-    </row>
-    <row r="649" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E649" s="21"/>
+      <c r="G648" s="21"/>
+    </row>
+    <row r="649" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F649" s="21"/>
-    </row>
-    <row r="650" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E650" s="21"/>
+      <c r="G649" s="21"/>
+    </row>
+    <row r="650" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F650" s="21"/>
-    </row>
-    <row r="651" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E651" s="21"/>
+      <c r="G650" s="21"/>
+    </row>
+    <row r="651" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F651" s="21"/>
-    </row>
-    <row r="652" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E652" s="21"/>
+      <c r="G651" s="21"/>
+    </row>
+    <row r="652" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F652" s="21"/>
-    </row>
-    <row r="653" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E653" s="21"/>
+      <c r="G652" s="21"/>
+    </row>
+    <row r="653" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F653" s="21"/>
-    </row>
-    <row r="654" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E654" s="21"/>
+      <c r="G653" s="21"/>
+    </row>
+    <row r="654" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F654" s="21"/>
-    </row>
-    <row r="655" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E655" s="21"/>
+      <c r="G654" s="21"/>
+    </row>
+    <row r="655" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F655" s="21"/>
-    </row>
-    <row r="656" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E656" s="21"/>
+      <c r="G655" s="21"/>
+    </row>
+    <row r="656" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F656" s="21"/>
-    </row>
-    <row r="657" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E657" s="21"/>
+      <c r="G656" s="21"/>
+    </row>
+    <row r="657" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F657" s="21"/>
-    </row>
-    <row r="658" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E658" s="21"/>
+      <c r="G657" s="21"/>
+    </row>
+    <row r="658" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F658" s="21"/>
-    </row>
-    <row r="659" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E659" s="21"/>
+      <c r="G658" s="21"/>
+    </row>
+    <row r="659" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F659" s="21"/>
-    </row>
-    <row r="660" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E660" s="21"/>
+      <c r="G659" s="21"/>
+    </row>
+    <row r="660" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F660" s="21"/>
-    </row>
-    <row r="667" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E667" s="21"/>
+      <c r="G660" s="21"/>
+    </row>
+    <row r="667" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F667" s="21"/>
-    </row>
-    <row r="668" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E668" s="21"/>
+      <c r="G667" s="21"/>
+    </row>
+    <row r="668" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F668" s="21"/>
-    </row>
-    <row r="669" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E669" s="21"/>
+      <c r="G668" s="21"/>
+    </row>
+    <row r="669" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F669" s="21"/>
-    </row>
-    <row r="670" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E670" s="21"/>
+      <c r="G669" s="21"/>
+    </row>
+    <row r="670" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F670" s="21"/>
-    </row>
-    <row r="671" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E671" s="21"/>
+      <c r="G670" s="21"/>
+    </row>
+    <row r="671" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F671" s="21"/>
-    </row>
-    <row r="672" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E672" s="21"/>
+      <c r="G671" s="21"/>
+    </row>
+    <row r="672" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F672" s="21"/>
-    </row>
-    <row r="673" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E673" s="21"/>
+      <c r="G672" s="21"/>
+    </row>
+    <row r="673" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F673" s="21"/>
-    </row>
-    <row r="674" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E674" s="21"/>
+      <c r="G673" s="21"/>
+    </row>
+    <row r="674" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F674" s="21"/>
-    </row>
-    <row r="675" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E675" s="21"/>
+      <c r="G674" s="21"/>
+    </row>
+    <row r="675" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F675" s="21"/>
-    </row>
-    <row r="676" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E676" s="21"/>
+      <c r="G675" s="21"/>
+    </row>
+    <row r="676" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F676" s="21"/>
-    </row>
-    <row r="677" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E677" s="21"/>
+      <c r="G676" s="21"/>
+    </row>
+    <row r="677" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F677" s="21"/>
-    </row>
-    <row r="678" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E678" s="21"/>
+      <c r="G677" s="21"/>
+    </row>
+    <row r="678" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F678" s="21"/>
-    </row>
-    <row r="679" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E679" s="21"/>
+      <c r="G678" s="21"/>
+    </row>
+    <row r="679" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F679" s="21"/>
+      <c r="G679" s="21"/>
     </row>
   </sheetData>
   <dataConsolidate/>
-  <dataValidations count="2">
-    <dataValidation type="date" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Session end date must be later than session start date." sqref="E71:E362 E369:E660 E667:E679 E4:E64">
-      <formula1>D4</formula1>
+  <dataValidations count="3">
+    <dataValidation type="date" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Session end date must be later than session start date." sqref="F71:F362 F369:F660 F667:F679 F4:F64">
+      <formula1>E4</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Session end date must be later than session start date." sqref="F1:G1"/>
+    <dataValidation errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Session end date must be later than session start date." sqref="G1:H1"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="You need to select a value from the drop down list." sqref="D1:D1048576"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6087,11 +6122,11 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$1:$A$48</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:G1048576</xm:sqref>
+          <xm:sqref>G2:H1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Sheet1!$G$20:$G$22</xm:f>
+            <xm:f>Sheet1!$G$20:$G$23</xm:f>
           </x14:formula1>
           <xm:sqref>A2:A1048576</xm:sqref>
         </x14:dataValidation>
@@ -6105,8 +6140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G207"/>
   <sheetViews>
-    <sheetView topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6392,7 +6427,7 @@
         <v>83</v>
       </c>
       <c r="G22" s="34" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -6401,6 +6436,9 @@
       </c>
       <c r="C23" s="6" t="s">
         <v>84</v>
+      </c>
+      <c r="G23" s="34" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Merging Sprint-5-RC into master.
</commit_message>
<xml_diff>
--- a/lcms.web/src/main/webapp/theme/samplefile/Classroom batch import template.xlsx
+++ b/lcms.web/src/main/webapp/theme/samplefile/Classroom batch import template.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="389">
   <si>
     <t>(GMT -12:00) Dateline (Eniwetok)</t>
   </si>
@@ -1990,6 +1990,33 @@
         <scheme val="minor"/>
       </rPr>
       <t>john.doe@360training.com</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Session Key</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Session1</t>
     </r>
   </si>
 </sst>
@@ -2162,7 +2189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2273,6 +2300,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2596,27 +2626,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="1"/>
-    <col min="2" max="3" width="26.42578125" style="32" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="1" max="3" width="26.42578125" style="26" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" style="26" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="26" customWidth="1"/>
     <col min="6" max="6" width="32.28515625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="87" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="42" t="s">
         <v>380</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="42" t="s">
         <v>383</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="42" t="s">
         <v>381</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="42" t="s">
         <v>382</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="42" t="s">
         <v>384</v>
       </c>
       <c r="F1" s="41" t="s">
@@ -3370,7 +3399,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I679"/>
+  <dimension ref="A1:J679"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -3381,15 +3410,16 @@
   <cols>
     <col min="1" max="1" width="28.28515625" style="11" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" style="11" customWidth="1"/>
-    <col min="3" max="3" width="51" style="11" customWidth="1"/>
-    <col min="4" max="4" width="29.42578125" style="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.42578125" style="25" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" style="25" customWidth="1"/>
-    <col min="7" max="7" width="18" style="11" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="11"/>
+    <col min="3" max="3" width="41.140625" style="11" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" style="11" customWidth="1"/>
+    <col min="5" max="5" width="29.42578125" style="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.42578125" style="25" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" style="25" customWidth="1"/>
+    <col min="8" max="8" width="18" style="11" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="39" t="s">
         <v>378</v>
       </c>
@@ -3400,2671 +3430,2676 @@
         <v>307</v>
       </c>
       <c r="D1" s="24" t="s">
+        <v>388</v>
+      </c>
+      <c r="E1" s="24" t="s">
         <v>315</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="F1" s="24" t="s">
         <v>314</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C2" s="2"/>
-      <c r="D2" s="21"/>
+      <c r="D2" s="37"/>
       <c r="E2" s="21"/>
       <c r="F2" s="21"/>
-      <c r="G2" s="2"/>
+      <c r="G2" s="21"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F3" s="21"/>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D4" s="21"/>
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G3" s="21"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E4" s="21"/>
       <c r="F4" s="21"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E5" s="21"/>
+      <c r="G4" s="21"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F5" s="21"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E6" s="21"/>
+      <c r="G5" s="21"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F6" s="21"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E7" s="21"/>
+      <c r="G6" s="21"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F7" s="21"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E8" s="21"/>
+      <c r="G7" s="21"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F8" s="21"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E9" s="21"/>
+      <c r="G8" s="21"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F9" s="21"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E10" s="21"/>
+      <c r="G9" s="21"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F10" s="21"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E11" s="21"/>
+      <c r="G10" s="21"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F11" s="21"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E12" s="21"/>
+      <c r="G11" s="21"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F12" s="21"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E13" s="21"/>
+      <c r="G12" s="21"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F13" s="21"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E14" s="21"/>
+      <c r="G13" s="21"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F14" s="21"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E15" s="21"/>
+      <c r="G14" s="21"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F15" s="21"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E16" s="21"/>
+      <c r="G15" s="21"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F16" s="21"/>
-    </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E17" s="21"/>
+      <c r="G16" s="21"/>
+    </row>
+    <row r="17" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F17" s="21"/>
-    </row>
-    <row r="18" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E18" s="21"/>
+      <c r="G17" s="21"/>
+    </row>
+    <row r="18" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F18" s="21"/>
-    </row>
-    <row r="19" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E19" s="21"/>
+      <c r="G18" s="21"/>
+    </row>
+    <row r="19" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F19" s="21"/>
-    </row>
-    <row r="20" spans="5:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E20" s="21"/>
+      <c r="G19" s="21"/>
+    </row>
+    <row r="20" spans="6:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F20" s="21"/>
-    </row>
-    <row r="21" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E21" s="21"/>
+      <c r="G20" s="21"/>
+    </row>
+    <row r="21" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F21" s="21"/>
-    </row>
-    <row r="22" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E22" s="21"/>
+      <c r="G21" s="21"/>
+    </row>
+    <row r="22" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F22" s="21"/>
-    </row>
-    <row r="23" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E23" s="21"/>
+      <c r="G22" s="21"/>
+    </row>
+    <row r="23" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F23" s="21"/>
-    </row>
-    <row r="24" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E24" s="21"/>
+      <c r="G23" s="21"/>
+    </row>
+    <row r="24" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F24" s="21"/>
-    </row>
-    <row r="25" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E25" s="21"/>
+      <c r="G24" s="21"/>
+    </row>
+    <row r="25" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F25" s="21"/>
-    </row>
-    <row r="26" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E26" s="21"/>
+      <c r="G25" s="21"/>
+    </row>
+    <row r="26" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F26" s="21"/>
-    </row>
-    <row r="27" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E27" s="21"/>
+      <c r="G26" s="21"/>
+    </row>
+    <row r="27" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F27" s="21"/>
-    </row>
-    <row r="28" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E28" s="21"/>
+      <c r="G27" s="21"/>
+    </row>
+    <row r="28" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F28" s="21"/>
-    </row>
-    <row r="29" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E29" s="21"/>
+      <c r="G28" s="21"/>
+    </row>
+    <row r="29" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F29" s="21"/>
-    </row>
-    <row r="30" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E30" s="21"/>
+      <c r="G29" s="21"/>
+    </row>
+    <row r="30" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F30" s="21"/>
-    </row>
-    <row r="31" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E31" s="21"/>
+      <c r="G30" s="21"/>
+    </row>
+    <row r="31" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F31" s="21"/>
-    </row>
-    <row r="32" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E32" s="21"/>
+      <c r="G31" s="21"/>
+    </row>
+    <row r="32" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F32" s="21"/>
-    </row>
-    <row r="33" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E33" s="21"/>
+      <c r="G32" s="21"/>
+    </row>
+    <row r="33" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F33" s="21"/>
-    </row>
-    <row r="34" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E34" s="21"/>
+      <c r="G33" s="21"/>
+    </row>
+    <row r="34" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F34" s="21"/>
-    </row>
-    <row r="35" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E35" s="21"/>
+      <c r="G34" s="21"/>
+    </row>
+    <row r="35" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F35" s="21"/>
-    </row>
-    <row r="36" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E36" s="21"/>
+      <c r="G35" s="21"/>
+    </row>
+    <row r="36" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F36" s="21"/>
-    </row>
-    <row r="37" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E37" s="21"/>
+      <c r="G36" s="21"/>
+    </row>
+    <row r="37" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F37" s="21"/>
-    </row>
-    <row r="38" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E38" s="21"/>
+      <c r="G37" s="21"/>
+    </row>
+    <row r="38" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F38" s="21"/>
-    </row>
-    <row r="39" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E39" s="21"/>
+      <c r="G38" s="21"/>
+    </row>
+    <row r="39" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F39" s="21"/>
-    </row>
-    <row r="40" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E40" s="21"/>
+      <c r="G39" s="21"/>
+    </row>
+    <row r="40" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F40" s="21"/>
-    </row>
-    <row r="41" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E41" s="21"/>
+      <c r="G40" s="21"/>
+    </row>
+    <row r="41" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F41" s="21"/>
-    </row>
-    <row r="42" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E42" s="21"/>
+      <c r="G41" s="21"/>
+    </row>
+    <row r="42" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F42" s="21"/>
-    </row>
-    <row r="43" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E43" s="21"/>
+      <c r="G42" s="21"/>
+    </row>
+    <row r="43" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F43" s="21"/>
-    </row>
-    <row r="44" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E44" s="21"/>
+      <c r="G43" s="21"/>
+    </row>
+    <row r="44" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F44" s="21"/>
-    </row>
-    <row r="45" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E45" s="21"/>
+      <c r="G44" s="21"/>
+    </row>
+    <row r="45" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F45" s="21"/>
-    </row>
-    <row r="46" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E46" s="21"/>
+      <c r="G45" s="21"/>
+    </row>
+    <row r="46" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F46" s="21"/>
-    </row>
-    <row r="47" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E47" s="21"/>
+      <c r="G46" s="21"/>
+    </row>
+    <row r="47" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F47" s="21"/>
-    </row>
-    <row r="48" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E48" s="21"/>
+      <c r="G47" s="21"/>
+    </row>
+    <row r="48" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F48" s="21"/>
-    </row>
-    <row r="49" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E49" s="21"/>
+      <c r="G48" s="21"/>
+    </row>
+    <row r="49" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F49" s="21"/>
-    </row>
-    <row r="50" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E50" s="21"/>
+      <c r="G49" s="21"/>
+    </row>
+    <row r="50" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F50" s="21"/>
-    </row>
-    <row r="51" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E51" s="21"/>
+      <c r="G50" s="21"/>
+    </row>
+    <row r="51" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F51" s="21"/>
-    </row>
-    <row r="52" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E52" s="21"/>
+      <c r="G51" s="21"/>
+    </row>
+    <row r="52" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F52" s="21"/>
-    </row>
-    <row r="53" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E53" s="21"/>
+      <c r="G52" s="21"/>
+    </row>
+    <row r="53" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F53" s="21"/>
-    </row>
-    <row r="54" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E54" s="21"/>
+      <c r="G53" s="21"/>
+    </row>
+    <row r="54" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F54" s="21"/>
-    </row>
-    <row r="55" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E55" s="21"/>
+      <c r="G54" s="21"/>
+    </row>
+    <row r="55" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F55" s="21"/>
-    </row>
-    <row r="56" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E56" s="21"/>
+      <c r="G55" s="21"/>
+    </row>
+    <row r="56" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F56" s="21"/>
-    </row>
-    <row r="57" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E57" s="21"/>
+      <c r="G56" s="21"/>
+    </row>
+    <row r="57" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F57" s="21"/>
-    </row>
-    <row r="58" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E58" s="21"/>
+      <c r="G57" s="21"/>
+    </row>
+    <row r="58" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F58" s="21"/>
-    </row>
-    <row r="59" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E59" s="21"/>
+      <c r="G58" s="21"/>
+    </row>
+    <row r="59" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F59" s="21"/>
-    </row>
-    <row r="60" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E60" s="21"/>
+      <c r="G59" s="21"/>
+    </row>
+    <row r="60" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F60" s="21"/>
-    </row>
-    <row r="61" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E61" s="21"/>
+      <c r="G60" s="21"/>
+    </row>
+    <row r="61" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F61" s="21"/>
-    </row>
-    <row r="62" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E62" s="21"/>
+      <c r="G61" s="21"/>
+    </row>
+    <row r="62" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F62" s="21"/>
-    </row>
-    <row r="63" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E63" s="21"/>
+      <c r="G62" s="21"/>
+    </row>
+    <row r="63" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F63" s="21"/>
-    </row>
-    <row r="64" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E64" s="21"/>
+      <c r="G63" s="21"/>
+    </row>
+    <row r="64" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F64" s="21"/>
-    </row>
-    <row r="71" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E71" s="21"/>
+      <c r="G64" s="21"/>
+    </row>
+    <row r="71" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F71" s="21"/>
-    </row>
-    <row r="72" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E72" s="21"/>
+      <c r="G71" s="21"/>
+    </row>
+    <row r="72" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F72" s="21"/>
-    </row>
-    <row r="73" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E73" s="21"/>
+      <c r="G72" s="21"/>
+    </row>
+    <row r="73" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F73" s="21"/>
-    </row>
-    <row r="74" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E74" s="21"/>
+      <c r="G73" s="21"/>
+    </row>
+    <row r="74" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F74" s="21"/>
-    </row>
-    <row r="75" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E75" s="21"/>
+      <c r="G74" s="21"/>
+    </row>
+    <row r="75" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F75" s="21"/>
-    </row>
-    <row r="76" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E76" s="21"/>
+      <c r="G75" s="21"/>
+    </row>
+    <row r="76" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F76" s="21"/>
-    </row>
-    <row r="77" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E77" s="21"/>
+      <c r="G76" s="21"/>
+    </row>
+    <row r="77" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F77" s="21"/>
-    </row>
-    <row r="78" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E78" s="21"/>
+      <c r="G77" s="21"/>
+    </row>
+    <row r="78" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F78" s="21"/>
-    </row>
-    <row r="79" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E79" s="21"/>
+      <c r="G78" s="21"/>
+    </row>
+    <row r="79" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F79" s="21"/>
-    </row>
-    <row r="80" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E80" s="21"/>
+      <c r="G79" s="21"/>
+    </row>
+    <row r="80" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F80" s="21"/>
-    </row>
-    <row r="81" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E81" s="21"/>
+      <c r="G80" s="21"/>
+    </row>
+    <row r="81" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F81" s="21"/>
-    </row>
-    <row r="82" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E82" s="21"/>
+      <c r="G81" s="21"/>
+    </row>
+    <row r="82" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F82" s="21"/>
-    </row>
-    <row r="83" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E83" s="21"/>
+      <c r="G82" s="21"/>
+    </row>
+    <row r="83" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F83" s="21"/>
-    </row>
-    <row r="84" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E84" s="21"/>
+      <c r="G83" s="21"/>
+    </row>
+    <row r="84" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F84" s="21"/>
-    </row>
-    <row r="85" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E85" s="21"/>
+      <c r="G84" s="21"/>
+    </row>
+    <row r="85" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F85" s="21"/>
-    </row>
-    <row r="86" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E86" s="21"/>
+      <c r="G85" s="21"/>
+    </row>
+    <row r="86" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F86" s="21"/>
-    </row>
-    <row r="87" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E87" s="21"/>
+      <c r="G86" s="21"/>
+    </row>
+    <row r="87" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F87" s="21"/>
-    </row>
-    <row r="88" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E88" s="21"/>
+      <c r="G87" s="21"/>
+    </row>
+    <row r="88" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F88" s="21"/>
-    </row>
-    <row r="89" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E89" s="21"/>
+      <c r="G88" s="21"/>
+    </row>
+    <row r="89" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F89" s="21"/>
-    </row>
-    <row r="90" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E90" s="21"/>
+      <c r="G89" s="21"/>
+    </row>
+    <row r="90" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F90" s="21"/>
-    </row>
-    <row r="91" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E91" s="21"/>
+      <c r="G90" s="21"/>
+    </row>
+    <row r="91" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F91" s="21"/>
-    </row>
-    <row r="92" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E92" s="21"/>
+      <c r="G91" s="21"/>
+    </row>
+    <row r="92" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F92" s="21"/>
-    </row>
-    <row r="93" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E93" s="21"/>
+      <c r="G92" s="21"/>
+    </row>
+    <row r="93" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F93" s="21"/>
-    </row>
-    <row r="94" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E94" s="21"/>
+      <c r="G93" s="21"/>
+    </row>
+    <row r="94" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F94" s="21"/>
-    </row>
-    <row r="95" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E95" s="21"/>
+      <c r="G94" s="21"/>
+    </row>
+    <row r="95" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F95" s="21"/>
-    </row>
-    <row r="96" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E96" s="21"/>
+      <c r="G95" s="21"/>
+    </row>
+    <row r="96" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F96" s="21"/>
-    </row>
-    <row r="97" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E97" s="21"/>
+      <c r="G96" s="21"/>
+    </row>
+    <row r="97" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F97" s="21"/>
-    </row>
-    <row r="98" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E98" s="21"/>
+      <c r="G97" s="21"/>
+    </row>
+    <row r="98" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F98" s="21"/>
-    </row>
-    <row r="99" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E99" s="21"/>
+      <c r="G98" s="21"/>
+    </row>
+    <row r="99" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F99" s="21"/>
-    </row>
-    <row r="100" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E100" s="21"/>
+      <c r="G99" s="21"/>
+    </row>
+    <row r="100" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F100" s="21"/>
-    </row>
-    <row r="101" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E101" s="21"/>
+      <c r="G100" s="21"/>
+    </row>
+    <row r="101" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F101" s="21"/>
-    </row>
-    <row r="102" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E102" s="21"/>
+      <c r="G101" s="21"/>
+    </row>
+    <row r="102" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F102" s="21"/>
-    </row>
-    <row r="103" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E103" s="21"/>
+      <c r="G102" s="21"/>
+    </row>
+    <row r="103" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F103" s="21"/>
-    </row>
-    <row r="104" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E104" s="21"/>
+      <c r="G103" s="21"/>
+    </row>
+    <row r="104" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F104" s="21"/>
-    </row>
-    <row r="105" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E105" s="21"/>
+      <c r="G104" s="21"/>
+    </row>
+    <row r="105" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F105" s="21"/>
-    </row>
-    <row r="106" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E106" s="21"/>
+      <c r="G105" s="21"/>
+    </row>
+    <row r="106" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F106" s="21"/>
-    </row>
-    <row r="107" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E107" s="21"/>
+      <c r="G106" s="21"/>
+    </row>
+    <row r="107" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F107" s="21"/>
-    </row>
-    <row r="108" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E108" s="21"/>
+      <c r="G107" s="21"/>
+    </row>
+    <row r="108" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F108" s="21"/>
-    </row>
-    <row r="109" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E109" s="21"/>
+      <c r="G108" s="21"/>
+    </row>
+    <row r="109" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F109" s="21"/>
-    </row>
-    <row r="110" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E110" s="21"/>
+      <c r="G109" s="21"/>
+    </row>
+    <row r="110" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F110" s="21"/>
-    </row>
-    <row r="111" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E111" s="21"/>
+      <c r="G110" s="21"/>
+    </row>
+    <row r="111" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F111" s="21"/>
-    </row>
-    <row r="112" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E112" s="21"/>
+      <c r="G111" s="21"/>
+    </row>
+    <row r="112" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F112" s="21"/>
-    </row>
-    <row r="113" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E113" s="21"/>
+      <c r="G112" s="21"/>
+    </row>
+    <row r="113" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F113" s="21"/>
-    </row>
-    <row r="114" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E114" s="21"/>
+      <c r="G113" s="21"/>
+    </row>
+    <row r="114" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F114" s="21"/>
-    </row>
-    <row r="115" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E115" s="21"/>
+      <c r="G114" s="21"/>
+    </row>
+    <row r="115" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F115" s="21"/>
-    </row>
-    <row r="116" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E116" s="21"/>
+      <c r="G115" s="21"/>
+    </row>
+    <row r="116" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F116" s="21"/>
-    </row>
-    <row r="117" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E117" s="21"/>
+      <c r="G116" s="21"/>
+    </row>
+    <row r="117" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F117" s="21"/>
-    </row>
-    <row r="118" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E118" s="21"/>
+      <c r="G117" s="21"/>
+    </row>
+    <row r="118" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F118" s="21"/>
-    </row>
-    <row r="119" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E119" s="21"/>
+      <c r="G118" s="21"/>
+    </row>
+    <row r="119" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F119" s="21"/>
-    </row>
-    <row r="120" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E120" s="21"/>
+      <c r="G119" s="21"/>
+    </row>
+    <row r="120" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F120" s="21"/>
-    </row>
-    <row r="121" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E121" s="21"/>
+      <c r="G120" s="21"/>
+    </row>
+    <row r="121" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F121" s="21"/>
-    </row>
-    <row r="122" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E122" s="21"/>
+      <c r="G121" s="21"/>
+    </row>
+    <row r="122" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F122" s="21"/>
-    </row>
-    <row r="123" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E123" s="21"/>
+      <c r="G122" s="21"/>
+    </row>
+    <row r="123" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F123" s="21"/>
-    </row>
-    <row r="124" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E124" s="21"/>
+      <c r="G123" s="21"/>
+    </row>
+    <row r="124" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F124" s="21"/>
-    </row>
-    <row r="125" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E125" s="21"/>
+      <c r="G124" s="21"/>
+    </row>
+    <row r="125" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F125" s="21"/>
-    </row>
-    <row r="126" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E126" s="21"/>
+      <c r="G125" s="21"/>
+    </row>
+    <row r="126" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F126" s="21"/>
-    </row>
-    <row r="127" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E127" s="21"/>
+      <c r="G126" s="21"/>
+    </row>
+    <row r="127" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F127" s="21"/>
-    </row>
-    <row r="128" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E128" s="21"/>
+      <c r="G127" s="21"/>
+    </row>
+    <row r="128" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F128" s="21"/>
-    </row>
-    <row r="129" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E129" s="21"/>
+      <c r="G128" s="21"/>
+    </row>
+    <row r="129" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F129" s="21"/>
-    </row>
-    <row r="130" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E130" s="21"/>
+      <c r="G129" s="21"/>
+    </row>
+    <row r="130" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F130" s="21"/>
-    </row>
-    <row r="131" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E131" s="21"/>
+      <c r="G130" s="21"/>
+    </row>
+    <row r="131" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F131" s="21"/>
-    </row>
-    <row r="132" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E132" s="21"/>
+      <c r="G131" s="21"/>
+    </row>
+    <row r="132" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F132" s="21"/>
-    </row>
-    <row r="133" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E133" s="21"/>
+      <c r="G132" s="21"/>
+    </row>
+    <row r="133" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F133" s="21"/>
-    </row>
-    <row r="134" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E134" s="21"/>
+      <c r="G133" s="21"/>
+    </row>
+    <row r="134" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F134" s="21"/>
-    </row>
-    <row r="135" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E135" s="21"/>
+      <c r="G134" s="21"/>
+    </row>
+    <row r="135" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F135" s="21"/>
-    </row>
-    <row r="136" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E136" s="21"/>
+      <c r="G135" s="21"/>
+    </row>
+    <row r="136" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F136" s="21"/>
-    </row>
-    <row r="137" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E137" s="21"/>
+      <c r="G136" s="21"/>
+    </row>
+    <row r="137" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F137" s="21"/>
-    </row>
-    <row r="138" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E138" s="21"/>
+      <c r="G137" s="21"/>
+    </row>
+    <row r="138" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F138" s="21"/>
-    </row>
-    <row r="139" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E139" s="21"/>
+      <c r="G138" s="21"/>
+    </row>
+    <row r="139" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F139" s="21"/>
-    </row>
-    <row r="140" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E140" s="21"/>
+      <c r="G139" s="21"/>
+    </row>
+    <row r="140" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F140" s="21"/>
-    </row>
-    <row r="141" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E141" s="21"/>
+      <c r="G140" s="21"/>
+    </row>
+    <row r="141" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F141" s="21"/>
-    </row>
-    <row r="142" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E142" s="21"/>
+      <c r="G141" s="21"/>
+    </row>
+    <row r="142" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F142" s="21"/>
-    </row>
-    <row r="143" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E143" s="21"/>
+      <c r="G142" s="21"/>
+    </row>
+    <row r="143" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F143" s="21"/>
-    </row>
-    <row r="144" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E144" s="21"/>
+      <c r="G143" s="21"/>
+    </row>
+    <row r="144" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F144" s="21"/>
-    </row>
-    <row r="145" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E145" s="21"/>
+      <c r="G144" s="21"/>
+    </row>
+    <row r="145" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F145" s="21"/>
-    </row>
-    <row r="146" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E146" s="21"/>
+      <c r="G145" s="21"/>
+    </row>
+    <row r="146" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F146" s="21"/>
-    </row>
-    <row r="147" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E147" s="21"/>
+      <c r="G146" s="21"/>
+    </row>
+    <row r="147" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F147" s="21"/>
-    </row>
-    <row r="148" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E148" s="21"/>
+      <c r="G147" s="21"/>
+    </row>
+    <row r="148" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F148" s="21"/>
-    </row>
-    <row r="149" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E149" s="21"/>
+      <c r="G148" s="21"/>
+    </row>
+    <row r="149" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F149" s="21"/>
-    </row>
-    <row r="150" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E150" s="21"/>
+      <c r="G149" s="21"/>
+    </row>
+    <row r="150" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F150" s="21"/>
-    </row>
-    <row r="151" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E151" s="21"/>
+      <c r="G150" s="21"/>
+    </row>
+    <row r="151" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F151" s="21"/>
-    </row>
-    <row r="152" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E152" s="21"/>
+      <c r="G151" s="21"/>
+    </row>
+    <row r="152" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F152" s="21"/>
-    </row>
-    <row r="153" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E153" s="21"/>
+      <c r="G152" s="21"/>
+    </row>
+    <row r="153" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F153" s="21"/>
-    </row>
-    <row r="154" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E154" s="21"/>
+      <c r="G153" s="21"/>
+    </row>
+    <row r="154" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F154" s="21"/>
-    </row>
-    <row r="155" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E155" s="21"/>
+      <c r="G154" s="21"/>
+    </row>
+    <row r="155" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F155" s="21"/>
-    </row>
-    <row r="156" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E156" s="21"/>
+      <c r="G155" s="21"/>
+    </row>
+    <row r="156" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F156" s="21"/>
-    </row>
-    <row r="157" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E157" s="21"/>
+      <c r="G156" s="21"/>
+    </row>
+    <row r="157" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F157" s="21"/>
-    </row>
-    <row r="158" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E158" s="21"/>
+      <c r="G157" s="21"/>
+    </row>
+    <row r="158" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F158" s="21"/>
-    </row>
-    <row r="159" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E159" s="21"/>
+      <c r="G158" s="21"/>
+    </row>
+    <row r="159" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F159" s="21"/>
-    </row>
-    <row r="160" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E160" s="21"/>
+      <c r="G159" s="21"/>
+    </row>
+    <row r="160" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F160" s="21"/>
-    </row>
-    <row r="161" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E161" s="21"/>
+      <c r="G160" s="21"/>
+    </row>
+    <row r="161" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F161" s="21"/>
-    </row>
-    <row r="162" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E162" s="21"/>
+      <c r="G161" s="21"/>
+    </row>
+    <row r="162" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F162" s="21"/>
-    </row>
-    <row r="163" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E163" s="21"/>
+      <c r="G162" s="21"/>
+    </row>
+    <row r="163" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F163" s="21"/>
-    </row>
-    <row r="164" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E164" s="21"/>
+      <c r="G163" s="21"/>
+    </row>
+    <row r="164" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F164" s="21"/>
-    </row>
-    <row r="165" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E165" s="21"/>
+      <c r="G164" s="21"/>
+    </row>
+    <row r="165" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F165" s="21"/>
-    </row>
-    <row r="166" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E166" s="21"/>
+      <c r="G165" s="21"/>
+    </row>
+    <row r="166" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F166" s="21"/>
-    </row>
-    <row r="167" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E167" s="21"/>
+      <c r="G166" s="21"/>
+    </row>
+    <row r="167" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F167" s="21"/>
-    </row>
-    <row r="168" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E168" s="21"/>
+      <c r="G167" s="21"/>
+    </row>
+    <row r="168" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F168" s="21"/>
-    </row>
-    <row r="169" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E169" s="21"/>
+      <c r="G168" s="21"/>
+    </row>
+    <row r="169" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F169" s="21"/>
-    </row>
-    <row r="170" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E170" s="21"/>
+      <c r="G169" s="21"/>
+    </row>
+    <row r="170" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F170" s="21"/>
-    </row>
-    <row r="171" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E171" s="21"/>
+      <c r="G170" s="21"/>
+    </row>
+    <row r="171" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F171" s="21"/>
-    </row>
-    <row r="172" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E172" s="21"/>
+      <c r="G171" s="21"/>
+    </row>
+    <row r="172" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F172" s="21"/>
-    </row>
-    <row r="173" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E173" s="21"/>
+      <c r="G172" s="21"/>
+    </row>
+    <row r="173" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F173" s="21"/>
-    </row>
-    <row r="174" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E174" s="21"/>
+      <c r="G173" s="21"/>
+    </row>
+    <row r="174" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F174" s="21"/>
-    </row>
-    <row r="175" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E175" s="21"/>
+      <c r="G174" s="21"/>
+    </row>
+    <row r="175" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F175" s="21"/>
-    </row>
-    <row r="176" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E176" s="21"/>
+      <c r="G175" s="21"/>
+    </row>
+    <row r="176" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F176" s="21"/>
-    </row>
-    <row r="177" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E177" s="21"/>
+      <c r="G176" s="21"/>
+    </row>
+    <row r="177" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F177" s="21"/>
-    </row>
-    <row r="178" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E178" s="21"/>
+      <c r="G177" s="21"/>
+    </row>
+    <row r="178" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F178" s="21"/>
-    </row>
-    <row r="179" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E179" s="21"/>
+      <c r="G178" s="21"/>
+    </row>
+    <row r="179" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F179" s="21"/>
-    </row>
-    <row r="180" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E180" s="21"/>
+      <c r="G179" s="21"/>
+    </row>
+    <row r="180" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F180" s="21"/>
-    </row>
-    <row r="181" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E181" s="21"/>
+      <c r="G180" s="21"/>
+    </row>
+    <row r="181" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F181" s="21"/>
-    </row>
-    <row r="182" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E182" s="21"/>
+      <c r="G181" s="21"/>
+    </row>
+    <row r="182" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F182" s="21"/>
-    </row>
-    <row r="183" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E183" s="21"/>
+      <c r="G182" s="21"/>
+    </row>
+    <row r="183" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F183" s="21"/>
-    </row>
-    <row r="184" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E184" s="21"/>
+      <c r="G183" s="21"/>
+    </row>
+    <row r="184" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F184" s="21"/>
-    </row>
-    <row r="185" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E185" s="21"/>
+      <c r="G184" s="21"/>
+    </row>
+    <row r="185" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F185" s="21"/>
-    </row>
-    <row r="186" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E186" s="21"/>
+      <c r="G185" s="21"/>
+    </row>
+    <row r="186" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F186" s="21"/>
-    </row>
-    <row r="187" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E187" s="21"/>
+      <c r="G186" s="21"/>
+    </row>
+    <row r="187" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F187" s="21"/>
-    </row>
-    <row r="188" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E188" s="21"/>
+      <c r="G187" s="21"/>
+    </row>
+    <row r="188" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F188" s="21"/>
-    </row>
-    <row r="189" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E189" s="21"/>
+      <c r="G188" s="21"/>
+    </row>
+    <row r="189" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F189" s="21"/>
-    </row>
-    <row r="190" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E190" s="21"/>
+      <c r="G189" s="21"/>
+    </row>
+    <row r="190" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F190" s="21"/>
-    </row>
-    <row r="191" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E191" s="21"/>
+      <c r="G190" s="21"/>
+    </row>
+    <row r="191" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F191" s="21"/>
-    </row>
-    <row r="192" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E192" s="21"/>
+      <c r="G191" s="21"/>
+    </row>
+    <row r="192" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F192" s="21"/>
-    </row>
-    <row r="193" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E193" s="21"/>
+      <c r="G192" s="21"/>
+    </row>
+    <row r="193" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F193" s="21"/>
-    </row>
-    <row r="194" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E194" s="21"/>
+      <c r="G193" s="21"/>
+    </row>
+    <row r="194" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F194" s="21"/>
-    </row>
-    <row r="195" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E195" s="21"/>
+      <c r="G194" s="21"/>
+    </row>
+    <row r="195" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F195" s="21"/>
-    </row>
-    <row r="196" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E196" s="21"/>
+      <c r="G195" s="21"/>
+    </row>
+    <row r="196" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F196" s="21"/>
-    </row>
-    <row r="197" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E197" s="21"/>
+      <c r="G196" s="21"/>
+    </row>
+    <row r="197" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F197" s="21"/>
-    </row>
-    <row r="198" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E198" s="21"/>
+      <c r="G197" s="21"/>
+    </row>
+    <row r="198" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F198" s="21"/>
-    </row>
-    <row r="199" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E199" s="21"/>
+      <c r="G198" s="21"/>
+    </row>
+    <row r="199" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F199" s="21"/>
-    </row>
-    <row r="200" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E200" s="21"/>
+      <c r="G199" s="21"/>
+    </row>
+    <row r="200" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F200" s="21"/>
-    </row>
-    <row r="201" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E201" s="21"/>
+      <c r="G200" s="21"/>
+    </row>
+    <row r="201" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F201" s="21"/>
-    </row>
-    <row r="202" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E202" s="21"/>
+      <c r="G201" s="21"/>
+    </row>
+    <row r="202" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F202" s="21"/>
-    </row>
-    <row r="203" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E203" s="21"/>
+      <c r="G202" s="21"/>
+    </row>
+    <row r="203" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F203" s="21"/>
-    </row>
-    <row r="204" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E204" s="21"/>
+      <c r="G203" s="21"/>
+    </row>
+    <row r="204" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F204" s="21"/>
-    </row>
-    <row r="205" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E205" s="21"/>
+      <c r="G204" s="21"/>
+    </row>
+    <row r="205" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F205" s="21"/>
-    </row>
-    <row r="206" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E206" s="21"/>
+      <c r="G205" s="21"/>
+    </row>
+    <row r="206" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F206" s="21"/>
-    </row>
-    <row r="207" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E207" s="21"/>
+      <c r="G206" s="21"/>
+    </row>
+    <row r="207" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F207" s="21"/>
-    </row>
-    <row r="208" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E208" s="21"/>
+      <c r="G207" s="21"/>
+    </row>
+    <row r="208" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F208" s="21"/>
-    </row>
-    <row r="209" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E209" s="21"/>
+      <c r="G208" s="21"/>
+    </row>
+    <row r="209" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F209" s="21"/>
-    </row>
-    <row r="210" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E210" s="21"/>
+      <c r="G209" s="21"/>
+    </row>
+    <row r="210" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F210" s="21"/>
-    </row>
-    <row r="211" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E211" s="21"/>
+      <c r="G210" s="21"/>
+    </row>
+    <row r="211" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F211" s="21"/>
-    </row>
-    <row r="212" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E212" s="21"/>
+      <c r="G211" s="21"/>
+    </row>
+    <row r="212" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F212" s="21"/>
-    </row>
-    <row r="213" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E213" s="21"/>
+      <c r="G212" s="21"/>
+    </row>
+    <row r="213" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F213" s="21"/>
-    </row>
-    <row r="214" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E214" s="21"/>
+      <c r="G213" s="21"/>
+    </row>
+    <row r="214" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F214" s="21"/>
-    </row>
-    <row r="215" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E215" s="21"/>
+      <c r="G214" s="21"/>
+    </row>
+    <row r="215" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F215" s="21"/>
-    </row>
-    <row r="216" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E216" s="21"/>
+      <c r="G215" s="21"/>
+    </row>
+    <row r="216" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F216" s="21"/>
-    </row>
-    <row r="217" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E217" s="21"/>
+      <c r="G216" s="21"/>
+    </row>
+    <row r="217" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F217" s="21"/>
-    </row>
-    <row r="218" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E218" s="21"/>
+      <c r="G217" s="21"/>
+    </row>
+    <row r="218" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F218" s="21"/>
-    </row>
-    <row r="219" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E219" s="21"/>
+      <c r="G218" s="21"/>
+    </row>
+    <row r="219" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F219" s="21"/>
-    </row>
-    <row r="220" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E220" s="21"/>
+      <c r="G219" s="21"/>
+    </row>
+    <row r="220" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F220" s="21"/>
-    </row>
-    <row r="221" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E221" s="21"/>
+      <c r="G220" s="21"/>
+    </row>
+    <row r="221" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F221" s="21"/>
-    </row>
-    <row r="222" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E222" s="21"/>
+      <c r="G221" s="21"/>
+    </row>
+    <row r="222" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F222" s="21"/>
-    </row>
-    <row r="223" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E223" s="21"/>
+      <c r="G222" s="21"/>
+    </row>
+    <row r="223" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F223" s="21"/>
-    </row>
-    <row r="224" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E224" s="21"/>
+      <c r="G223" s="21"/>
+    </row>
+    <row r="224" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F224" s="21"/>
-    </row>
-    <row r="225" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E225" s="21"/>
+      <c r="G224" s="21"/>
+    </row>
+    <row r="225" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F225" s="21"/>
-    </row>
-    <row r="226" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E226" s="21"/>
+      <c r="G225" s="21"/>
+    </row>
+    <row r="226" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F226" s="21"/>
-    </row>
-    <row r="227" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E227" s="21"/>
+      <c r="G226" s="21"/>
+    </row>
+    <row r="227" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F227" s="21"/>
-    </row>
-    <row r="228" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E228" s="21"/>
+      <c r="G227" s="21"/>
+    </row>
+    <row r="228" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F228" s="21"/>
-    </row>
-    <row r="229" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E229" s="21"/>
+      <c r="G228" s="21"/>
+    </row>
+    <row r="229" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F229" s="21"/>
-    </row>
-    <row r="230" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E230" s="21"/>
+      <c r="G229" s="21"/>
+    </row>
+    <row r="230" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F230" s="21"/>
-    </row>
-    <row r="231" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E231" s="21"/>
+      <c r="G230" s="21"/>
+    </row>
+    <row r="231" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F231" s="21"/>
-    </row>
-    <row r="232" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E232" s="21"/>
+      <c r="G231" s="21"/>
+    </row>
+    <row r="232" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F232" s="21"/>
-    </row>
-    <row r="233" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E233" s="21"/>
+      <c r="G232" s="21"/>
+    </row>
+    <row r="233" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F233" s="21"/>
-    </row>
-    <row r="234" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E234" s="21"/>
+      <c r="G233" s="21"/>
+    </row>
+    <row r="234" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F234" s="21"/>
-    </row>
-    <row r="235" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E235" s="21"/>
+      <c r="G234" s="21"/>
+    </row>
+    <row r="235" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F235" s="21"/>
-    </row>
-    <row r="236" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E236" s="21"/>
+      <c r="G235" s="21"/>
+    </row>
+    <row r="236" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F236" s="21"/>
-    </row>
-    <row r="237" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E237" s="21"/>
+      <c r="G236" s="21"/>
+    </row>
+    <row r="237" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F237" s="21"/>
-    </row>
-    <row r="238" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E238" s="21"/>
+      <c r="G237" s="21"/>
+    </row>
+    <row r="238" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F238" s="21"/>
-    </row>
-    <row r="239" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E239" s="21"/>
+      <c r="G238" s="21"/>
+    </row>
+    <row r="239" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F239" s="21"/>
-    </row>
-    <row r="240" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E240" s="21"/>
+      <c r="G239" s="21"/>
+    </row>
+    <row r="240" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F240" s="21"/>
-    </row>
-    <row r="241" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E241" s="21"/>
+      <c r="G240" s="21"/>
+    </row>
+    <row r="241" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F241" s="21"/>
-    </row>
-    <row r="242" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E242" s="21"/>
+      <c r="G241" s="21"/>
+    </row>
+    <row r="242" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F242" s="21"/>
-    </row>
-    <row r="243" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E243" s="21"/>
+      <c r="G242" s="21"/>
+    </row>
+    <row r="243" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F243" s="21"/>
-    </row>
-    <row r="244" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E244" s="21"/>
+      <c r="G243" s="21"/>
+    </row>
+    <row r="244" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F244" s="21"/>
-    </row>
-    <row r="245" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E245" s="21"/>
+      <c r="G244" s="21"/>
+    </row>
+    <row r="245" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F245" s="21"/>
-    </row>
-    <row r="246" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E246" s="21"/>
+      <c r="G245" s="21"/>
+    </row>
+    <row r="246" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F246" s="21"/>
-    </row>
-    <row r="247" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E247" s="21"/>
+      <c r="G246" s="21"/>
+    </row>
+    <row r="247" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F247" s="21"/>
-    </row>
-    <row r="248" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E248" s="21"/>
+      <c r="G247" s="21"/>
+    </row>
+    <row r="248" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F248" s="21"/>
-    </row>
-    <row r="249" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E249" s="21"/>
+      <c r="G248" s="21"/>
+    </row>
+    <row r="249" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F249" s="21"/>
-    </row>
-    <row r="250" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E250" s="21"/>
+      <c r="G249" s="21"/>
+    </row>
+    <row r="250" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F250" s="21"/>
-    </row>
-    <row r="251" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E251" s="21"/>
+      <c r="G250" s="21"/>
+    </row>
+    <row r="251" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F251" s="21"/>
-    </row>
-    <row r="252" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E252" s="21"/>
+      <c r="G251" s="21"/>
+    </row>
+    <row r="252" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F252" s="21"/>
-    </row>
-    <row r="253" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E253" s="21"/>
+      <c r="G252" s="21"/>
+    </row>
+    <row r="253" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F253" s="21"/>
-    </row>
-    <row r="254" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E254" s="21"/>
+      <c r="G253" s="21"/>
+    </row>
+    <row r="254" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F254" s="21"/>
-    </row>
-    <row r="255" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E255" s="21"/>
+      <c r="G254" s="21"/>
+    </row>
+    <row r="255" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F255" s="21"/>
-    </row>
-    <row r="256" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E256" s="21"/>
+      <c r="G255" s="21"/>
+    </row>
+    <row r="256" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F256" s="21"/>
-    </row>
-    <row r="257" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E257" s="21"/>
+      <c r="G256" s="21"/>
+    </row>
+    <row r="257" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F257" s="21"/>
-    </row>
-    <row r="258" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E258" s="21"/>
+      <c r="G257" s="21"/>
+    </row>
+    <row r="258" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F258" s="21"/>
-    </row>
-    <row r="259" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E259" s="21"/>
+      <c r="G258" s="21"/>
+    </row>
+    <row r="259" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F259" s="21"/>
-    </row>
-    <row r="260" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E260" s="21"/>
+      <c r="G259" s="21"/>
+    </row>
+    <row r="260" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F260" s="21"/>
-    </row>
-    <row r="261" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E261" s="21"/>
+      <c r="G260" s="21"/>
+    </row>
+    <row r="261" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F261" s="21"/>
-    </row>
-    <row r="262" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E262" s="21"/>
+      <c r="G261" s="21"/>
+    </row>
+    <row r="262" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F262" s="21"/>
-    </row>
-    <row r="263" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E263" s="21"/>
+      <c r="G262" s="21"/>
+    </row>
+    <row r="263" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F263" s="21"/>
-    </row>
-    <row r="264" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E264" s="21"/>
+      <c r="G263" s="21"/>
+    </row>
+    <row r="264" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F264" s="21"/>
-    </row>
-    <row r="265" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E265" s="21"/>
+      <c r="G264" s="21"/>
+    </row>
+    <row r="265" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F265" s="21"/>
-    </row>
-    <row r="266" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E266" s="21"/>
+      <c r="G265" s="21"/>
+    </row>
+    <row r="266" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F266" s="21"/>
-    </row>
-    <row r="267" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E267" s="21"/>
+      <c r="G266" s="21"/>
+    </row>
+    <row r="267" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F267" s="21"/>
-    </row>
-    <row r="268" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E268" s="21"/>
+      <c r="G267" s="21"/>
+    </row>
+    <row r="268" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F268" s="21"/>
-    </row>
-    <row r="269" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E269" s="21"/>
+      <c r="G268" s="21"/>
+    </row>
+    <row r="269" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F269" s="21"/>
-    </row>
-    <row r="270" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E270" s="21"/>
+      <c r="G269" s="21"/>
+    </row>
+    <row r="270" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F270" s="21"/>
-    </row>
-    <row r="271" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E271" s="21"/>
+      <c r="G270" s="21"/>
+    </row>
+    <row r="271" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F271" s="21"/>
-    </row>
-    <row r="272" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E272" s="21"/>
+      <c r="G271" s="21"/>
+    </row>
+    <row r="272" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F272" s="21"/>
-    </row>
-    <row r="273" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E273" s="21"/>
+      <c r="G272" s="21"/>
+    </row>
+    <row r="273" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F273" s="21"/>
-    </row>
-    <row r="274" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E274" s="21"/>
+      <c r="G273" s="21"/>
+    </row>
+    <row r="274" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F274" s="21"/>
-    </row>
-    <row r="275" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E275" s="21"/>
+      <c r="G274" s="21"/>
+    </row>
+    <row r="275" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F275" s="21"/>
-    </row>
-    <row r="276" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E276" s="21"/>
+      <c r="G275" s="21"/>
+    </row>
+    <row r="276" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F276" s="21"/>
-    </row>
-    <row r="277" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E277" s="21"/>
+      <c r="G276" s="21"/>
+    </row>
+    <row r="277" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F277" s="21"/>
-    </row>
-    <row r="278" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E278" s="21"/>
+      <c r="G277" s="21"/>
+    </row>
+    <row r="278" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F278" s="21"/>
-    </row>
-    <row r="279" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E279" s="21"/>
+      <c r="G278" s="21"/>
+    </row>
+    <row r="279" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F279" s="21"/>
-    </row>
-    <row r="280" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E280" s="21"/>
+      <c r="G279" s="21"/>
+    </row>
+    <row r="280" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F280" s="21"/>
-    </row>
-    <row r="281" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E281" s="21"/>
+      <c r="G280" s="21"/>
+    </row>
+    <row r="281" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F281" s="21"/>
-    </row>
-    <row r="282" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E282" s="21"/>
+      <c r="G281" s="21"/>
+    </row>
+    <row r="282" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F282" s="21"/>
-    </row>
-    <row r="283" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E283" s="21"/>
+      <c r="G282" s="21"/>
+    </row>
+    <row r="283" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F283" s="21"/>
-    </row>
-    <row r="284" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E284" s="21"/>
+      <c r="G283" s="21"/>
+    </row>
+    <row r="284" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F284" s="21"/>
-    </row>
-    <row r="285" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E285" s="21"/>
+      <c r="G284" s="21"/>
+    </row>
+    <row r="285" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F285" s="21"/>
-    </row>
-    <row r="286" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E286" s="21"/>
+      <c r="G285" s="21"/>
+    </row>
+    <row r="286" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F286" s="21"/>
-    </row>
-    <row r="287" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E287" s="21"/>
+      <c r="G286" s="21"/>
+    </row>
+    <row r="287" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F287" s="21"/>
-    </row>
-    <row r="288" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E288" s="21"/>
+      <c r="G287" s="21"/>
+    </row>
+    <row r="288" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F288" s="21"/>
-    </row>
-    <row r="289" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E289" s="21"/>
+      <c r="G288" s="21"/>
+    </row>
+    <row r="289" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F289" s="21"/>
-    </row>
-    <row r="290" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E290" s="21"/>
+      <c r="G289" s="21"/>
+    </row>
+    <row r="290" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F290" s="21"/>
-    </row>
-    <row r="291" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E291" s="21"/>
+      <c r="G290" s="21"/>
+    </row>
+    <row r="291" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F291" s="21"/>
-    </row>
-    <row r="292" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E292" s="21"/>
+      <c r="G291" s="21"/>
+    </row>
+    <row r="292" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F292" s="21"/>
-    </row>
-    <row r="293" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E293" s="21"/>
+      <c r="G292" s="21"/>
+    </row>
+    <row r="293" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F293" s="21"/>
-    </row>
-    <row r="294" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E294" s="21"/>
+      <c r="G293" s="21"/>
+    </row>
+    <row r="294" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F294" s="21"/>
-    </row>
-    <row r="295" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E295" s="21"/>
+      <c r="G294" s="21"/>
+    </row>
+    <row r="295" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F295" s="21"/>
-    </row>
-    <row r="296" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E296" s="21"/>
+      <c r="G295" s="21"/>
+    </row>
+    <row r="296" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F296" s="21"/>
-    </row>
-    <row r="297" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E297" s="21"/>
+      <c r="G296" s="21"/>
+    </row>
+    <row r="297" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F297" s="21"/>
-    </row>
-    <row r="298" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E298" s="21"/>
+      <c r="G297" s="21"/>
+    </row>
+    <row r="298" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F298" s="21"/>
-    </row>
-    <row r="299" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E299" s="21"/>
+      <c r="G298" s="21"/>
+    </row>
+    <row r="299" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F299" s="21"/>
-    </row>
-    <row r="300" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E300" s="21"/>
+      <c r="G299" s="21"/>
+    </row>
+    <row r="300" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F300" s="21"/>
-    </row>
-    <row r="301" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E301" s="21"/>
+      <c r="G300" s="21"/>
+    </row>
+    <row r="301" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F301" s="21"/>
-    </row>
-    <row r="302" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E302" s="21"/>
+      <c r="G301" s="21"/>
+    </row>
+    <row r="302" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F302" s="21"/>
-    </row>
-    <row r="303" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E303" s="21"/>
+      <c r="G302" s="21"/>
+    </row>
+    <row r="303" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F303" s="21"/>
-    </row>
-    <row r="304" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E304" s="21"/>
+      <c r="G303" s="21"/>
+    </row>
+    <row r="304" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F304" s="21"/>
-    </row>
-    <row r="305" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E305" s="21"/>
+      <c r="G304" s="21"/>
+    </row>
+    <row r="305" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F305" s="21"/>
-    </row>
-    <row r="306" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E306" s="21"/>
+      <c r="G305" s="21"/>
+    </row>
+    <row r="306" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F306" s="21"/>
-    </row>
-    <row r="307" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E307" s="21"/>
+      <c r="G306" s="21"/>
+    </row>
+    <row r="307" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F307" s="21"/>
-    </row>
-    <row r="308" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E308" s="21"/>
+      <c r="G307" s="21"/>
+    </row>
+    <row r="308" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F308" s="21"/>
-    </row>
-    <row r="309" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E309" s="21"/>
+      <c r="G308" s="21"/>
+    </row>
+    <row r="309" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F309" s="21"/>
-    </row>
-    <row r="310" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E310" s="21"/>
+      <c r="G309" s="21"/>
+    </row>
+    <row r="310" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F310" s="21"/>
-    </row>
-    <row r="311" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E311" s="21"/>
+      <c r="G310" s="21"/>
+    </row>
+    <row r="311" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F311" s="21"/>
-    </row>
-    <row r="312" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E312" s="21"/>
+      <c r="G311" s="21"/>
+    </row>
+    <row r="312" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F312" s="21"/>
-    </row>
-    <row r="313" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E313" s="21"/>
+      <c r="G312" s="21"/>
+    </row>
+    <row r="313" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F313" s="21"/>
-    </row>
-    <row r="314" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E314" s="21"/>
+      <c r="G313" s="21"/>
+    </row>
+    <row r="314" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F314" s="21"/>
-    </row>
-    <row r="315" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E315" s="21"/>
+      <c r="G314" s="21"/>
+    </row>
+    <row r="315" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F315" s="21"/>
-    </row>
-    <row r="316" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E316" s="21"/>
+      <c r="G315" s="21"/>
+    </row>
+    <row r="316" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F316" s="21"/>
-    </row>
-    <row r="317" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E317" s="21"/>
+      <c r="G316" s="21"/>
+    </row>
+    <row r="317" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F317" s="21"/>
-    </row>
-    <row r="318" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E318" s="21"/>
+      <c r="G317" s="21"/>
+    </row>
+    <row r="318" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F318" s="21"/>
-    </row>
-    <row r="319" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E319" s="21"/>
+      <c r="G318" s="21"/>
+    </row>
+    <row r="319" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F319" s="21"/>
-    </row>
-    <row r="320" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E320" s="21"/>
+      <c r="G319" s="21"/>
+    </row>
+    <row r="320" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F320" s="21"/>
-    </row>
-    <row r="321" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E321" s="21"/>
+      <c r="G320" s="21"/>
+    </row>
+    <row r="321" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F321" s="21"/>
-    </row>
-    <row r="322" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E322" s="21"/>
+      <c r="G321" s="21"/>
+    </row>
+    <row r="322" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F322" s="21"/>
-    </row>
-    <row r="323" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E323" s="21"/>
+      <c r="G322" s="21"/>
+    </row>
+    <row r="323" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F323" s="21"/>
-    </row>
-    <row r="324" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E324" s="21"/>
+      <c r="G323" s="21"/>
+    </row>
+    <row r="324" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F324" s="21"/>
-    </row>
-    <row r="325" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E325" s="21"/>
+      <c r="G324" s="21"/>
+    </row>
+    <row r="325" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F325" s="21"/>
-    </row>
-    <row r="326" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E326" s="21"/>
+      <c r="G325" s="21"/>
+    </row>
+    <row r="326" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F326" s="21"/>
-    </row>
-    <row r="327" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E327" s="21"/>
+      <c r="G326" s="21"/>
+    </row>
+    <row r="327" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F327" s="21"/>
-    </row>
-    <row r="328" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E328" s="21"/>
+      <c r="G327" s="21"/>
+    </row>
+    <row r="328" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F328" s="21"/>
-    </row>
-    <row r="329" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E329" s="21"/>
+      <c r="G328" s="21"/>
+    </row>
+    <row r="329" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F329" s="21"/>
-    </row>
-    <row r="330" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E330" s="21"/>
+      <c r="G329" s="21"/>
+    </row>
+    <row r="330" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F330" s="21"/>
-    </row>
-    <row r="331" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E331" s="21"/>
+      <c r="G330" s="21"/>
+    </row>
+    <row r="331" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F331" s="21"/>
-    </row>
-    <row r="332" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E332" s="21"/>
+      <c r="G331" s="21"/>
+    </row>
+    <row r="332" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F332" s="21"/>
-    </row>
-    <row r="333" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E333" s="21"/>
+      <c r="G332" s="21"/>
+    </row>
+    <row r="333" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F333" s="21"/>
-    </row>
-    <row r="334" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E334" s="21"/>
+      <c r="G333" s="21"/>
+    </row>
+    <row r="334" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F334" s="21"/>
-    </row>
-    <row r="335" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E335" s="21"/>
+      <c r="G334" s="21"/>
+    </row>
+    <row r="335" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F335" s="21"/>
-    </row>
-    <row r="336" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E336" s="21"/>
+      <c r="G335" s="21"/>
+    </row>
+    <row r="336" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F336" s="21"/>
-    </row>
-    <row r="337" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E337" s="21"/>
+      <c r="G336" s="21"/>
+    </row>
+    <row r="337" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F337" s="21"/>
-    </row>
-    <row r="338" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E338" s="21"/>
+      <c r="G337" s="21"/>
+    </row>
+    <row r="338" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F338" s="21"/>
-    </row>
-    <row r="339" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E339" s="21"/>
+      <c r="G338" s="21"/>
+    </row>
+    <row r="339" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F339" s="21"/>
-    </row>
-    <row r="340" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E340" s="21"/>
+      <c r="G339" s="21"/>
+    </row>
+    <row r="340" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F340" s="21"/>
-    </row>
-    <row r="341" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E341" s="21"/>
+      <c r="G340" s="21"/>
+    </row>
+    <row r="341" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F341" s="21"/>
-    </row>
-    <row r="342" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E342" s="21"/>
+      <c r="G341" s="21"/>
+    </row>
+    <row r="342" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F342" s="21"/>
-    </row>
-    <row r="343" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E343" s="21"/>
+      <c r="G342" s="21"/>
+    </row>
+    <row r="343" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F343" s="21"/>
-    </row>
-    <row r="344" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E344" s="21"/>
+      <c r="G343" s="21"/>
+    </row>
+    <row r="344" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F344" s="21"/>
-    </row>
-    <row r="345" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E345" s="21"/>
+      <c r="G344" s="21"/>
+    </row>
+    <row r="345" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F345" s="21"/>
-    </row>
-    <row r="346" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E346" s="21"/>
+      <c r="G345" s="21"/>
+    </row>
+    <row r="346" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F346" s="21"/>
-    </row>
-    <row r="347" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E347" s="21"/>
+      <c r="G346" s="21"/>
+    </row>
+    <row r="347" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F347" s="21"/>
-    </row>
-    <row r="348" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E348" s="21"/>
+      <c r="G347" s="21"/>
+    </row>
+    <row r="348" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F348" s="21"/>
-    </row>
-    <row r="349" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E349" s="21"/>
+      <c r="G348" s="21"/>
+    </row>
+    <row r="349" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F349" s="21"/>
-    </row>
-    <row r="350" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E350" s="21"/>
+      <c r="G349" s="21"/>
+    </row>
+    <row r="350" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F350" s="21"/>
-    </row>
-    <row r="351" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E351" s="21"/>
+      <c r="G350" s="21"/>
+    </row>
+    <row r="351" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F351" s="21"/>
-    </row>
-    <row r="352" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E352" s="21"/>
+      <c r="G351" s="21"/>
+    </row>
+    <row r="352" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F352" s="21"/>
-    </row>
-    <row r="353" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E353" s="21"/>
+      <c r="G352" s="21"/>
+    </row>
+    <row r="353" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F353" s="21"/>
-    </row>
-    <row r="354" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E354" s="21"/>
+      <c r="G353" s="21"/>
+    </row>
+    <row r="354" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F354" s="21"/>
-    </row>
-    <row r="355" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E355" s="21"/>
+      <c r="G354" s="21"/>
+    </row>
+    <row r="355" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F355" s="21"/>
-    </row>
-    <row r="356" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E356" s="21"/>
+      <c r="G355" s="21"/>
+    </row>
+    <row r="356" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F356" s="21"/>
-    </row>
-    <row r="357" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E357" s="21"/>
+      <c r="G356" s="21"/>
+    </row>
+    <row r="357" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F357" s="21"/>
-    </row>
-    <row r="358" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E358" s="21"/>
+      <c r="G357" s="21"/>
+    </row>
+    <row r="358" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F358" s="21"/>
-    </row>
-    <row r="359" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E359" s="21"/>
+      <c r="G358" s="21"/>
+    </row>
+    <row r="359" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F359" s="21"/>
-    </row>
-    <row r="360" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E360" s="21"/>
+      <c r="G359" s="21"/>
+    </row>
+    <row r="360" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F360" s="21"/>
-    </row>
-    <row r="361" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E361" s="21"/>
+      <c r="G360" s="21"/>
+    </row>
+    <row r="361" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F361" s="21"/>
-    </row>
-    <row r="362" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E362" s="21"/>
+      <c r="G361" s="21"/>
+    </row>
+    <row r="362" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F362" s="21"/>
-    </row>
-    <row r="369" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E369" s="21"/>
+      <c r="G362" s="21"/>
+    </row>
+    <row r="369" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F369" s="21"/>
-    </row>
-    <row r="370" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E370" s="21"/>
+      <c r="G369" s="21"/>
+    </row>
+    <row r="370" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F370" s="21"/>
-    </row>
-    <row r="371" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E371" s="21"/>
+      <c r="G370" s="21"/>
+    </row>
+    <row r="371" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F371" s="21"/>
-    </row>
-    <row r="372" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E372" s="21"/>
+      <c r="G371" s="21"/>
+    </row>
+    <row r="372" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F372" s="21"/>
-    </row>
-    <row r="373" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E373" s="21"/>
+      <c r="G372" s="21"/>
+    </row>
+    <row r="373" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F373" s="21"/>
-    </row>
-    <row r="374" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E374" s="21"/>
+      <c r="G373" s="21"/>
+    </row>
+    <row r="374" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F374" s="21"/>
-    </row>
-    <row r="375" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E375" s="21"/>
+      <c r="G374" s="21"/>
+    </row>
+    <row r="375" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F375" s="21"/>
-    </row>
-    <row r="376" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E376" s="21"/>
+      <c r="G375" s="21"/>
+    </row>
+    <row r="376" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F376" s="21"/>
-    </row>
-    <row r="377" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E377" s="21"/>
+      <c r="G376" s="21"/>
+    </row>
+    <row r="377" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F377" s="21"/>
-    </row>
-    <row r="378" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E378" s="21"/>
+      <c r="G377" s="21"/>
+    </row>
+    <row r="378" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F378" s="21"/>
-    </row>
-    <row r="379" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E379" s="21"/>
+      <c r="G378" s="21"/>
+    </row>
+    <row r="379" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F379" s="21"/>
-    </row>
-    <row r="380" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E380" s="21"/>
+      <c r="G379" s="21"/>
+    </row>
+    <row r="380" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F380" s="21"/>
-    </row>
-    <row r="381" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E381" s="21"/>
+      <c r="G380" s="21"/>
+    </row>
+    <row r="381" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F381" s="21"/>
-    </row>
-    <row r="382" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E382" s="21"/>
+      <c r="G381" s="21"/>
+    </row>
+    <row r="382" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F382" s="21"/>
-    </row>
-    <row r="383" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E383" s="21"/>
+      <c r="G382" s="21"/>
+    </row>
+    <row r="383" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F383" s="21"/>
-    </row>
-    <row r="384" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E384" s="21"/>
+      <c r="G383" s="21"/>
+    </row>
+    <row r="384" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F384" s="21"/>
-    </row>
-    <row r="385" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E385" s="21"/>
+      <c r="G384" s="21"/>
+    </row>
+    <row r="385" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F385" s="21"/>
-    </row>
-    <row r="386" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E386" s="21"/>
+      <c r="G385" s="21"/>
+    </row>
+    <row r="386" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F386" s="21"/>
-    </row>
-    <row r="387" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E387" s="21"/>
+      <c r="G386" s="21"/>
+    </row>
+    <row r="387" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F387" s="21"/>
-    </row>
-    <row r="388" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E388" s="21"/>
+      <c r="G387" s="21"/>
+    </row>
+    <row r="388" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F388" s="21"/>
-    </row>
-    <row r="389" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E389" s="21"/>
+      <c r="G388" s="21"/>
+    </row>
+    <row r="389" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F389" s="21"/>
-    </row>
-    <row r="390" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E390" s="21"/>
+      <c r="G389" s="21"/>
+    </row>
+    <row r="390" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F390" s="21"/>
-    </row>
-    <row r="391" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E391" s="21"/>
+      <c r="G390" s="21"/>
+    </row>
+    <row r="391" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F391" s="21"/>
-    </row>
-    <row r="392" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E392" s="21"/>
+      <c r="G391" s="21"/>
+    </row>
+    <row r="392" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F392" s="21"/>
-    </row>
-    <row r="393" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E393" s="21"/>
+      <c r="G392" s="21"/>
+    </row>
+    <row r="393" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F393" s="21"/>
-    </row>
-    <row r="394" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E394" s="21"/>
+      <c r="G393" s="21"/>
+    </row>
+    <row r="394" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F394" s="21"/>
-    </row>
-    <row r="395" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E395" s="21"/>
+      <c r="G394" s="21"/>
+    </row>
+    <row r="395" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F395" s="21"/>
-    </row>
-    <row r="396" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E396" s="21"/>
+      <c r="G395" s="21"/>
+    </row>
+    <row r="396" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F396" s="21"/>
-    </row>
-    <row r="397" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E397" s="21"/>
+      <c r="G396" s="21"/>
+    </row>
+    <row r="397" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F397" s="21"/>
-    </row>
-    <row r="398" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E398" s="21"/>
+      <c r="G397" s="21"/>
+    </row>
+    <row r="398" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F398" s="21"/>
-    </row>
-    <row r="399" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E399" s="21"/>
+      <c r="G398" s="21"/>
+    </row>
+    <row r="399" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F399" s="21"/>
-    </row>
-    <row r="400" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E400" s="21"/>
+      <c r="G399" s="21"/>
+    </row>
+    <row r="400" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F400" s="21"/>
-    </row>
-    <row r="401" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E401" s="21"/>
+      <c r="G400" s="21"/>
+    </row>
+    <row r="401" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F401" s="21"/>
-    </row>
-    <row r="402" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E402" s="21"/>
+      <c r="G401" s="21"/>
+    </row>
+    <row r="402" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F402" s="21"/>
-    </row>
-    <row r="403" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E403" s="21"/>
+      <c r="G402" s="21"/>
+    </row>
+    <row r="403" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F403" s="21"/>
-    </row>
-    <row r="404" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E404" s="21"/>
+      <c r="G403" s="21"/>
+    </row>
+    <row r="404" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F404" s="21"/>
-    </row>
-    <row r="405" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E405" s="21"/>
+      <c r="G404" s="21"/>
+    </row>
+    <row r="405" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F405" s="21"/>
-    </row>
-    <row r="406" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E406" s="21"/>
+      <c r="G405" s="21"/>
+    </row>
+    <row r="406" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F406" s="21"/>
-    </row>
-    <row r="407" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E407" s="21"/>
+      <c r="G406" s="21"/>
+    </row>
+    <row r="407" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F407" s="21"/>
-    </row>
-    <row r="408" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E408" s="21"/>
+      <c r="G407" s="21"/>
+    </row>
+    <row r="408" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F408" s="21"/>
-    </row>
-    <row r="409" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E409" s="21"/>
+      <c r="G408" s="21"/>
+    </row>
+    <row r="409" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F409" s="21"/>
-    </row>
-    <row r="410" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E410" s="21"/>
+      <c r="G409" s="21"/>
+    </row>
+    <row r="410" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F410" s="21"/>
-    </row>
-    <row r="411" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E411" s="21"/>
+      <c r="G410" s="21"/>
+    </row>
+    <row r="411" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F411" s="21"/>
-    </row>
-    <row r="412" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E412" s="21"/>
+      <c r="G411" s="21"/>
+    </row>
+    <row r="412" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F412" s="21"/>
-    </row>
-    <row r="413" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E413" s="21"/>
+      <c r="G412" s="21"/>
+    </row>
+    <row r="413" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F413" s="21"/>
-    </row>
-    <row r="414" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E414" s="21"/>
+      <c r="G413" s="21"/>
+    </row>
+    <row r="414" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F414" s="21"/>
-    </row>
-    <row r="415" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E415" s="21"/>
+      <c r="G414" s="21"/>
+    </row>
+    <row r="415" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F415" s="21"/>
-    </row>
-    <row r="416" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E416" s="21"/>
+      <c r="G415" s="21"/>
+    </row>
+    <row r="416" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F416" s="21"/>
-    </row>
-    <row r="417" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E417" s="21"/>
+      <c r="G416" s="21"/>
+    </row>
+    <row r="417" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F417" s="21"/>
-    </row>
-    <row r="418" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E418" s="21"/>
+      <c r="G417" s="21"/>
+    </row>
+    <row r="418" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F418" s="21"/>
-    </row>
-    <row r="419" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E419" s="21"/>
+      <c r="G418" s="21"/>
+    </row>
+    <row r="419" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F419" s="21"/>
-    </row>
-    <row r="420" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E420" s="21"/>
+      <c r="G419" s="21"/>
+    </row>
+    <row r="420" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F420" s="21"/>
-    </row>
-    <row r="421" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E421" s="21"/>
+      <c r="G420" s="21"/>
+    </row>
+    <row r="421" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F421" s="21"/>
-    </row>
-    <row r="422" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E422" s="21"/>
+      <c r="G421" s="21"/>
+    </row>
+    <row r="422" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F422" s="21"/>
-    </row>
-    <row r="423" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E423" s="21"/>
+      <c r="G422" s="21"/>
+    </row>
+    <row r="423" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F423" s="21"/>
-    </row>
-    <row r="424" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E424" s="21"/>
+      <c r="G423" s="21"/>
+    </row>
+    <row r="424" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F424" s="21"/>
-    </row>
-    <row r="425" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E425" s="21"/>
+      <c r="G424" s="21"/>
+    </row>
+    <row r="425" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F425" s="21"/>
-    </row>
-    <row r="426" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E426" s="21"/>
+      <c r="G425" s="21"/>
+    </row>
+    <row r="426" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F426" s="21"/>
-    </row>
-    <row r="427" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E427" s="21"/>
+      <c r="G426" s="21"/>
+    </row>
+    <row r="427" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F427" s="21"/>
-    </row>
-    <row r="428" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E428" s="21"/>
+      <c r="G427" s="21"/>
+    </row>
+    <row r="428" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F428" s="21"/>
-    </row>
-    <row r="429" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E429" s="21"/>
+      <c r="G428" s="21"/>
+    </row>
+    <row r="429" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F429" s="21"/>
-    </row>
-    <row r="430" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E430" s="21"/>
+      <c r="G429" s="21"/>
+    </row>
+    <row r="430" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F430" s="21"/>
-    </row>
-    <row r="431" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E431" s="21"/>
+      <c r="G430" s="21"/>
+    </row>
+    <row r="431" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F431" s="21"/>
-    </row>
-    <row r="432" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E432" s="21"/>
+      <c r="G431" s="21"/>
+    </row>
+    <row r="432" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F432" s="21"/>
-    </row>
-    <row r="433" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E433" s="21"/>
+      <c r="G432" s="21"/>
+    </row>
+    <row r="433" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F433" s="21"/>
-    </row>
-    <row r="434" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E434" s="21"/>
+      <c r="G433" s="21"/>
+    </row>
+    <row r="434" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F434" s="21"/>
-    </row>
-    <row r="435" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E435" s="21"/>
+      <c r="G434" s="21"/>
+    </row>
+    <row r="435" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F435" s="21"/>
-    </row>
-    <row r="436" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E436" s="21"/>
+      <c r="G435" s="21"/>
+    </row>
+    <row r="436" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F436" s="21"/>
-    </row>
-    <row r="437" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E437" s="21"/>
+      <c r="G436" s="21"/>
+    </row>
+    <row r="437" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F437" s="21"/>
-    </row>
-    <row r="438" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E438" s="21"/>
+      <c r="G437" s="21"/>
+    </row>
+    <row r="438" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F438" s="21"/>
-    </row>
-    <row r="439" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E439" s="21"/>
+      <c r="G438" s="21"/>
+    </row>
+    <row r="439" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F439" s="21"/>
-    </row>
-    <row r="440" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E440" s="21"/>
+      <c r="G439" s="21"/>
+    </row>
+    <row r="440" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F440" s="21"/>
-    </row>
-    <row r="441" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E441" s="21"/>
+      <c r="G440" s="21"/>
+    </row>
+    <row r="441" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F441" s="21"/>
-    </row>
-    <row r="442" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E442" s="21"/>
+      <c r="G441" s="21"/>
+    </row>
+    <row r="442" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F442" s="21"/>
-    </row>
-    <row r="443" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E443" s="21"/>
+      <c r="G442" s="21"/>
+    </row>
+    <row r="443" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F443" s="21"/>
-    </row>
-    <row r="444" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E444" s="21"/>
+      <c r="G443" s="21"/>
+    </row>
+    <row r="444" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F444" s="21"/>
-    </row>
-    <row r="445" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E445" s="21"/>
+      <c r="G444" s="21"/>
+    </row>
+    <row r="445" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F445" s="21"/>
-    </row>
-    <row r="446" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E446" s="21"/>
+      <c r="G445" s="21"/>
+    </row>
+    <row r="446" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F446" s="21"/>
-    </row>
-    <row r="447" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E447" s="21"/>
+      <c r="G446" s="21"/>
+    </row>
+    <row r="447" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F447" s="21"/>
-    </row>
-    <row r="448" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E448" s="21"/>
+      <c r="G447" s="21"/>
+    </row>
+    <row r="448" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F448" s="21"/>
-    </row>
-    <row r="449" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E449" s="21"/>
+      <c r="G448" s="21"/>
+    </row>
+    <row r="449" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F449" s="21"/>
-    </row>
-    <row r="450" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E450" s="21"/>
+      <c r="G449" s="21"/>
+    </row>
+    <row r="450" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F450" s="21"/>
-    </row>
-    <row r="451" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E451" s="21"/>
+      <c r="G450" s="21"/>
+    </row>
+    <row r="451" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F451" s="21"/>
-    </row>
-    <row r="452" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E452" s="21"/>
+      <c r="G451" s="21"/>
+    </row>
+    <row r="452" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F452" s="21"/>
-    </row>
-    <row r="453" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E453" s="21"/>
+      <c r="G452" s="21"/>
+    </row>
+    <row r="453" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F453" s="21"/>
-    </row>
-    <row r="454" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E454" s="21"/>
+      <c r="G453" s="21"/>
+    </row>
+    <row r="454" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F454" s="21"/>
-    </row>
-    <row r="455" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E455" s="21"/>
+      <c r="G454" s="21"/>
+    </row>
+    <row r="455" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F455" s="21"/>
-    </row>
-    <row r="456" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E456" s="21"/>
+      <c r="G455" s="21"/>
+    </row>
+    <row r="456" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F456" s="21"/>
-    </row>
-    <row r="457" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E457" s="21"/>
+      <c r="G456" s="21"/>
+    </row>
+    <row r="457" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F457" s="21"/>
-    </row>
-    <row r="458" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E458" s="21"/>
+      <c r="G457" s="21"/>
+    </row>
+    <row r="458" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F458" s="21"/>
-    </row>
-    <row r="459" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E459" s="21"/>
+      <c r="G458" s="21"/>
+    </row>
+    <row r="459" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F459" s="21"/>
-    </row>
-    <row r="460" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E460" s="21"/>
+      <c r="G459" s="21"/>
+    </row>
+    <row r="460" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F460" s="21"/>
-    </row>
-    <row r="461" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E461" s="21"/>
+      <c r="G460" s="21"/>
+    </row>
+    <row r="461" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F461" s="21"/>
-    </row>
-    <row r="462" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E462" s="21"/>
+      <c r="G461" s="21"/>
+    </row>
+    <row r="462" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F462" s="21"/>
-    </row>
-    <row r="463" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E463" s="21"/>
+      <c r="G462" s="21"/>
+    </row>
+    <row r="463" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F463" s="21"/>
-    </row>
-    <row r="464" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E464" s="21"/>
+      <c r="G463" s="21"/>
+    </row>
+    <row r="464" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F464" s="21"/>
-    </row>
-    <row r="465" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E465" s="21"/>
+      <c r="G464" s="21"/>
+    </row>
+    <row r="465" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F465" s="21"/>
-    </row>
-    <row r="466" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E466" s="21"/>
+      <c r="G465" s="21"/>
+    </row>
+    <row r="466" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F466" s="21"/>
-    </row>
-    <row r="467" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E467" s="21"/>
+      <c r="G466" s="21"/>
+    </row>
+    <row r="467" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F467" s="21"/>
-    </row>
-    <row r="468" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E468" s="21"/>
+      <c r="G467" s="21"/>
+    </row>
+    <row r="468" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F468" s="21"/>
-    </row>
-    <row r="469" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E469" s="21"/>
+      <c r="G468" s="21"/>
+    </row>
+    <row r="469" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F469" s="21"/>
-    </row>
-    <row r="470" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E470" s="21"/>
+      <c r="G469" s="21"/>
+    </row>
+    <row r="470" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F470" s="21"/>
-    </row>
-    <row r="471" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E471" s="21"/>
+      <c r="G470" s="21"/>
+    </row>
+    <row r="471" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F471" s="21"/>
-    </row>
-    <row r="472" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E472" s="21"/>
+      <c r="G471" s="21"/>
+    </row>
+    <row r="472" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F472" s="21"/>
-    </row>
-    <row r="473" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E473" s="21"/>
+      <c r="G472" s="21"/>
+    </row>
+    <row r="473" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F473" s="21"/>
-    </row>
-    <row r="474" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E474" s="21"/>
+      <c r="G473" s="21"/>
+    </row>
+    <row r="474" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F474" s="21"/>
-    </row>
-    <row r="475" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E475" s="21"/>
+      <c r="G474" s="21"/>
+    </row>
+    <row r="475" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F475" s="21"/>
-    </row>
-    <row r="476" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E476" s="21"/>
+      <c r="G475" s="21"/>
+    </row>
+    <row r="476" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F476" s="21"/>
-    </row>
-    <row r="477" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E477" s="21"/>
+      <c r="G476" s="21"/>
+    </row>
+    <row r="477" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F477" s="21"/>
-    </row>
-    <row r="478" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E478" s="21"/>
+      <c r="G477" s="21"/>
+    </row>
+    <row r="478" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F478" s="21"/>
-    </row>
-    <row r="479" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E479" s="21"/>
+      <c r="G478" s="21"/>
+    </row>
+    <row r="479" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F479" s="21"/>
-    </row>
-    <row r="480" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E480" s="21"/>
+      <c r="G479" s="21"/>
+    </row>
+    <row r="480" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F480" s="21"/>
-    </row>
-    <row r="481" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E481" s="21"/>
+      <c r="G480" s="21"/>
+    </row>
+    <row r="481" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F481" s="21"/>
-    </row>
-    <row r="482" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E482" s="21"/>
+      <c r="G481" s="21"/>
+    </row>
+    <row r="482" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F482" s="21"/>
-    </row>
-    <row r="483" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E483" s="21"/>
+      <c r="G482" s="21"/>
+    </row>
+    <row r="483" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F483" s="21"/>
-    </row>
-    <row r="484" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E484" s="21"/>
+      <c r="G483" s="21"/>
+    </row>
+    <row r="484" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F484" s="21"/>
-    </row>
-    <row r="485" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E485" s="21"/>
+      <c r="G484" s="21"/>
+    </row>
+    <row r="485" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F485" s="21"/>
-    </row>
-    <row r="486" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E486" s="21"/>
+      <c r="G485" s="21"/>
+    </row>
+    <row r="486" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F486" s="21"/>
-    </row>
-    <row r="487" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E487" s="21"/>
+      <c r="G486" s="21"/>
+    </row>
+    <row r="487" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F487" s="21"/>
-    </row>
-    <row r="488" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E488" s="21"/>
+      <c r="G487" s="21"/>
+    </row>
+    <row r="488" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F488" s="21"/>
-    </row>
-    <row r="489" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E489" s="21"/>
+      <c r="G488" s="21"/>
+    </row>
+    <row r="489" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F489" s="21"/>
-    </row>
-    <row r="490" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E490" s="21"/>
+      <c r="G489" s="21"/>
+    </row>
+    <row r="490" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F490" s="21"/>
-    </row>
-    <row r="491" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E491" s="21"/>
+      <c r="G490" s="21"/>
+    </row>
+    <row r="491" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F491" s="21"/>
-    </row>
-    <row r="492" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E492" s="21"/>
+      <c r="G491" s="21"/>
+    </row>
+    <row r="492" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F492" s="21"/>
-    </row>
-    <row r="493" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E493" s="21"/>
+      <c r="G492" s="21"/>
+    </row>
+    <row r="493" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F493" s="21"/>
-    </row>
-    <row r="494" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E494" s="21"/>
+      <c r="G493" s="21"/>
+    </row>
+    <row r="494" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F494" s="21"/>
-    </row>
-    <row r="495" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E495" s="21"/>
+      <c r="G494" s="21"/>
+    </row>
+    <row r="495" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F495" s="21"/>
-    </row>
-    <row r="496" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E496" s="21"/>
+      <c r="G495" s="21"/>
+    </row>
+    <row r="496" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F496" s="21"/>
-    </row>
-    <row r="497" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E497" s="21"/>
+      <c r="G496" s="21"/>
+    </row>
+    <row r="497" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F497" s="21"/>
-    </row>
-    <row r="498" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E498" s="21"/>
+      <c r="G497" s="21"/>
+    </row>
+    <row r="498" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F498" s="21"/>
-    </row>
-    <row r="499" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E499" s="21"/>
+      <c r="G498" s="21"/>
+    </row>
+    <row r="499" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F499" s="21"/>
-    </row>
-    <row r="500" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E500" s="21"/>
+      <c r="G499" s="21"/>
+    </row>
+    <row r="500" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F500" s="21"/>
-    </row>
-    <row r="501" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E501" s="21"/>
+      <c r="G500" s="21"/>
+    </row>
+    <row r="501" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F501" s="21"/>
-    </row>
-    <row r="502" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E502" s="21"/>
+      <c r="G501" s="21"/>
+    </row>
+    <row r="502" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F502" s="21"/>
-    </row>
-    <row r="503" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E503" s="21"/>
+      <c r="G502" s="21"/>
+    </row>
+    <row r="503" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F503" s="21"/>
-    </row>
-    <row r="504" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E504" s="21"/>
+      <c r="G503" s="21"/>
+    </row>
+    <row r="504" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F504" s="21"/>
-    </row>
-    <row r="505" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E505" s="21"/>
+      <c r="G504" s="21"/>
+    </row>
+    <row r="505" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F505" s="21"/>
-    </row>
-    <row r="506" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E506" s="21"/>
+      <c r="G505" s="21"/>
+    </row>
+    <row r="506" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F506" s="21"/>
-    </row>
-    <row r="507" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E507" s="21"/>
+      <c r="G506" s="21"/>
+    </row>
+    <row r="507" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F507" s="21"/>
-    </row>
-    <row r="508" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E508" s="21"/>
+      <c r="G507" s="21"/>
+    </row>
+    <row r="508" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F508" s="21"/>
-    </row>
-    <row r="509" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E509" s="21"/>
+      <c r="G508" s="21"/>
+    </row>
+    <row r="509" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F509" s="21"/>
-    </row>
-    <row r="510" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E510" s="21"/>
+      <c r="G509" s="21"/>
+    </row>
+    <row r="510" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F510" s="21"/>
-    </row>
-    <row r="511" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E511" s="21"/>
+      <c r="G510" s="21"/>
+    </row>
+    <row r="511" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F511" s="21"/>
-    </row>
-    <row r="512" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E512" s="21"/>
+      <c r="G511" s="21"/>
+    </row>
+    <row r="512" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F512" s="21"/>
-    </row>
-    <row r="513" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E513" s="21"/>
+      <c r="G512" s="21"/>
+    </row>
+    <row r="513" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F513" s="21"/>
-    </row>
-    <row r="514" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E514" s="21"/>
+      <c r="G513" s="21"/>
+    </row>
+    <row r="514" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F514" s="21"/>
-    </row>
-    <row r="515" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E515" s="21"/>
+      <c r="G514" s="21"/>
+    </row>
+    <row r="515" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F515" s="21"/>
-    </row>
-    <row r="516" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E516" s="21"/>
+      <c r="G515" s="21"/>
+    </row>
+    <row r="516" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F516" s="21"/>
-    </row>
-    <row r="517" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E517" s="21"/>
+      <c r="G516" s="21"/>
+    </row>
+    <row r="517" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F517" s="21"/>
-    </row>
-    <row r="518" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E518" s="21"/>
+      <c r="G517" s="21"/>
+    </row>
+    <row r="518" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F518" s="21"/>
-    </row>
-    <row r="519" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E519" s="21"/>
+      <c r="G518" s="21"/>
+    </row>
+    <row r="519" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F519" s="21"/>
-    </row>
-    <row r="520" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E520" s="21"/>
+      <c r="G519" s="21"/>
+    </row>
+    <row r="520" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F520" s="21"/>
-    </row>
-    <row r="521" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E521" s="21"/>
+      <c r="G520" s="21"/>
+    </row>
+    <row r="521" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F521" s="21"/>
-    </row>
-    <row r="522" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E522" s="21"/>
+      <c r="G521" s="21"/>
+    </row>
+    <row r="522" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F522" s="21"/>
-    </row>
-    <row r="523" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E523" s="21"/>
+      <c r="G522" s="21"/>
+    </row>
+    <row r="523" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F523" s="21"/>
-    </row>
-    <row r="524" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E524" s="21"/>
+      <c r="G523" s="21"/>
+    </row>
+    <row r="524" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F524" s="21"/>
-    </row>
-    <row r="525" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E525" s="21"/>
+      <c r="G524" s="21"/>
+    </row>
+    <row r="525" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F525" s="21"/>
-    </row>
-    <row r="526" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E526" s="21"/>
+      <c r="G525" s="21"/>
+    </row>
+    <row r="526" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F526" s="21"/>
-    </row>
-    <row r="527" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E527" s="21"/>
+      <c r="G526" s="21"/>
+    </row>
+    <row r="527" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F527" s="21"/>
-    </row>
-    <row r="528" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E528" s="21"/>
+      <c r="G527" s="21"/>
+    </row>
+    <row r="528" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F528" s="21"/>
-    </row>
-    <row r="529" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E529" s="21"/>
+      <c r="G528" s="21"/>
+    </row>
+    <row r="529" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F529" s="21"/>
-    </row>
-    <row r="530" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E530" s="21"/>
+      <c r="G529" s="21"/>
+    </row>
+    <row r="530" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F530" s="21"/>
-    </row>
-    <row r="531" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E531" s="21"/>
+      <c r="G530" s="21"/>
+    </row>
+    <row r="531" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F531" s="21"/>
-    </row>
-    <row r="532" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E532" s="21"/>
+      <c r="G531" s="21"/>
+    </row>
+    <row r="532" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F532" s="21"/>
-    </row>
-    <row r="533" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E533" s="21"/>
+      <c r="G532" s="21"/>
+    </row>
+    <row r="533" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F533" s="21"/>
-    </row>
-    <row r="534" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E534" s="21"/>
+      <c r="G533" s="21"/>
+    </row>
+    <row r="534" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F534" s="21"/>
-    </row>
-    <row r="535" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E535" s="21"/>
+      <c r="G534" s="21"/>
+    </row>
+    <row r="535" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F535" s="21"/>
-    </row>
-    <row r="536" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E536" s="21"/>
+      <c r="G535" s="21"/>
+    </row>
+    <row r="536" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F536" s="21"/>
-    </row>
-    <row r="537" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E537" s="21"/>
+      <c r="G536" s="21"/>
+    </row>
+    <row r="537" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F537" s="21"/>
-    </row>
-    <row r="538" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E538" s="21"/>
+      <c r="G537" s="21"/>
+    </row>
+    <row r="538" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F538" s="21"/>
-    </row>
-    <row r="539" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E539" s="21"/>
+      <c r="G538" s="21"/>
+    </row>
+    <row r="539" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F539" s="21"/>
-    </row>
-    <row r="540" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E540" s="21"/>
+      <c r="G539" s="21"/>
+    </row>
+    <row r="540" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F540" s="21"/>
-    </row>
-    <row r="541" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E541" s="21"/>
+      <c r="G540" s="21"/>
+    </row>
+    <row r="541" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F541" s="21"/>
-    </row>
-    <row r="542" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E542" s="21"/>
+      <c r="G541" s="21"/>
+    </row>
+    <row r="542" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F542" s="21"/>
-    </row>
-    <row r="543" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E543" s="21"/>
+      <c r="G542" s="21"/>
+    </row>
+    <row r="543" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F543" s="21"/>
-    </row>
-    <row r="544" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E544" s="21"/>
+      <c r="G543" s="21"/>
+    </row>
+    <row r="544" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F544" s="21"/>
-    </row>
-    <row r="545" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E545" s="21"/>
+      <c r="G544" s="21"/>
+    </row>
+    <row r="545" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F545" s="21"/>
-    </row>
-    <row r="546" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E546" s="21"/>
+      <c r="G545" s="21"/>
+    </row>
+    <row r="546" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F546" s="21"/>
-    </row>
-    <row r="547" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E547" s="21"/>
+      <c r="G546" s="21"/>
+    </row>
+    <row r="547" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F547" s="21"/>
-    </row>
-    <row r="548" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E548" s="21"/>
+      <c r="G547" s="21"/>
+    </row>
+    <row r="548" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F548" s="21"/>
-    </row>
-    <row r="549" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E549" s="21"/>
+      <c r="G548" s="21"/>
+    </row>
+    <row r="549" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F549" s="21"/>
-    </row>
-    <row r="550" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E550" s="21"/>
+      <c r="G549" s="21"/>
+    </row>
+    <row r="550" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F550" s="21"/>
-    </row>
-    <row r="551" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E551" s="21"/>
+      <c r="G550" s="21"/>
+    </row>
+    <row r="551" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F551" s="21"/>
-    </row>
-    <row r="552" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E552" s="21"/>
+      <c r="G551" s="21"/>
+    </row>
+    <row r="552" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F552" s="21"/>
-    </row>
-    <row r="553" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E553" s="21"/>
+      <c r="G552" s="21"/>
+    </row>
+    <row r="553" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F553" s="21"/>
-    </row>
-    <row r="554" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E554" s="21"/>
+      <c r="G553" s="21"/>
+    </row>
+    <row r="554" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F554" s="21"/>
-    </row>
-    <row r="555" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E555" s="21"/>
+      <c r="G554" s="21"/>
+    </row>
+    <row r="555" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F555" s="21"/>
-    </row>
-    <row r="556" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E556" s="21"/>
+      <c r="G555" s="21"/>
+    </row>
+    <row r="556" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F556" s="21"/>
-    </row>
-    <row r="557" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E557" s="21"/>
+      <c r="G556" s="21"/>
+    </row>
+    <row r="557" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F557" s="21"/>
-    </row>
-    <row r="558" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E558" s="21"/>
+      <c r="G557" s="21"/>
+    </row>
+    <row r="558" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F558" s="21"/>
-    </row>
-    <row r="559" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E559" s="21"/>
+      <c r="G558" s="21"/>
+    </row>
+    <row r="559" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F559" s="21"/>
-    </row>
-    <row r="560" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E560" s="21"/>
+      <c r="G559" s="21"/>
+    </row>
+    <row r="560" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F560" s="21"/>
-    </row>
-    <row r="561" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E561" s="21"/>
+      <c r="G560" s="21"/>
+    </row>
+    <row r="561" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F561" s="21"/>
-    </row>
-    <row r="562" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E562" s="21"/>
+      <c r="G561" s="21"/>
+    </row>
+    <row r="562" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F562" s="21"/>
-    </row>
-    <row r="563" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E563" s="21"/>
+      <c r="G562" s="21"/>
+    </row>
+    <row r="563" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F563" s="21"/>
-    </row>
-    <row r="564" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E564" s="21"/>
+      <c r="G563" s="21"/>
+    </row>
+    <row r="564" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F564" s="21"/>
-    </row>
-    <row r="565" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E565" s="21"/>
+      <c r="G564" s="21"/>
+    </row>
+    <row r="565" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F565" s="21"/>
-    </row>
-    <row r="566" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E566" s="21"/>
+      <c r="G565" s="21"/>
+    </row>
+    <row r="566" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F566" s="21"/>
-    </row>
-    <row r="567" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E567" s="21"/>
+      <c r="G566" s="21"/>
+    </row>
+    <row r="567" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F567" s="21"/>
-    </row>
-    <row r="568" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E568" s="21"/>
+      <c r="G567" s="21"/>
+    </row>
+    <row r="568" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F568" s="21"/>
-    </row>
-    <row r="569" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E569" s="21"/>
+      <c r="G568" s="21"/>
+    </row>
+    <row r="569" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F569" s="21"/>
-    </row>
-    <row r="570" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E570" s="21"/>
+      <c r="G569" s="21"/>
+    </row>
+    <row r="570" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F570" s="21"/>
-    </row>
-    <row r="571" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E571" s="21"/>
+      <c r="G570" s="21"/>
+    </row>
+    <row r="571" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F571" s="21"/>
-    </row>
-    <row r="572" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E572" s="21"/>
+      <c r="G571" s="21"/>
+    </row>
+    <row r="572" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F572" s="21"/>
-    </row>
-    <row r="573" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E573" s="21"/>
+      <c r="G572" s="21"/>
+    </row>
+    <row r="573" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F573" s="21"/>
-    </row>
-    <row r="574" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E574" s="21"/>
+      <c r="G573" s="21"/>
+    </row>
+    <row r="574" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F574" s="21"/>
-    </row>
-    <row r="575" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E575" s="21"/>
+      <c r="G574" s="21"/>
+    </row>
+    <row r="575" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F575" s="21"/>
-    </row>
-    <row r="576" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E576" s="21"/>
+      <c r="G575" s="21"/>
+    </row>
+    <row r="576" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F576" s="21"/>
-    </row>
-    <row r="577" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E577" s="21"/>
+      <c r="G576" s="21"/>
+    </row>
+    <row r="577" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F577" s="21"/>
-    </row>
-    <row r="578" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E578" s="21"/>
+      <c r="G577" s="21"/>
+    </row>
+    <row r="578" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F578" s="21"/>
-    </row>
-    <row r="579" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E579" s="21"/>
+      <c r="G578" s="21"/>
+    </row>
+    <row r="579" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F579" s="21"/>
-    </row>
-    <row r="580" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E580" s="21"/>
+      <c r="G579" s="21"/>
+    </row>
+    <row r="580" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F580" s="21"/>
-    </row>
-    <row r="581" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E581" s="21"/>
+      <c r="G580" s="21"/>
+    </row>
+    <row r="581" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F581" s="21"/>
-    </row>
-    <row r="582" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E582" s="21"/>
+      <c r="G581" s="21"/>
+    </row>
+    <row r="582" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F582" s="21"/>
-    </row>
-    <row r="583" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E583" s="21"/>
+      <c r="G582" s="21"/>
+    </row>
+    <row r="583" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F583" s="21"/>
-    </row>
-    <row r="584" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E584" s="21"/>
+      <c r="G583" s="21"/>
+    </row>
+    <row r="584" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F584" s="21"/>
-    </row>
-    <row r="585" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E585" s="21"/>
+      <c r="G584" s="21"/>
+    </row>
+    <row r="585" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F585" s="21"/>
-    </row>
-    <row r="586" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E586" s="21"/>
+      <c r="G585" s="21"/>
+    </row>
+    <row r="586" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F586" s="21"/>
-    </row>
-    <row r="587" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E587" s="21"/>
+      <c r="G586" s="21"/>
+    </row>
+    <row r="587" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F587" s="21"/>
-    </row>
-    <row r="588" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E588" s="21"/>
+      <c r="G587" s="21"/>
+    </row>
+    <row r="588" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F588" s="21"/>
-    </row>
-    <row r="589" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E589" s="21"/>
+      <c r="G588" s="21"/>
+    </row>
+    <row r="589" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F589" s="21"/>
-    </row>
-    <row r="590" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E590" s="21"/>
+      <c r="G589" s="21"/>
+    </row>
+    <row r="590" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F590" s="21"/>
-    </row>
-    <row r="591" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E591" s="21"/>
+      <c r="G590" s="21"/>
+    </row>
+    <row r="591" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F591" s="21"/>
-    </row>
-    <row r="592" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E592" s="21"/>
+      <c r="G591" s="21"/>
+    </row>
+    <row r="592" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F592" s="21"/>
-    </row>
-    <row r="593" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E593" s="21"/>
+      <c r="G592" s="21"/>
+    </row>
+    <row r="593" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F593" s="21"/>
-    </row>
-    <row r="594" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E594" s="21"/>
+      <c r="G593" s="21"/>
+    </row>
+    <row r="594" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F594" s="21"/>
-    </row>
-    <row r="595" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E595" s="21"/>
+      <c r="G594" s="21"/>
+    </row>
+    <row r="595" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F595" s="21"/>
-    </row>
-    <row r="596" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E596" s="21"/>
+      <c r="G595" s="21"/>
+    </row>
+    <row r="596" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F596" s="21"/>
-    </row>
-    <row r="597" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E597" s="21"/>
+      <c r="G596" s="21"/>
+    </row>
+    <row r="597" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F597" s="21"/>
-    </row>
-    <row r="598" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E598" s="21"/>
+      <c r="G597" s="21"/>
+    </row>
+    <row r="598" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F598" s="21"/>
-    </row>
-    <row r="599" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E599" s="21"/>
+      <c r="G598" s="21"/>
+    </row>
+    <row r="599" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F599" s="21"/>
-    </row>
-    <row r="600" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E600" s="21"/>
+      <c r="G599" s="21"/>
+    </row>
+    <row r="600" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F600" s="21"/>
-    </row>
-    <row r="601" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E601" s="21"/>
+      <c r="G600" s="21"/>
+    </row>
+    <row r="601" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F601" s="21"/>
-    </row>
-    <row r="602" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E602" s="21"/>
+      <c r="G601" s="21"/>
+    </row>
+    <row r="602" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F602" s="21"/>
-    </row>
-    <row r="603" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E603" s="21"/>
+      <c r="G602" s="21"/>
+    </row>
+    <row r="603" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F603" s="21"/>
-    </row>
-    <row r="604" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E604" s="21"/>
+      <c r="G603" s="21"/>
+    </row>
+    <row r="604" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F604" s="21"/>
-    </row>
-    <row r="605" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E605" s="21"/>
+      <c r="G604" s="21"/>
+    </row>
+    <row r="605" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F605" s="21"/>
-    </row>
-    <row r="606" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E606" s="21"/>
+      <c r="G605" s="21"/>
+    </row>
+    <row r="606" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F606" s="21"/>
-    </row>
-    <row r="607" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E607" s="21"/>
+      <c r="G606" s="21"/>
+    </row>
+    <row r="607" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F607" s="21"/>
-    </row>
-    <row r="608" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E608" s="21"/>
+      <c r="G607" s="21"/>
+    </row>
+    <row r="608" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F608" s="21"/>
-    </row>
-    <row r="609" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E609" s="21"/>
+      <c r="G608" s="21"/>
+    </row>
+    <row r="609" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F609" s="21"/>
-    </row>
-    <row r="610" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E610" s="21"/>
+      <c r="G609" s="21"/>
+    </row>
+    <row r="610" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F610" s="21"/>
-    </row>
-    <row r="611" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E611" s="21"/>
+      <c r="G610" s="21"/>
+    </row>
+    <row r="611" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F611" s="21"/>
-    </row>
-    <row r="612" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E612" s="21"/>
+      <c r="G611" s="21"/>
+    </row>
+    <row r="612" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F612" s="21"/>
-    </row>
-    <row r="613" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E613" s="21"/>
+      <c r="G612" s="21"/>
+    </row>
+    <row r="613" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F613" s="21"/>
-    </row>
-    <row r="614" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E614" s="21"/>
+      <c r="G613" s="21"/>
+    </row>
+    <row r="614" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F614" s="21"/>
-    </row>
-    <row r="615" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E615" s="21"/>
+      <c r="G614" s="21"/>
+    </row>
+    <row r="615" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F615" s="21"/>
-    </row>
-    <row r="616" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E616" s="21"/>
+      <c r="G615" s="21"/>
+    </row>
+    <row r="616" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F616" s="21"/>
-    </row>
-    <row r="617" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E617" s="21"/>
+      <c r="G616" s="21"/>
+    </row>
+    <row r="617" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F617" s="21"/>
-    </row>
-    <row r="618" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E618" s="21"/>
+      <c r="G617" s="21"/>
+    </row>
+    <row r="618" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F618" s="21"/>
-    </row>
-    <row r="619" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E619" s="21"/>
+      <c r="G618" s="21"/>
+    </row>
+    <row r="619" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F619" s="21"/>
-    </row>
-    <row r="620" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E620" s="21"/>
+      <c r="G619" s="21"/>
+    </row>
+    <row r="620" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F620" s="21"/>
-    </row>
-    <row r="621" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E621" s="21"/>
+      <c r="G620" s="21"/>
+    </row>
+    <row r="621" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F621" s="21"/>
-    </row>
-    <row r="622" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E622" s="21"/>
+      <c r="G621" s="21"/>
+    </row>
+    <row r="622" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F622" s="21"/>
-    </row>
-    <row r="623" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E623" s="21"/>
+      <c r="G622" s="21"/>
+    </row>
+    <row r="623" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F623" s="21"/>
-    </row>
-    <row r="624" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E624" s="21"/>
+      <c r="G623" s="21"/>
+    </row>
+    <row r="624" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F624" s="21"/>
-    </row>
-    <row r="625" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E625" s="21"/>
+      <c r="G624" s="21"/>
+    </row>
+    <row r="625" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F625" s="21"/>
-    </row>
-    <row r="626" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E626" s="21"/>
+      <c r="G625" s="21"/>
+    </row>
+    <row r="626" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F626" s="21"/>
-    </row>
-    <row r="627" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E627" s="21"/>
+      <c r="G626" s="21"/>
+    </row>
+    <row r="627" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F627" s="21"/>
-    </row>
-    <row r="628" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E628" s="21"/>
+      <c r="G627" s="21"/>
+    </row>
+    <row r="628" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F628" s="21"/>
-    </row>
-    <row r="629" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E629" s="21"/>
+      <c r="G628" s="21"/>
+    </row>
+    <row r="629" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F629" s="21"/>
-    </row>
-    <row r="630" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E630" s="21"/>
+      <c r="G629" s="21"/>
+    </row>
+    <row r="630" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F630" s="21"/>
-    </row>
-    <row r="631" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E631" s="21"/>
+      <c r="G630" s="21"/>
+    </row>
+    <row r="631" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F631" s="21"/>
-    </row>
-    <row r="632" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E632" s="21"/>
+      <c r="G631" s="21"/>
+    </row>
+    <row r="632" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F632" s="21"/>
-    </row>
-    <row r="633" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E633" s="21"/>
+      <c r="G632" s="21"/>
+    </row>
+    <row r="633" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F633" s="21"/>
-    </row>
-    <row r="634" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E634" s="21"/>
+      <c r="G633" s="21"/>
+    </row>
+    <row r="634" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F634" s="21"/>
-    </row>
-    <row r="635" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E635" s="21"/>
+      <c r="G634" s="21"/>
+    </row>
+    <row r="635" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F635" s="21"/>
-    </row>
-    <row r="636" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E636" s="21"/>
+      <c r="G635" s="21"/>
+    </row>
+    <row r="636" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F636" s="21"/>
-    </row>
-    <row r="637" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E637" s="21"/>
+      <c r="G636" s="21"/>
+    </row>
+    <row r="637" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F637" s="21"/>
-    </row>
-    <row r="638" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E638" s="21"/>
+      <c r="G637" s="21"/>
+    </row>
+    <row r="638" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F638" s="21"/>
-    </row>
-    <row r="639" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E639" s="21"/>
+      <c r="G638" s="21"/>
+    </row>
+    <row r="639" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F639" s="21"/>
-    </row>
-    <row r="640" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E640" s="21"/>
+      <c r="G639" s="21"/>
+    </row>
+    <row r="640" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F640" s="21"/>
-    </row>
-    <row r="641" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E641" s="21"/>
+      <c r="G640" s="21"/>
+    </row>
+    <row r="641" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F641" s="21"/>
-    </row>
-    <row r="642" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E642" s="21"/>
+      <c r="G641" s="21"/>
+    </row>
+    <row r="642" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F642" s="21"/>
-    </row>
-    <row r="643" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E643" s="21"/>
+      <c r="G642" s="21"/>
+    </row>
+    <row r="643" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F643" s="21"/>
-    </row>
-    <row r="644" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E644" s="21"/>
+      <c r="G643" s="21"/>
+    </row>
+    <row r="644" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F644" s="21"/>
-    </row>
-    <row r="645" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E645" s="21"/>
+      <c r="G644" s="21"/>
+    </row>
+    <row r="645" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F645" s="21"/>
-    </row>
-    <row r="646" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E646" s="21"/>
+      <c r="G645" s="21"/>
+    </row>
+    <row r="646" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F646" s="21"/>
-    </row>
-    <row r="647" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E647" s="21"/>
+      <c r="G646" s="21"/>
+    </row>
+    <row r="647" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F647" s="21"/>
-    </row>
-    <row r="648" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E648" s="21"/>
+      <c r="G647" s="21"/>
+    </row>
+    <row r="648" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F648" s="21"/>
-    </row>
-    <row r="649" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E649" s="21"/>
+      <c r="G648" s="21"/>
+    </row>
+    <row r="649" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F649" s="21"/>
-    </row>
-    <row r="650" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E650" s="21"/>
+      <c r="G649" s="21"/>
+    </row>
+    <row r="650" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F650" s="21"/>
-    </row>
-    <row r="651" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E651" s="21"/>
+      <c r="G650" s="21"/>
+    </row>
+    <row r="651" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F651" s="21"/>
-    </row>
-    <row r="652" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E652" s="21"/>
+      <c r="G651" s="21"/>
+    </row>
+    <row r="652" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F652" s="21"/>
-    </row>
-    <row r="653" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E653" s="21"/>
+      <c r="G652" s="21"/>
+    </row>
+    <row r="653" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F653" s="21"/>
-    </row>
-    <row r="654" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E654" s="21"/>
+      <c r="G653" s="21"/>
+    </row>
+    <row r="654" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F654" s="21"/>
-    </row>
-    <row r="655" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E655" s="21"/>
+      <c r="G654" s="21"/>
+    </row>
+    <row r="655" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F655" s="21"/>
-    </row>
-    <row r="656" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E656" s="21"/>
+      <c r="G655" s="21"/>
+    </row>
+    <row r="656" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F656" s="21"/>
-    </row>
-    <row r="657" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E657" s="21"/>
+      <c r="G656" s="21"/>
+    </row>
+    <row r="657" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F657" s="21"/>
-    </row>
-    <row r="658" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E658" s="21"/>
+      <c r="G657" s="21"/>
+    </row>
+    <row r="658" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F658" s="21"/>
-    </row>
-    <row r="659" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E659" s="21"/>
+      <c r="G658" s="21"/>
+    </row>
+    <row r="659" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F659" s="21"/>
-    </row>
-    <row r="660" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E660" s="21"/>
+      <c r="G659" s="21"/>
+    </row>
+    <row r="660" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F660" s="21"/>
-    </row>
-    <row r="667" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E667" s="21"/>
+      <c r="G660" s="21"/>
+    </row>
+    <row r="667" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F667" s="21"/>
-    </row>
-    <row r="668" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E668" s="21"/>
+      <c r="G667" s="21"/>
+    </row>
+    <row r="668" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F668" s="21"/>
-    </row>
-    <row r="669" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E669" s="21"/>
+      <c r="G668" s="21"/>
+    </row>
+    <row r="669" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F669" s="21"/>
-    </row>
-    <row r="670" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E670" s="21"/>
+      <c r="G669" s="21"/>
+    </row>
+    <row r="670" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F670" s="21"/>
-    </row>
-    <row r="671" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E671" s="21"/>
+      <c r="G670" s="21"/>
+    </row>
+    <row r="671" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F671" s="21"/>
-    </row>
-    <row r="672" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E672" s="21"/>
+      <c r="G671" s="21"/>
+    </row>
+    <row r="672" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F672" s="21"/>
-    </row>
-    <row r="673" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E673" s="21"/>
+      <c r="G672" s="21"/>
+    </row>
+    <row r="673" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F673" s="21"/>
-    </row>
-    <row r="674" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E674" s="21"/>
+      <c r="G673" s="21"/>
+    </row>
+    <row r="674" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F674" s="21"/>
-    </row>
-    <row r="675" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E675" s="21"/>
+      <c r="G674" s="21"/>
+    </row>
+    <row r="675" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F675" s="21"/>
-    </row>
-    <row r="676" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E676" s="21"/>
+      <c r="G675" s="21"/>
+    </row>
+    <row r="676" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F676" s="21"/>
-    </row>
-    <row r="677" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E677" s="21"/>
+      <c r="G676" s="21"/>
+    </row>
+    <row r="677" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F677" s="21"/>
-    </row>
-    <row r="678" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E678" s="21"/>
+      <c r="G677" s="21"/>
+    </row>
+    <row r="678" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F678" s="21"/>
-    </row>
-    <row r="679" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E679" s="21"/>
+      <c r="G678" s="21"/>
+    </row>
+    <row r="679" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F679" s="21"/>
+      <c r="G679" s="21"/>
     </row>
   </sheetData>
   <dataConsolidate/>
-  <dataValidations count="2">
-    <dataValidation type="date" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Session end date must be later than session start date." sqref="E71:E362 E369:E660 E667:E679 E4:E64">
-      <formula1>D4</formula1>
+  <dataValidations count="3">
+    <dataValidation type="date" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Session end date must be later than session start date." sqref="F71:F362 F369:F660 F667:F679 F4:F64">
+      <formula1>E4</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Session end date must be later than session start date." sqref="F1:G1"/>
+    <dataValidation errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Session end date must be later than session start date." sqref="G1:H1"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="You need to select a value from the drop down list." sqref="D1:D1048576"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6087,11 +6122,11 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$1:$A$48</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:G1048576</xm:sqref>
+          <xm:sqref>G2:H1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Sheet1!$G$20:$G$22</xm:f>
+            <xm:f>Sheet1!$G$20:$G$23</xm:f>
           </x14:formula1>
           <xm:sqref>A2:A1048576</xm:sqref>
         </x14:dataValidation>
@@ -6105,8 +6140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G207"/>
   <sheetViews>
-    <sheetView topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6392,7 +6427,7 @@
         <v>83</v>
       </c>
       <c r="G22" s="34" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -6401,6 +6436,9 @@
       </c>
       <c r="C23" s="6" t="s">
         <v>84</v>
+      </c>
+      <c r="G23" s="34" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
WLCMS-3112 Duration and Price fields in Classroom Batch Import file.
</commit_message>
<xml_diff>
--- a/lcms.web/src/main/webapp/theme/samplefile/Classroom batch import template.xlsx
+++ b/lcms.web/src/main/webapp/theme/samplefile/Classroom batch import template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\360 SVN\lcms.web\src\main\webapp\theme\samplefile\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WLCMS-GitHub\lcms.web\src\main\webapp\theme\samplefile\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="391">
   <si>
     <t>(GMT -12:00) Dateline (Eniwetok)</t>
   </si>
@@ -2017,6 +2017,72 @@
         <scheme val="minor"/>
       </rPr>
       <t>Session1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Course Duration</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  (optional) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Provide the complete duration time in hours of this instructor led course.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Course Price</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>This price wil display as the course selling price on our store.</t>
     </r>
   </si>
 </sst>
@@ -2189,7 +2255,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2303,6 +2369,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2675,7 +2744,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2687,21 +2756,23 @@
     <col min="1" max="1" width="24.7109375" style="33" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="29.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="33.85546875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="33.42578125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="37.28515625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="42.140625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="35.5703125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="20.7109375" style="2" customWidth="1"/>
-    <col min="13" max="13" width="20.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17" style="2" customWidth="1"/>
-    <col min="15" max="15" width="25.28515625" style="2" customWidth="1"/>
-    <col min="16" max="16" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="2"/>
+    <col min="4" max="4" width="20.5703125" style="17" customWidth="1"/>
+    <col min="5" max="7" width="29.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="33.85546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="33.42578125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="37.28515625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="42.140625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="35.5703125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="35.5703125" style="17" customWidth="1"/>
+    <col min="14" max="14" width="20.7109375" style="2" customWidth="1"/>
+    <col min="15" max="15" width="20.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17" style="2" customWidth="1"/>
+    <col min="17" max="17" width="25.28515625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
         <v>375</v>
       </c>
@@ -2711,50 +2782,56 @@
       <c r="C1" s="7" t="s">
         <v>288</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="43" t="s">
+        <v>389</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>289</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="F1" s="31" t="s">
         <v>367</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>290</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>305</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>298</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>297</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>291</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>292</v>
       </c>
-      <c r="L1" s="41" t="s">
+      <c r="M1" s="43" t="s">
+        <v>390</v>
+      </c>
+      <c r="N1" s="41" t="s">
         <v>293</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="O1" s="7" t="s">
         <v>294</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>295</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>296</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="R1" s="7" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="D2" s="17"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -2763,12 +2840,14 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
-      <c r="M2" s="28"/>
+      <c r="M2" s="17"/>
       <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
+      <c r="O2" s="28"/>
       <c r="P2" s="2"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B7" s="9"/>
     </row>
   </sheetData>
@@ -2790,13 +2869,13 @@
           <x14:formula1>
             <xm:f>Sheet1!$E$2:$E$18</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F1048576</xm:sqref>
+          <xm:sqref>G2:G1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Instructor!$B$2:$B$100</xm:f>
           </x14:formula1>
-          <xm:sqref>L2:L1048576</xm:sqref>
+          <xm:sqref>N2:N1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>